<commit_message>
[MS-OXCSTOR]: Update code as fixed TDI.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7886" uniqueCount="2418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7884" uniqueCount="2419">
   <si>
     <t>Req ID</t>
   </si>
@@ -7472,9 +7472,6 @@
     <t>MS-OXCSTOR_R1121:i</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCSTOR_R1121001, MS-OXCSTOR_R1121002.</t>
-  </si>
-  <si>
     <t>[In Receiving a RopLongTermIdFromId ROP Request] If the REPLID is not in the REPLID and REPLGUID to-and-from mapping table, the operation [RopLongTermIdFromId] SHOULD&lt;43&gt; fail with a ReturnValue of 0x8004010F.</t>
   </si>
   <si>
@@ -7497,6 +7494,12 @@
   </si>
   <si>
     <t>MS-OXCSTOR_R59748</t>
+  </si>
+  <si>
+    <t>Verified by requirement: MS-OXCSTOR_R94801002.</t>
+  </si>
+  <si>
+    <t>Verified by requirement: MS-OXCSTOR_R94801001.</t>
   </si>
 </sst>
 </file>
@@ -7771,21 +7774,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7809,6 +7797,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8825,127 +8828,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8958,12 +8961,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8976,12 +8979,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8994,12 +8997,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9012,60 +9015,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -23728,7 +23731,7 @@
     </row>
     <row r="601" spans="1:9" ht="60">
       <c r="A601" s="22" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="B601" s="30" t="s">
         <v>1196</v>
@@ -29939,7 +29942,7 @@
         <v>1205</v>
       </c>
       <c r="C848" s="31" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="D848" s="29"/>
       <c r="E848" s="29" t="s">
@@ -30240,7 +30243,7 @@
       <c r="B860" s="30" t="s">
         <v>1205</v>
       </c>
-      <c r="C860" s="31" t="s">
+      <c r="C860" s="20" t="s">
         <v>2002</v>
       </c>
       <c r="D860" s="29"/>
@@ -30259,14 +30262,14 @@
       <c r="I860" s="31"/>
     </row>
     <row r="861" spans="1:9" ht="45">
-      <c r="A861" s="29" t="s">
+      <c r="A861" s="22" t="s">
         <v>881</v>
       </c>
       <c r="B861" s="30" t="s">
         <v>1206</v>
       </c>
-      <c r="C861" s="31" t="s">
-        <v>2411</v>
+      <c r="C861" s="20" t="s">
+        <v>2410</v>
       </c>
       <c r="D861" s="29"/>
       <c r="E861" s="29" t="s">
@@ -30306,7 +30309,7 @@
       <c r="H862" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I862" s="31" t="s">
+      <c r="I862" s="20" t="s">
         <v>2401</v>
       </c>
     </row>
@@ -30736,13 +30739,13 @@
       <c r="I879" s="31"/>
     </row>
     <row r="880" spans="1:9" ht="30">
-      <c r="A880" s="29" t="s">
+      <c r="A880" s="22" t="s">
         <v>899</v>
       </c>
       <c r="B880" s="30" t="s">
         <v>1206</v>
       </c>
-      <c r="C880" s="31" t="s">
+      <c r="C880" s="20" t="s">
         <v>2020</v>
       </c>
       <c r="D880" s="29"/>
@@ -30760,7 +30763,7 @@
       </c>
       <c r="I880" s="31"/>
     </row>
-    <row r="881" spans="1:9" ht="60">
+    <row r="881" spans="1:9" ht="45">
       <c r="A881" s="29" t="s">
         <v>900</v>
       </c>
@@ -30783,9 +30786,7 @@
       <c r="H881" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I881" s="31" t="s">
-        <v>2409</v>
-      </c>
+      <c r="I881" s="31"/>
     </row>
     <row r="882" spans="1:9" ht="30">
       <c r="A882" s="29" t="s">
@@ -34689,7 +34690,7 @@
     </row>
     <row r="1034" spans="1:9" ht="45">
       <c r="A1034" s="22" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="B1034" s="30" t="s">
         <v>1217</v>
@@ -34718,7 +34719,7 @@
     </row>
     <row r="1035" spans="1:9" ht="45">
       <c r="A1035" s="22" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="B1035" s="30" t="s">
         <v>1217</v>
@@ -34994,11 +34995,9 @@
         <v>15</v>
       </c>
       <c r="H1044" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1044" s="31" t="s">
-        <v>2231</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1044" s="31"/>
     </row>
     <row r="1045" spans="1:9" ht="45">
       <c r="A1045" s="29" t="s">
@@ -35620,7 +35619,7 @@
         <v>1217</v>
       </c>
       <c r="C1067" s="31" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="D1067" s="29" t="s">
         <v>2190</v>
@@ -35752,8 +35751,8 @@
       <c r="B1072" s="30" t="s">
         <v>1217</v>
       </c>
-      <c r="C1072" s="31" t="s">
-        <v>2414</v>
+      <c r="C1072" s="20" t="s">
+        <v>2413</v>
       </c>
       <c r="D1072" s="29" t="s">
         <v>2193</v>
@@ -36076,13 +36075,13 @@
       </c>
     </row>
     <row r="1084" spans="1:9" ht="45">
-      <c r="A1084" s="29" t="s">
+      <c r="A1084" s="22" t="s">
         <v>2396</v>
       </c>
       <c r="B1084" s="30" t="s">
         <v>1217</v>
       </c>
-      <c r="C1084" s="31" t="s">
+      <c r="C1084" s="20" t="s">
         <v>2400</v>
       </c>
       <c r="D1084" s="29" t="s">
@@ -36105,13 +36104,13 @@
       </c>
     </row>
     <row r="1085" spans="1:9" ht="60">
-      <c r="A1085" s="29" t="s">
+      <c r="A1085" s="22" t="s">
         <v>2397</v>
       </c>
       <c r="B1085" s="30" t="s">
         <v>1217</v>
       </c>
-      <c r="C1085" s="31" t="s">
+      <c r="C1085" s="20" t="s">
         <v>2402</v>
       </c>
       <c r="D1085" s="29" t="s">
@@ -36156,10 +36155,10 @@
         <v>15</v>
       </c>
       <c r="H1086" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1086" s="31" t="s">
-        <v>2231</v>
+        <v>17</v>
+      </c>
+      <c r="I1086" s="20" t="s">
+        <v>2417</v>
       </c>
     </row>
     <row r="1087" spans="1:9" ht="45">
@@ -36185,10 +36184,10 @@
         <v>15</v>
       </c>
       <c r="H1087" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1087" s="31" t="s">
-        <v>2231</v>
+        <v>17</v>
+      </c>
+      <c r="I1087" s="20" t="s">
+        <v>2418</v>
       </c>
     </row>
     <row r="1088" spans="1:9" ht="60">
@@ -36257,7 +36256,7 @@
         <v>1217</v>
       </c>
       <c r="C1090" s="31" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="D1090" s="29" t="s">
         <v>2200</v>
@@ -36337,7 +36336,7 @@
       </c>
     </row>
     <row r="1093" spans="1:9" ht="45">
-      <c r="A1093" s="29" t="s">
+      <c r="A1093" s="22" t="s">
         <v>2384</v>
       </c>
       <c r="B1093" s="30" t="s">
@@ -36753,6 +36752,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36760,11 +36764,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1102:I1107 A20:H1040 I20:I1043 A34:I1100">
@@ -36883,21 +36882,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -36946,16 +36930,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -36969,16 +36969,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXCSTOR]: Update as fixed TDI.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7882" uniqueCount="2419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7876" uniqueCount="2418">
   <si>
     <t>Req ID</t>
   </si>
@@ -6689,9 +6689,6 @@
     <t>Implementation set this field [StoreState in RopLogon ROP Success Response Buffer for Private Mailbox] to 0x00000000 [if the mailbox currently has any active search folders]. (Exchange 2010 and above follow this behavior.)</t>
   </si>
   <si>
-    <t>Implementation returns the Folder ID of all of the following folders in this field [FolderIds in RopLogon ROP Success Response Buffer for Public Folders]: Public Folders Root Folder (All other folders listed here are direct or indirect children of this folder), Interpersonal messages subtree, Non-interpersonal messages subtree, EForms Registry, Free/Busy Data, Offline address book Data, EForms Registry for the user's locale, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, NNTP Article Index, Empty, Empty, Empty. (Exchange 2003, Exchange 2007 and Exchange 2010 follow this behavior)</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] The implementation does not set the PerUserGuid field to an empty GUID. (&lt;9&gt; Section 2.2.1.1.4: Exchange 2007 does not set the PerUserGuid field to an empty GUID.)</t>
   </si>
   <si>
@@ -7220,9 +7217,6 @@
     <t>MS-OXCSTOR_R59747:I, MS-OXCSTOR_R1:i</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXCSTOR_R59747001, MS-OXCSTOR_R59747002.</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] The implementation returns ecMailboxDisabled [if the client attempts to log on to a mailbox that is disabled]. (&lt;20&gt; Section 3.2.5.1.1: Exchange 2003 returns ecMailboxDisabled.)</t>
   </si>
   <si>
@@ -7409,9 +7403,6 @@
     <t>MS-OXCSTOR_R1021:I, MS-OXCSTOR_R1:i</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCSTOR_R1021001, MS-OXCSTOR_R1021002, MS-OXCSTOR_R1021003.</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] The implementation does fail with "0x000004ED" when the client sends a RopWritePerUserInformation ROP request with invalid value set in Data field. &lt;50&gt; Section 3.2.5.13.1:  Returned in Exchange 2007 only.</t>
   </si>
   <si>
@@ -7430,9 +7421,6 @@
     <t>MS-OXCSTOR_R603"i</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCSTOR_R603001, MS-OXCSTOR_R603002.</t>
-  </si>
-  <si>
     <t>MS-OXCSTOR_R94801001</t>
   </si>
   <si>
@@ -7500,6 +7488,15 @@
   </si>
   <si>
     <t>Verified by requirement: MS-OXCSTOR_R94801001.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCSTOR_R155, MS-OXCSTOR_R5979301.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCSTOR_R59747001, MS-OXCSTOR_R59747002.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior]  Implementation returns the Folder ID of all of the following folders in this field [FolderIds in RopLogon ROP Success Response Buffer for Public Folders]: Public Folders Root Folder (All other folders listed here are direct or indirect children of this folder), Interpersonal messages subtree, Non-interpersonal messages subtree, EForms Registry, Free/Busy Data, Offline address book Data, EForms Registry for the user's locale, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, NNTP Article Index, Empty, Empty, Empty. (Exchange 2003, Exchange 2007 and Exchange 2010 follow this behavior)</t>
   </si>
 </sst>
 </file>
@@ -7554,6 +7551,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -7774,6 +7772,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7797,21 +7810,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8793,7 +8791,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -8803,7 +8801,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -8817,7 +8815,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -8828,127 +8826,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8961,12 +8959,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8979,12 +8977,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8997,12 +8995,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9015,60 +9013,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9654,13 +9652,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="29" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>1111</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -9679,13 +9677,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="29" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>1111</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -9951,7 +9949,7 @@
         <v>17</v>
       </c>
       <c r="I53" s="31" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30">
@@ -10328,7 +10326,7 @@
         <v>17</v>
       </c>
       <c r="I68" s="31" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="45">
@@ -10342,7 +10340,7 @@
         <v>1267</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="E69" s="29" t="s">
         <v>19</v>
@@ -10407,7 +10405,7 @@
         <v>17</v>
       </c>
       <c r="I71" s="31" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="30">
@@ -10484,7 +10482,7 @@
         <v>17</v>
       </c>
       <c r="I74" s="31" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="30">
@@ -10961,7 +10959,7 @@
         <v>17</v>
       </c>
       <c r="I93" s="31" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="45">
@@ -11563,7 +11561,7 @@
         <v>17</v>
       </c>
       <c r="I117" s="31" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="30">
@@ -11740,7 +11738,7 @@
         <v>17</v>
       </c>
       <c r="I124" s="31" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="90">
@@ -11764,9 +11762,11 @@
         <v>15</v>
       </c>
       <c r="H125" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I125" s="31"/>
+        <v>17</v>
+      </c>
+      <c r="I125" s="20" t="s">
+        <v>2415</v>
+      </c>
     </row>
     <row r="126" spans="1:9" ht="30">
       <c r="A126" s="29" t="s">
@@ -11967,7 +11967,7 @@
         <v>17</v>
       </c>
       <c r="I133" s="31" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="30">
@@ -13628,7 +13628,7 @@
         <v>1124</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
@@ -13878,7 +13878,7 @@
         <v>1124</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="D210" s="29"/>
       <c r="E210" s="29" t="s">
@@ -13969,7 +13969,7 @@
         <v>17</v>
       </c>
       <c r="I213" s="31" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="214" spans="1:9" ht="30">
@@ -14396,7 +14396,7 @@
         <v>17</v>
       </c>
       <c r="I230" s="31" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="231" spans="1:9" ht="45">
@@ -14757,7 +14757,7 @@
         <v>1134</v>
       </c>
       <c r="C245" s="31" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="29" t="s">
@@ -14848,7 +14848,7 @@
         <v>17</v>
       </c>
       <c r="I248" s="31" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="249" spans="1:9" ht="45">
@@ -15025,7 +15025,7 @@
         <v>17</v>
       </c>
       <c r="I255" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="256" spans="1:9" ht="60">
@@ -15052,7 +15052,7 @@
         <v>17</v>
       </c>
       <c r="I256" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="257" spans="1:9" ht="60">
@@ -15079,7 +15079,7 @@
         <v>17</v>
       </c>
       <c r="I257" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="258" spans="1:9" ht="60">
@@ -15106,7 +15106,7 @@
         <v>17</v>
       </c>
       <c r="I258" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="259" spans="1:9" ht="30">
@@ -15183,7 +15183,7 @@
         <v>17</v>
       </c>
       <c r="I261" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="262" spans="1:9" ht="60">
@@ -15210,7 +15210,7 @@
         <v>17</v>
       </c>
       <c r="I262" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="263" spans="1:9" ht="60">
@@ -15237,7 +15237,7 @@
         <v>17</v>
       </c>
       <c r="I263" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="30">
@@ -15289,7 +15289,7 @@
         <v>17</v>
       </c>
       <c r="I265" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="266" spans="1:9" ht="60">
@@ -15316,7 +15316,7 @@
         <v>17</v>
       </c>
       <c r="I266" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="267" spans="1:9" ht="60">
@@ -15343,7 +15343,7 @@
         <v>17</v>
       </c>
       <c r="I267" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="268" spans="1:9" ht="30">
@@ -15395,7 +15395,7 @@
         <v>17</v>
       </c>
       <c r="I269" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="270" spans="1:9" ht="45">
@@ -18459,7 +18459,7 @@
         <v>1587</v>
       </c>
       <c r="D392" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E392" s="29" t="s">
         <v>19</v>
@@ -18486,7 +18486,7 @@
         <v>1588</v>
       </c>
       <c r="D393" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E393" s="29" t="s">
         <v>19</v>
@@ -18513,7 +18513,7 @@
         <v>1589</v>
       </c>
       <c r="D394" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E394" s="29" t="s">
         <v>19</v>
@@ -18540,7 +18540,7 @@
         <v>1590</v>
       </c>
       <c r="D395" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E395" s="29" t="s">
         <v>19</v>
@@ -18567,7 +18567,7 @@
         <v>1591</v>
       </c>
       <c r="D396" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E396" s="29" t="s">
         <v>19</v>
@@ -18579,7 +18579,7 @@
         <v>15</v>
       </c>
       <c r="H396" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I396" s="31"/>
     </row>
@@ -18594,7 +18594,7 @@
         <v>1592</v>
       </c>
       <c r="D397" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E397" s="29" t="s">
         <v>19</v>
@@ -18621,7 +18621,7 @@
         <v>1593</v>
       </c>
       <c r="D398" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E398" s="29" t="s">
         <v>19</v>
@@ -18648,7 +18648,7 @@
         <v>1594</v>
       </c>
       <c r="D399" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E399" s="29" t="s">
         <v>19</v>
@@ -18675,7 +18675,7 @@
         <v>1595</v>
       </c>
       <c r="D400" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E400" s="29" t="s">
         <v>19</v>
@@ -18702,7 +18702,7 @@
         <v>1596</v>
       </c>
       <c r="D401" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E401" s="29" t="s">
         <v>19</v>
@@ -18729,7 +18729,7 @@
         <v>1597</v>
       </c>
       <c r="D402" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E402" s="29" t="s">
         <v>19</v>
@@ -18756,7 +18756,7 @@
         <v>1598</v>
       </c>
       <c r="D403" s="29" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E403" s="29" t="s">
         <v>19</v>
@@ -18880,7 +18880,7 @@
         <v>1165</v>
       </c>
       <c r="C408" s="31" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="D408" s="29"/>
       <c r="E408" s="29" t="s">
@@ -18955,7 +18955,7 @@
         <v>1166</v>
       </c>
       <c r="C411" s="31" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="D411" s="29"/>
       <c r="E411" s="29" t="s">
@@ -19030,7 +19030,7 @@
         <v>1167</v>
       </c>
       <c r="C414" s="31" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="D414" s="29"/>
       <c r="E414" s="29" t="s">
@@ -19093,7 +19093,7 @@
         <v>15</v>
       </c>
       <c r="H416" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I416" s="31"/>
     </row>
@@ -19105,7 +19105,7 @@
         <v>1168</v>
       </c>
       <c r="C417" s="31" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
       <c r="D417" s="29"/>
       <c r="E417" s="29" t="s">
@@ -19118,7 +19118,7 @@
         <v>15</v>
       </c>
       <c r="H417" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I417" s="31"/>
     </row>
@@ -19230,7 +19230,7 @@
         <v>1170</v>
       </c>
       <c r="C422" s="31" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
       <c r="D422" s="29"/>
       <c r="E422" s="29" t="s">
@@ -19280,7 +19280,7 @@
         <v>1171</v>
       </c>
       <c r="C424" s="31" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
       <c r="D424" s="29"/>
       <c r="E424" s="29" t="s">
@@ -19330,7 +19330,7 @@
         <v>1172</v>
       </c>
       <c r="C426" s="31" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="D426" s="29"/>
       <c r="E426" s="29" t="s">
@@ -19405,7 +19405,7 @@
         <v>1173</v>
       </c>
       <c r="C429" s="31" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="D429" s="29"/>
       <c r="E429" s="29" t="s">
@@ -19455,7 +19455,7 @@
         <v>1174</v>
       </c>
       <c r="C431" s="31" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
       <c r="D431" s="29"/>
       <c r="E431" s="29" t="s">
@@ -19505,7 +19505,7 @@
         <v>1175</v>
       </c>
       <c r="C433" s="31" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="D433" s="29"/>
       <c r="E433" s="29" t="s">
@@ -19555,7 +19555,7 @@
         <v>1176</v>
       </c>
       <c r="C435" s="31" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="D435" s="29"/>
       <c r="E435" s="29" t="s">
@@ -19680,10 +19680,10 @@
         <v>1178</v>
       </c>
       <c r="C440" s="31" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
       <c r="D440" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E440" s="29" t="s">
         <v>19</v>
@@ -19698,7 +19698,7 @@
         <v>17</v>
       </c>
       <c r="I440" s="20" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="441" spans="1:9">
@@ -19712,7 +19712,7 @@
         <v>1624</v>
       </c>
       <c r="D441" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E441" s="29" t="s">
         <v>19</v>
@@ -19736,7 +19736,7 @@
         <v>1178</v>
       </c>
       <c r="C442" s="31" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
       <c r="D442" s="29"/>
       <c r="E442" s="29" t="s">
@@ -19752,7 +19752,7 @@
         <v>17</v>
       </c>
       <c r="I442" s="31" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="443" spans="1:9" ht="60">
@@ -19763,10 +19763,10 @@
         <v>1178</v>
       </c>
       <c r="C443" s="31" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="D443" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E443" s="29" t="s">
         <v>19</v>
@@ -19781,7 +19781,7 @@
         <v>17</v>
       </c>
       <c r="I443" s="31" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="444" spans="1:9">
@@ -19795,7 +19795,7 @@
         <v>1625</v>
       </c>
       <c r="D444" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E444" s="29" t="s">
         <v>19</v>
@@ -19822,7 +19822,7 @@
         <v>1626</v>
       </c>
       <c r="D445" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E445" s="29" t="s">
         <v>19</v>
@@ -19849,7 +19849,7 @@
         <v>1627</v>
       </c>
       <c r="D446" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E446" s="29" t="s">
         <v>19</v>
@@ -19876,7 +19876,7 @@
         <v>1628</v>
       </c>
       <c r="D447" s="29" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E447" s="29" t="s">
         <v>19</v>
@@ -20125,7 +20125,7 @@
         <v>1182</v>
       </c>
       <c r="C457" s="31" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29" t="s">
@@ -20250,7 +20250,7 @@
         <v>1183</v>
       </c>
       <c r="C462" s="31" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="D462" s="29"/>
       <c r="E462" s="29" t="s">
@@ -20378,7 +20378,7 @@
         <v>1646</v>
       </c>
       <c r="D467" s="29" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="E467" s="29" t="s">
         <v>19</v>
@@ -20405,7 +20405,7 @@
         <v>1647</v>
       </c>
       <c r="D468" s="29" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="E468" s="29" t="s">
         <v>19</v>
@@ -20445,7 +20445,7 @@
         <v>20</v>
       </c>
       <c r="I469" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="470" spans="1:9" ht="30">
@@ -20456,7 +20456,7 @@
         <v>1185</v>
       </c>
       <c r="C470" s="31" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="D470" s="29"/>
       <c r="E470" s="29" t="s">
@@ -20756,7 +20756,7 @@
         <v>32</v>
       </c>
       <c r="C482" s="31" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="D482" s="29"/>
       <c r="E482" s="29" t="s">
@@ -23331,7 +23331,7 @@
         <v>1193</v>
       </c>
       <c r="C585" s="31" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="D585" s="29"/>
       <c r="E585" s="29" t="s">
@@ -23431,7 +23431,7 @@
         <v>1194</v>
       </c>
       <c r="C589" s="31" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="D589" s="29"/>
       <c r="E589" s="29" t="s">
@@ -23606,7 +23606,7 @@
         <v>1196</v>
       </c>
       <c r="C596" s="31" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
       <c r="D596" s="29"/>
       <c r="E596" s="29" t="s">
@@ -23622,7 +23622,7 @@
         <v>17</v>
       </c>
       <c r="I596" s="20" t="s">
-        <v>2325</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="597" spans="1:9" ht="45">
@@ -23658,7 +23658,7 @@
         <v>1196</v>
       </c>
       <c r="C598" s="31" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D598" s="29"/>
       <c r="E598" s="29" t="s">
@@ -23674,7 +23674,7 @@
         <v>17</v>
       </c>
       <c r="I598" s="20" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="599" spans="1:9" ht="45">
@@ -23701,7 +23701,7 @@
         <v>20</v>
       </c>
       <c r="I599" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="600" spans="1:9" ht="30">
@@ -23731,7 +23731,7 @@
     </row>
     <row r="601" spans="1:9" ht="60">
       <c r="A601" s="22" t="s">
-        <v>2416</v>
+        <v>2412</v>
       </c>
       <c r="B601" s="30" t="s">
         <v>1196</v>
@@ -23750,7 +23750,7 @@
         <v>15</v>
       </c>
       <c r="H601" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I601" s="31"/>
     </row>
@@ -23762,7 +23762,7 @@
         <v>1196</v>
       </c>
       <c r="C602" s="31" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="D602" s="29"/>
       <c r="E602" s="29" t="s">
@@ -23787,7 +23787,7 @@
         <v>1196</v>
       </c>
       <c r="C603" s="31" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
       <c r="D603" s="29"/>
       <c r="E603" s="29" t="s">
@@ -23803,7 +23803,7 @@
         <v>17</v>
       </c>
       <c r="I603" s="20" t="s">
-        <v>2338</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="604" spans="1:9" ht="45">
@@ -23814,7 +23814,7 @@
         <v>1196</v>
       </c>
       <c r="C604" s="31" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="D604" s="29"/>
       <c r="E604" s="29" t="s">
@@ -23839,7 +23839,7 @@
         <v>1196</v>
       </c>
       <c r="C605" s="31" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="D605" s="29"/>
       <c r="E605" s="29" t="s">
@@ -23855,7 +23855,7 @@
         <v>17</v>
       </c>
       <c r="I605" s="31" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="606" spans="1:9" ht="30">
@@ -23866,7 +23866,7 @@
         <v>1196</v>
       </c>
       <c r="C606" s="31" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
       <c r="D606" s="29"/>
       <c r="E606" s="29" t="s">
@@ -23916,7 +23916,7 @@
         <v>1196</v>
       </c>
       <c r="C608" s="31" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="D608" s="29"/>
       <c r="E608" s="29" t="s">
@@ -23932,7 +23932,7 @@
         <v>17</v>
       </c>
       <c r="I608" s="31" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="609" spans="1:9" ht="75">
@@ -23968,7 +23968,7 @@
         <v>1196</v>
       </c>
       <c r="C610" s="31" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
       <c r="D610" s="29"/>
       <c r="E610" s="29" t="s">
@@ -23984,7 +23984,7 @@
         <v>17</v>
       </c>
       <c r="I610" s="31" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="611" spans="1:9" ht="45">
@@ -23995,7 +23995,7 @@
         <v>1196</v>
       </c>
       <c r="C611" s="31" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="D611" s="29"/>
       <c r="E611" s="29" t="s">
@@ -24020,7 +24020,7 @@
         <v>1196</v>
       </c>
       <c r="C612" s="31" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
       <c r="D612" s="29"/>
       <c r="E612" s="29" t="s">
@@ -24036,7 +24036,7 @@
         <v>17</v>
       </c>
       <c r="I612" s="31" t="s">
-        <v>2361</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="613" spans="1:9" ht="45">
@@ -24047,7 +24047,7 @@
         <v>1196</v>
       </c>
       <c r="C613" s="31" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="D613" s="29"/>
       <c r="E613" s="29" t="s">
@@ -24222,7 +24222,7 @@
         <v>1196</v>
       </c>
       <c r="C620" s="31" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="D620" s="29"/>
       <c r="E620" s="29" t="s">
@@ -24363,7 +24363,7 @@
         <v>17</v>
       </c>
       <c r="I625" s="31" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="626" spans="1:9" ht="30">
@@ -24449,7 +24449,7 @@
         <v>1197</v>
       </c>
       <c r="C629" s="31" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="D629" s="29"/>
       <c r="E629" s="29" t="s">
@@ -24474,7 +24474,7 @@
         <v>1197</v>
       </c>
       <c r="C630" s="31" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="D630" s="29"/>
       <c r="E630" s="29" t="s">
@@ -24499,7 +24499,7 @@
         <v>1197</v>
       </c>
       <c r="C631" s="31" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="D631" s="29"/>
       <c r="E631" s="29" t="s">
@@ -24524,7 +24524,7 @@
         <v>1197</v>
       </c>
       <c r="C632" s="31" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="D632" s="29"/>
       <c r="E632" s="29" t="s">
@@ -24715,7 +24715,7 @@
         <v>17</v>
       </c>
       <c r="I639" s="31" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="640" spans="1:9" ht="45">
@@ -24742,7 +24742,7 @@
         <v>17</v>
       </c>
       <c r="I640" s="31" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="641" spans="1:9" ht="45">
@@ -24756,7 +24756,7 @@
         <v>1796</v>
       </c>
       <c r="D641" s="29" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="E641" s="29" t="s">
         <v>19</v>
@@ -25155,7 +25155,7 @@
         <v>1198</v>
       </c>
       <c r="C657" s="31" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
       <c r="D657" s="29"/>
       <c r="E657" s="29" t="s">
@@ -25171,7 +25171,7 @@
         <v>17</v>
       </c>
       <c r="I657" s="31" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="658" spans="1:9" ht="30">
@@ -25445,7 +25445,7 @@
         <v>15</v>
       </c>
       <c r="H668" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I668" s="31"/>
     </row>
@@ -25470,7 +25470,7 @@
         <v>15</v>
       </c>
       <c r="H669" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I669" s="31"/>
     </row>
@@ -26807,7 +26807,7 @@
         <v>1200</v>
       </c>
       <c r="C723" s="31" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="D723" s="29"/>
       <c r="E723" s="29" t="s">
@@ -26832,7 +26832,7 @@
         <v>1200</v>
       </c>
       <c r="C724" s="31" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
       <c r="D724" s="29"/>
       <c r="E724" s="29" t="s">
@@ -27573,7 +27573,7 @@
         <v>17</v>
       </c>
       <c r="I753" s="31" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="754" spans="1:9" ht="45">
@@ -27600,7 +27600,7 @@
         <v>17</v>
       </c>
       <c r="I754" s="31" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="755" spans="1:9" ht="45">
@@ -27611,7 +27611,7 @@
         <v>1202</v>
       </c>
       <c r="C755" s="31" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
       <c r="D755" s="29"/>
       <c r="E755" s="29" t="s">
@@ -27627,7 +27627,7 @@
         <v>17</v>
       </c>
       <c r="I755" s="31" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="756" spans="1:9" ht="45">
@@ -28263,7 +28263,7 @@
         <v>1203</v>
       </c>
       <c r="C781" s="31" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="D781" s="29"/>
       <c r="E781" s="29" t="s">
@@ -28363,7 +28363,7 @@
         <v>1203</v>
       </c>
       <c r="C785" s="31" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="D785" s="29"/>
       <c r="E785" s="29" t="s">
@@ -28913,7 +28913,7 @@
         <v>1204</v>
       </c>
       <c r="C807" s="31" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="D807" s="29"/>
       <c r="E807" s="29" t="s">
@@ -28938,7 +28938,7 @@
         <v>1204</v>
       </c>
       <c r="C808" s="31" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
       <c r="D808" s="29"/>
       <c r="E808" s="29" t="s">
@@ -29163,7 +29163,7 @@
         <v>1204</v>
       </c>
       <c r="C817" s="31" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="D817" s="29"/>
       <c r="E817" s="29" t="s">
@@ -29313,7 +29313,7 @@
         <v>1204</v>
       </c>
       <c r="C823" s="31" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="D823" s="29"/>
       <c r="E823" s="29" t="s">
@@ -29604,7 +29604,7 @@
         <v>17</v>
       </c>
       <c r="I834" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="835" spans="1:9" ht="30">
@@ -29656,7 +29656,7 @@
         <v>17</v>
       </c>
       <c r="I836" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="837" spans="1:9" ht="30">
@@ -29942,7 +29942,7 @@
         <v>1205</v>
       </c>
       <c r="C848" s="31" t="s">
-        <v>2409</v>
+        <v>2405</v>
       </c>
       <c r="D848" s="29"/>
       <c r="E848" s="29" t="s">
@@ -29958,7 +29958,7 @@
         <v>17</v>
       </c>
       <c r="I848" s="31" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="849" spans="1:9" ht="30">
@@ -30269,7 +30269,7 @@
         <v>1206</v>
       </c>
       <c r="C861" s="20" t="s">
-        <v>2410</v>
+        <v>2406</v>
       </c>
       <c r="D861" s="29"/>
       <c r="E861" s="29" t="s">
@@ -30288,13 +30288,13 @@
     </row>
     <row r="862" spans="1:9" ht="60">
       <c r="A862" s="29" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="B862" s="30" t="s">
         <v>1206</v>
       </c>
       <c r="C862" s="31" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="D862" s="29"/>
       <c r="E862" s="29" t="s">
@@ -30310,7 +30310,7 @@
         <v>17</v>
       </c>
       <c r="I862" s="20" t="s">
-        <v>2401</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="863" spans="1:9" ht="45">
@@ -30771,7 +30771,7 @@
         <v>1206</v>
       </c>
       <c r="C881" s="31" t="s">
-        <v>2403</v>
+        <v>2399</v>
       </c>
       <c r="D881" s="29"/>
       <c r="E881" s="29" t="s">
@@ -31971,7 +31971,7 @@
         <v>1210</v>
       </c>
       <c r="C929" s="31" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="D929" s="29"/>
       <c r="E929" s="29" t="s">
@@ -31987,7 +31987,7 @@
         <v>17</v>
       </c>
       <c r="I929" s="31" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="930" spans="1:9" ht="45">
@@ -32148,7 +32148,7 @@
         <v>1210</v>
       </c>
       <c r="C936" s="31" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="D936" s="29"/>
       <c r="E936" s="29" t="s">
@@ -32164,7 +32164,7 @@
         <v>17</v>
       </c>
       <c r="I936" s="31" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="937" spans="1:9" ht="45">
@@ -32191,7 +32191,7 @@
         <v>17</v>
       </c>
       <c r="I937" s="31" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="938" spans="1:9" ht="45">
@@ -32202,7 +32202,7 @@
         <v>1210</v>
       </c>
       <c r="C938" s="31" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="D938" s="29"/>
       <c r="E938" s="29" t="s">
@@ -32218,7 +32218,7 @@
         <v>17</v>
       </c>
       <c r="I938" s="31" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="939" spans="1:9" ht="30">
@@ -33221,7 +33221,7 @@
       </c>
       <c r="I978" s="31"/>
     </row>
-    <row r="979" spans="1:9" ht="75">
+    <row r="979" spans="1:9" ht="45">
       <c r="A979" s="29" t="s">
         <v>998</v>
       </c>
@@ -33229,7 +33229,7 @@
         <v>1214</v>
       </c>
       <c r="C979" s="31" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="D979" s="29"/>
       <c r="E979" s="29" t="s">
@@ -33244,9 +33244,7 @@
       <c r="H979" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I979" s="31" t="s">
-        <v>2388</v>
-      </c>
+      <c r="I979" s="31"/>
     </row>
     <row r="980" spans="1:9" ht="60">
       <c r="A980" s="29" t="s">
@@ -33449,7 +33447,7 @@
       <c r="I987" s="31"/>
     </row>
     <row r="988" spans="1:9" ht="30">
-      <c r="A988" s="29" t="s">
+      <c r="A988" s="22" t="s">
         <v>1007</v>
       </c>
       <c r="B988" s="30" t="s">
@@ -33469,11 +33467,11 @@
         <v>15</v>
       </c>
       <c r="H988" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I988" s="31"/>
     </row>
-    <row r="989" spans="1:9" ht="60">
+    <row r="989" spans="1:9" ht="45">
       <c r="A989" s="29" t="s">
         <v>1008</v>
       </c>
@@ -33481,7 +33479,7 @@
         <v>1214</v>
       </c>
       <c r="C989" s="31" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="D989" s="29"/>
       <c r="E989" s="29" t="s">
@@ -33496,9 +33494,7 @@
       <c r="H989" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I989" s="31" t="s">
-        <v>2395</v>
-      </c>
+      <c r="I989" s="20"/>
     </row>
     <row r="990" spans="1:9" ht="30">
       <c r="A990" s="29" t="s">
@@ -33736,7 +33732,7 @@
         <v>2129</v>
       </c>
       <c r="D999" s="29" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="E999" s="29" t="s">
         <v>22</v>
@@ -33763,7 +33759,7 @@
         <v>2130</v>
       </c>
       <c r="D1000" s="29" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="E1000" s="29" t="s">
         <v>22</v>
@@ -33790,7 +33786,7 @@
         <v>2131</v>
       </c>
       <c r="D1001" s="29" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="E1001" s="29" t="s">
         <v>22</v>
@@ -33864,10 +33860,10 @@
         <v>1217</v>
       </c>
       <c r="C1004" s="31" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="D1004" s="29" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="E1004" s="29" t="s">
         <v>22</v>
@@ -33894,7 +33890,7 @@
         <v>2134</v>
       </c>
       <c r="D1005" s="29" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="E1005" s="29" t="s">
         <v>22</v>
@@ -33921,7 +33917,7 @@
         <v>2135</v>
       </c>
       <c r="D1006" s="29" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="E1006" s="29" t="s">
         <v>22</v>
@@ -33936,7 +33932,7 @@
         <v>20</v>
       </c>
       <c r="I1006" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1007" spans="1:9" ht="60">
@@ -33950,7 +33946,7 @@
         <v>2136</v>
       </c>
       <c r="D1007" s="29" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="E1007" s="29" t="s">
         <v>22</v>
@@ -33977,7 +33973,7 @@
         <v>2137</v>
       </c>
       <c r="D1008" s="29" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="E1008" s="29" t="s">
         <v>22</v>
@@ -34004,7 +34000,7 @@
         <v>2138</v>
       </c>
       <c r="D1009" s="29" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="E1009" s="29" t="s">
         <v>22</v>
@@ -34078,7 +34074,7 @@
         <v>1217</v>
       </c>
       <c r="C1012" s="31" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="D1012" s="29"/>
       <c r="E1012" s="29" t="s">
@@ -34094,7 +34090,7 @@
         <v>17</v>
       </c>
       <c r="I1012" s="31" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="1013" spans="1:9" ht="30">
@@ -34105,7 +34101,7 @@
         <v>1217</v>
       </c>
       <c r="C1013" s="31" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="D1013" s="29"/>
       <c r="E1013" s="29" t="s">
@@ -34133,7 +34129,7 @@
         <v>2141</v>
       </c>
       <c r="D1014" s="29" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="E1014" s="29" t="s">
         <v>22</v>
@@ -34210,7 +34206,7 @@
         <v>2144</v>
       </c>
       <c r="D1017" s="29" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="E1017" s="29" t="s">
         <v>22</v>
@@ -34225,7 +34221,7 @@
         <v>20</v>
       </c>
       <c r="I1017" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1018" spans="1:9" ht="45">
@@ -34239,7 +34235,7 @@
         <v>2145</v>
       </c>
       <c r="D1018" s="29" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="E1018" s="29" t="s">
         <v>22</v>
@@ -34254,7 +34250,7 @@
         <v>20</v>
       </c>
       <c r="I1018" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1019" spans="1:9" ht="60">
@@ -34268,7 +34264,7 @@
         <v>2146</v>
       </c>
       <c r="D1019" s="29" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="E1019" s="29" t="s">
         <v>22</v>
@@ -34283,7 +34279,7 @@
         <v>20</v>
       </c>
       <c r="I1019" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1020" spans="1:9" ht="45">
@@ -34297,7 +34293,7 @@
         <v>2147</v>
       </c>
       <c r="D1020" s="29" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="E1020" s="29" t="s">
         <v>22</v>
@@ -34312,21 +34308,21 @@
         <v>20</v>
       </c>
       <c r="I1020" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1021" spans="1:9" ht="90">
-      <c r="A1021" s="29" t="s">
+      <c r="A1021" s="22" t="s">
         <v>1040</v>
       </c>
       <c r="B1021" s="30" t="s">
         <v>1217</v>
       </c>
-      <c r="C1021" s="31" t="s">
-        <v>2301</v>
+      <c r="C1021" s="20" t="s">
+        <v>2300</v>
       </c>
       <c r="D1021" s="29" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="E1021" s="29" t="s">
         <v>22</v>
@@ -34341,21 +34337,21 @@
         <v>20</v>
       </c>
       <c r="I1021" s="31" t="s">
-        <v>2231</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:9" ht="105">
-      <c r="A1022" s="29" t="s">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:9" ht="120">
+      <c r="A1022" s="22" t="s">
         <v>1041</v>
       </c>
       <c r="B1022" s="30" t="s">
         <v>1217</v>
       </c>
-      <c r="C1022" s="31" t="s">
-        <v>2148</v>
+      <c r="C1022" s="20" t="s">
+        <v>2417</v>
       </c>
       <c r="D1022" s="29" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="E1022" s="29" t="s">
         <v>22</v>
@@ -34370,7 +34366,7 @@
         <v>20</v>
       </c>
       <c r="I1022" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1023" spans="1:9" ht="45">
@@ -34381,10 +34377,10 @@
         <v>1217</v>
       </c>
       <c r="C1023" s="31" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="D1023" s="29" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="E1023" s="29" t="s">
         <v>22</v>
@@ -34399,7 +34395,7 @@
         <v>21</v>
       </c>
       <c r="I1023" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1024" spans="1:9" ht="45">
@@ -34410,10 +34406,10 @@
         <v>1217</v>
       </c>
       <c r="C1024" s="31" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="D1024" s="29" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="E1024" s="29" t="s">
         <v>22</v>
@@ -34428,7 +34424,7 @@
         <v>21</v>
       </c>
       <c r="I1024" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1025" spans="1:9" ht="60">
@@ -34439,10 +34435,10 @@
         <v>1217</v>
       </c>
       <c r="C1025" s="31" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="D1025" s="29" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="E1025" s="29" t="s">
         <v>22</v>
@@ -34457,7 +34453,7 @@
         <v>20</v>
       </c>
       <c r="I1025" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1026" spans="1:9" ht="60">
@@ -34468,10 +34464,10 @@
         <v>1217</v>
       </c>
       <c r="C1026" s="31" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="D1026" s="29" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="E1026" s="29" t="s">
         <v>22</v>
@@ -34486,7 +34482,7 @@
         <v>20</v>
       </c>
       <c r="I1026" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1027" spans="1:9" ht="75">
@@ -34497,10 +34493,10 @@
         <v>1217</v>
       </c>
       <c r="C1027" s="31" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="D1027" s="29" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="E1027" s="29" t="s">
         <v>22</v>
@@ -34524,10 +34520,10 @@
         <v>1217</v>
       </c>
       <c r="C1028" s="31" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="D1028" s="29" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="E1028" s="29" t="s">
         <v>22</v>
@@ -34542,7 +34538,7 @@
         <v>20</v>
       </c>
       <c r="I1028" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1029" spans="1:9" ht="45">
@@ -34553,7 +34549,7 @@
         <v>1217</v>
       </c>
       <c r="C1029" s="31" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="D1029" s="29"/>
       <c r="E1029" s="29" t="s">
@@ -34572,16 +34568,16 @@
     </row>
     <row r="1030" spans="1:9" ht="45">
       <c r="A1030" s="22" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="B1030" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1030" s="20" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="D1030" s="29" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="E1030" s="29" t="s">
         <v>22</v>
@@ -34596,21 +34592,21 @@
         <v>20</v>
       </c>
       <c r="I1030" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1031" spans="1:9" ht="45">
       <c r="A1031" s="22" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="B1031" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1031" s="20" t="s">
+        <v>2307</v>
+      </c>
+      <c r="D1031" s="29" t="s">
         <v>2308</v>
-      </c>
-      <c r="D1031" s="29" t="s">
-        <v>2309</v>
       </c>
       <c r="E1031" s="29" t="s">
         <v>22</v>
@@ -34625,7 +34621,7 @@
         <v>20</v>
       </c>
       <c r="I1031" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1032" spans="1:9" ht="90">
@@ -34636,10 +34632,10 @@
         <v>1217</v>
       </c>
       <c r="C1032" s="31" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="D1032" s="29" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="E1032" s="29" t="s">
         <v>22</v>
@@ -34654,7 +34650,7 @@
         <v>20</v>
       </c>
       <c r="I1032" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1033" spans="1:9" ht="45">
@@ -34665,10 +34661,10 @@
         <v>1217</v>
       </c>
       <c r="C1033" s="31" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="D1033" s="29" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="E1033" s="29" t="s">
         <v>22</v>
@@ -34683,21 +34679,21 @@
         <v>20</v>
       </c>
       <c r="I1033" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1034" spans="1:9" ht="45">
       <c r="A1034" s="22" t="s">
-        <v>2414</v>
+        <v>2410</v>
       </c>
       <c r="B1034" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1034" s="20" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="D1034" s="29" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="E1034" s="29" t="s">
         <v>22</v>
@@ -34712,21 +34708,21 @@
         <v>20</v>
       </c>
       <c r="I1034" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1035" spans="1:9" ht="45">
       <c r="A1035" s="22" t="s">
-        <v>2415</v>
+        <v>2411</v>
       </c>
       <c r="B1035" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1035" s="20" t="s">
+        <v>2312</v>
+      </c>
+      <c r="D1035" s="29" t="s">
         <v>2313</v>
-      </c>
-      <c r="D1035" s="29" t="s">
-        <v>2314</v>
       </c>
       <c r="E1035" s="29" t="s">
         <v>22</v>
@@ -34741,7 +34737,7 @@
         <v>20</v>
       </c>
       <c r="I1035" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1036" spans="1:9" ht="60">
@@ -34752,10 +34748,10 @@
         <v>1217</v>
       </c>
       <c r="C1036" s="31" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1036" s="29" t="s">
         <v>2318</v>
-      </c>
-      <c r="D1036" s="29" t="s">
-        <v>2319</v>
       </c>
       <c r="E1036" s="29" t="s">
         <v>22</v>
@@ -34779,10 +34775,10 @@
         <v>1217</v>
       </c>
       <c r="C1037" s="31" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="D1037" s="29" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="E1037" s="29" t="s">
         <v>22</v>
@@ -34797,7 +34793,7 @@
         <v>17</v>
       </c>
       <c r="I1037" s="31" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="1038" spans="1:9" ht="105">
@@ -34808,10 +34804,10 @@
         <v>1217</v>
       </c>
       <c r="C1038" s="31" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="D1038" s="29" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="E1038" s="29" t="s">
         <v>22</v>
@@ -34829,16 +34825,16 @@
     </row>
     <row r="1039" spans="1:9" ht="45">
       <c r="A1039" s="29" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="B1039" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1039" s="31" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="D1039" s="29" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="E1039" s="29" t="s">
         <v>22</v>
@@ -34853,21 +34849,21 @@
         <v>20</v>
       </c>
       <c r="I1039" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1040" spans="1:9" ht="45">
       <c r="A1040" s="29" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="B1040" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1040" s="31" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="D1040" s="29" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="E1040" s="29" t="s">
         <v>22</v>
@@ -34882,7 +34878,7 @@
         <v>20</v>
       </c>
       <c r="I1040" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1041" spans="1:9" ht="45">
@@ -34893,10 +34889,10 @@
         <v>1217</v>
       </c>
       <c r="C1041" s="20" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="D1041" s="29" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="E1041" s="29" t="s">
         <v>22</v>
@@ -34920,10 +34916,10 @@
         <v>1217</v>
       </c>
       <c r="C1042" s="20" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="D1042" s="29" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="E1042" s="29" t="s">
         <v>22</v>
@@ -34938,7 +34934,7 @@
         <v>20</v>
       </c>
       <c r="I1042" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1043" spans="1:9" ht="45">
@@ -34949,10 +34945,10 @@
         <v>1217</v>
       </c>
       <c r="C1043" s="20" t="s">
-        <v>2342</v>
+        <v>2340</v>
       </c>
       <c r="D1043" s="22" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="E1043" s="29" t="s">
         <v>22</v>
@@ -34967,21 +34963,21 @@
         <v>20</v>
       </c>
       <c r="I1043" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1044" spans="1:9" ht="45">
       <c r="A1044" s="22" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="B1044" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1044" s="20" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="D1044" s="22" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="E1044" s="22" t="s">
         <v>22</v>
@@ -35005,10 +35001,10 @@
         <v>1217</v>
       </c>
       <c r="C1045" s="20" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="D1045" s="29" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="E1045" s="29" t="s">
         <v>22</v>
@@ -35032,10 +35028,10 @@
         <v>1217</v>
       </c>
       <c r="C1046" s="20" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
       <c r="D1046" s="29" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="E1046" s="29" t="s">
         <v>22</v>
@@ -35053,16 +35049,16 @@
     </row>
     <row r="1047" spans="1:9" ht="60">
       <c r="A1047" s="22" t="s">
-        <v>2335</v>
+        <v>2333</v>
       </c>
       <c r="B1047" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1047" s="20" t="s">
-        <v>2334</v>
+        <v>2332</v>
       </c>
       <c r="D1047" s="22" t="s">
-        <v>2337</v>
+        <v>2335</v>
       </c>
       <c r="E1047" s="29" t="s">
         <v>22</v>
@@ -35077,21 +35073,21 @@
         <v>20</v>
       </c>
       <c r="I1047" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1048" spans="1:9" ht="60">
       <c r="A1048" s="22" t="s">
-        <v>2336</v>
+        <v>2334</v>
       </c>
       <c r="B1048" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1048" s="20" t="s">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="D1048" s="22" t="s">
-        <v>2337</v>
+        <v>2335</v>
       </c>
       <c r="E1048" s="29" t="s">
         <v>22</v>
@@ -35106,7 +35102,7 @@
         <v>20</v>
       </c>
       <c r="I1048" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1049" spans="1:9" ht="75">
@@ -35117,10 +35113,10 @@
         <v>1217</v>
       </c>
       <c r="C1049" s="20" t="s">
-        <v>2339</v>
+        <v>2337</v>
       </c>
       <c r="D1049" s="29" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="E1049" s="29" t="s">
         <v>22</v>
@@ -35144,7 +35140,7 @@
         <v>1217</v>
       </c>
       <c r="C1050" s="20" t="s">
-        <v>2340</v>
+        <v>2338</v>
       </c>
       <c r="D1050" s="29"/>
       <c r="E1050" s="29" t="s">
@@ -35160,7 +35156,7 @@
         <v>17</v>
       </c>
       <c r="I1050" s="31" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="1051" spans="1:9" ht="45">
@@ -35171,7 +35167,7 @@
         <v>1217</v>
       </c>
       <c r="C1051" s="20" t="s">
-        <v>2341</v>
+        <v>2339</v>
       </c>
       <c r="D1051" s="29"/>
       <c r="E1051" s="29" t="s">
@@ -35196,10 +35192,10 @@
         <v>1217</v>
       </c>
       <c r="C1052" s="20" t="s">
-        <v>2343</v>
+        <v>2341</v>
       </c>
       <c r="D1052" s="29" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="E1052" s="29" t="s">
         <v>22</v>
@@ -35223,10 +35219,10 @@
         <v>1217</v>
       </c>
       <c r="C1053" s="20" t="s">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="D1053" s="29" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="E1053" s="29" t="s">
         <v>22</v>
@@ -35250,10 +35246,10 @@
         <v>1217</v>
       </c>
       <c r="C1054" s="20" t="s">
-        <v>2345</v>
+        <v>2343</v>
       </c>
       <c r="D1054" s="29" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="E1054" s="29" t="s">
         <v>22</v>
@@ -35277,10 +35273,10 @@
         <v>1217</v>
       </c>
       <c r="C1055" s="20" t="s">
-        <v>2346</v>
+        <v>2344</v>
       </c>
       <c r="D1055" s="29" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="E1055" s="29" t="s">
         <v>22</v>
@@ -35298,16 +35294,16 @@
     </row>
     <row r="1056" spans="1:9" ht="90">
       <c r="A1056" s="22" t="s">
-        <v>2347</v>
+        <v>2345</v>
       </c>
       <c r="B1056" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1056" s="20" t="s">
-        <v>2350</v>
+        <v>2348</v>
       </c>
       <c r="D1056" s="22" t="s">
-        <v>2348</v>
+        <v>2346</v>
       </c>
       <c r="E1056" s="29" t="s">
         <v>22</v>
@@ -35322,7 +35318,7 @@
         <v>20</v>
       </c>
       <c r="I1056" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1057" spans="1:9" ht="90">
@@ -35333,10 +35329,10 @@
         <v>1217</v>
       </c>
       <c r="C1057" s="20" t="s">
-        <v>2351</v>
+        <v>2349</v>
       </c>
       <c r="D1057" s="29" t="s">
-        <v>2349</v>
+        <v>2347</v>
       </c>
       <c r="E1057" s="29" t="s">
         <v>22</v>
@@ -35351,7 +35347,7 @@
         <v>20</v>
       </c>
       <c r="I1057" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1058" spans="1:9" ht="75">
@@ -35362,10 +35358,10 @@
         <v>1217</v>
       </c>
       <c r="C1058" s="31" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
       <c r="D1058" s="29" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="E1058" s="29" t="s">
         <v>22</v>
@@ -35380,7 +35376,7 @@
         <v>20</v>
       </c>
       <c r="I1058" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1059" spans="1:9" ht="45">
@@ -35391,10 +35387,10 @@
         <v>1217</v>
       </c>
       <c r="C1059" s="20" t="s">
-        <v>2354</v>
+        <v>2352</v>
       </c>
       <c r="D1059" s="29" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="E1059" s="29" t="s">
         <v>22</v>
@@ -35409,7 +35405,7 @@
         <v>20</v>
       </c>
       <c r="I1059" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1060" spans="1:9" ht="60">
@@ -35420,10 +35416,10 @@
         <v>1217</v>
       </c>
       <c r="C1060" s="31" t="s">
-        <v>2355</v>
+        <v>2353</v>
       </c>
       <c r="D1060" s="29" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="E1060" s="29" t="s">
         <v>22</v>
@@ -35438,7 +35434,7 @@
         <v>20</v>
       </c>
       <c r="I1060" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1061" spans="1:9" ht="45">
@@ -35449,7 +35445,7 @@
         <v>1217</v>
       </c>
       <c r="C1061" s="31" t="s">
-        <v>2356</v>
+        <v>2354</v>
       </c>
       <c r="D1061" s="29"/>
       <c r="E1061" s="29" t="s">
@@ -35474,10 +35470,10 @@
         <v>1217</v>
       </c>
       <c r="C1062" s="31" t="s">
-        <v>2357</v>
+        <v>2355</v>
       </c>
       <c r="D1062" s="29" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="E1062" s="29" t="s">
         <v>22</v>
@@ -35501,10 +35497,10 @@
         <v>1217</v>
       </c>
       <c r="C1063" s="31" t="s">
-        <v>2358</v>
+        <v>2356</v>
       </c>
       <c r="D1063" s="29" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="E1063" s="29" t="s">
         <v>22</v>
@@ -35519,7 +35515,7 @@
         <v>20</v>
       </c>
       <c r="I1063" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1064" spans="1:9" ht="45">
@@ -35530,10 +35526,10 @@
         <v>1217</v>
       </c>
       <c r="C1064" s="31" t="s">
-        <v>2360</v>
+        <v>2358</v>
       </c>
       <c r="D1064" s="29" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="E1064" s="29" t="s">
         <v>22</v>
@@ -35548,21 +35544,21 @@
         <v>20</v>
       </c>
       <c r="I1064" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1065" spans="1:9" ht="45">
       <c r="A1065" s="29" t="s">
-        <v>2362</v>
+        <v>2360</v>
       </c>
       <c r="B1065" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1065" s="31" t="s">
-        <v>2359</v>
+        <v>2357</v>
       </c>
       <c r="D1065" s="29" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="E1065" s="29" t="s">
         <v>22</v>
@@ -35577,7 +35573,7 @@
         <v>20</v>
       </c>
       <c r="I1065" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1066" spans="1:9" ht="45">
@@ -35588,10 +35584,10 @@
         <v>1217</v>
       </c>
       <c r="C1066" s="31" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
       <c r="D1066" s="29" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="E1066" s="29" t="s">
         <v>22</v>
@@ -35615,10 +35611,10 @@
         <v>1217</v>
       </c>
       <c r="C1067" s="31" t="s">
-        <v>2411</v>
+        <v>2407</v>
       </c>
       <c r="D1067" s="29" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="E1067" s="29" t="s">
         <v>22</v>
@@ -35642,10 +35638,10 @@
         <v>1217</v>
       </c>
       <c r="C1068" s="31" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
       <c r="D1068" s="29" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="E1068" s="29" t="s">
         <v>22</v>
@@ -35669,10 +35665,10 @@
         <v>1217</v>
       </c>
       <c r="C1069" s="31" t="s">
-        <v>2366</v>
+        <v>2364</v>
       </c>
       <c r="D1069" s="29" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="E1069" s="29" t="s">
         <v>22</v>
@@ -35696,7 +35692,7 @@
         <v>1217</v>
       </c>
       <c r="C1070" s="31" t="s">
-        <v>2367</v>
+        <v>2365</v>
       </c>
       <c r="D1070" s="29"/>
       <c r="E1070" s="29" t="s">
@@ -35721,10 +35717,10 @@
         <v>1217</v>
       </c>
       <c r="C1071" s="31" t="s">
-        <v>2368</v>
+        <v>2366</v>
       </c>
       <c r="D1071" s="29" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="E1071" s="29" t="s">
         <v>22</v>
@@ -35748,10 +35744,10 @@
         <v>1217</v>
       </c>
       <c r="C1072" s="20" t="s">
-        <v>2413</v>
+        <v>2409</v>
       </c>
       <c r="D1072" s="29" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="E1072" s="29" t="s">
         <v>22</v>
@@ -35766,7 +35762,7 @@
         <v>20</v>
       </c>
       <c r="I1072" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1073" spans="1:9" ht="30">
@@ -35777,10 +35773,10 @@
         <v>1217</v>
       </c>
       <c r="C1073" s="31" t="s">
-        <v>2369</v>
+        <v>2367</v>
       </c>
       <c r="D1073" s="29" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="E1073" s="29" t="s">
         <v>22</v>
@@ -35804,10 +35800,10 @@
         <v>1217</v>
       </c>
       <c r="C1074" s="31" t="s">
-        <v>2370</v>
+        <v>2368</v>
       </c>
       <c r="D1074" s="29" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="E1074" s="29" t="s">
         <v>22</v>
@@ -35831,10 +35827,10 @@
         <v>1217</v>
       </c>
       <c r="C1075" s="31" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="D1075" s="29" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="E1075" s="29" t="s">
         <v>22</v>
@@ -35858,10 +35854,10 @@
         <v>1217</v>
       </c>
       <c r="C1076" s="31" t="s">
-        <v>2372</v>
+        <v>2370</v>
       </c>
       <c r="D1076" s="29" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="E1076" s="29" t="s">
         <v>22</v>
@@ -35885,10 +35881,10 @@
         <v>1217</v>
       </c>
       <c r="C1077" s="31" t="s">
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="D1077" s="29" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="E1077" s="29" t="s">
         <v>22</v>
@@ -35912,10 +35908,10 @@
         <v>1217</v>
       </c>
       <c r="C1078" s="31" t="s">
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="D1078" s="29" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="E1078" s="29" t="s">
         <v>22</v>
@@ -35939,10 +35935,10 @@
         <v>1217</v>
       </c>
       <c r="C1079" s="31" t="s">
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="D1079" s="29" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="E1079" s="29" t="s">
         <v>22</v>
@@ -35966,10 +35962,10 @@
         <v>1217</v>
       </c>
       <c r="C1080" s="31" t="s">
-        <v>2376</v>
+        <v>2374</v>
       </c>
       <c r="D1080" s="29" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="E1080" s="29" t="s">
         <v>22</v>
@@ -35993,10 +35989,10 @@
         <v>1217</v>
       </c>
       <c r="C1081" s="31" t="s">
-        <v>2377</v>
+        <v>2375</v>
       </c>
       <c r="D1081" s="29" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="E1081" s="29" t="s">
         <v>22</v>
@@ -36020,10 +36016,10 @@
         <v>1217</v>
       </c>
       <c r="C1082" s="31" t="s">
-        <v>2378</v>
+        <v>2376</v>
       </c>
       <c r="D1082" s="29" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="E1082" s="29" t="s">
         <v>22</v>
@@ -36038,7 +36034,7 @@
         <v>20</v>
       </c>
       <c r="I1082" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1083" spans="1:9" ht="60">
@@ -36049,10 +36045,10 @@
         <v>1217</v>
       </c>
       <c r="C1083" s="31" t="s">
-        <v>2399</v>
+        <v>2395</v>
       </c>
       <c r="D1083" s="29" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="E1083" s="29" t="s">
         <v>22</v>
@@ -36067,21 +36063,21 @@
         <v>20</v>
       </c>
       <c r="I1083" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1084" spans="1:9" ht="45">
       <c r="A1084" s="22" t="s">
-        <v>2396</v>
+        <v>2392</v>
       </c>
       <c r="B1084" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1084" s="20" t="s">
-        <v>2400</v>
+        <v>2396</v>
       </c>
       <c r="D1084" s="29" t="s">
-        <v>2398</v>
+        <v>2394</v>
       </c>
       <c r="E1084" s="29" t="s">
         <v>22</v>
@@ -36096,21 +36092,21 @@
         <v>20</v>
       </c>
       <c r="I1084" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1085" spans="1:9" ht="60">
       <c r="A1085" s="22" t="s">
-        <v>2397</v>
+        <v>2393</v>
       </c>
       <c r="B1085" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1085" s="20" t="s">
-        <v>2402</v>
+        <v>2398</v>
       </c>
       <c r="D1085" s="29" t="s">
-        <v>2398</v>
+        <v>2394</v>
       </c>
       <c r="E1085" s="29" t="s">
         <v>22</v>
@@ -36125,21 +36121,21 @@
         <v>20</v>
       </c>
       <c r="I1085" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1086" spans="1:9" ht="45">
       <c r="A1086" s="29" t="s">
-        <v>2406</v>
+        <v>2402</v>
       </c>
       <c r="B1086" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1086" s="31" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1086" s="29" t="s">
         <v>2404</v>
-      </c>
-      <c r="D1086" s="29" t="s">
-        <v>2408</v>
       </c>
       <c r="E1086" s="29" t="s">
         <v>22</v>
@@ -36154,21 +36150,21 @@
         <v>17</v>
       </c>
       <c r="I1086" s="20" t="s">
-        <v>2417</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="1087" spans="1:9" ht="45">
       <c r="A1087" s="29" t="s">
-        <v>2407</v>
+        <v>2403</v>
       </c>
       <c r="B1087" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1087" s="31" t="s">
-        <v>2405</v>
+        <v>2401</v>
       </c>
       <c r="D1087" s="29" t="s">
-        <v>2408</v>
+        <v>2404</v>
       </c>
       <c r="E1087" s="29" t="s">
         <v>22</v>
@@ -36183,7 +36179,7 @@
         <v>17</v>
       </c>
       <c r="I1087" s="20" t="s">
-        <v>2418</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="1088" spans="1:9" ht="60">
@@ -36194,10 +36190,10 @@
         <v>1217</v>
       </c>
       <c r="C1088" s="31" t="s">
-        <v>2379</v>
+        <v>2377</v>
       </c>
       <c r="D1088" s="29" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="E1088" s="29" t="s">
         <v>22</v>
@@ -36212,7 +36208,7 @@
         <v>20</v>
       </c>
       <c r="I1088" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1089" spans="1:9" ht="45">
@@ -36223,10 +36219,10 @@
         <v>1217</v>
       </c>
       <c r="C1089" s="31" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="D1089" s="29" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="E1089" s="29" t="s">
         <v>22</v>
@@ -36241,7 +36237,7 @@
         <v>20</v>
       </c>
       <c r="I1089" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1090" spans="1:9" ht="60">
@@ -36252,10 +36248,10 @@
         <v>1217</v>
       </c>
       <c r="C1090" s="31" t="s">
-        <v>2412</v>
+        <v>2408</v>
       </c>
       <c r="D1090" s="29" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="E1090" s="29" t="s">
         <v>22</v>
@@ -36270,7 +36266,7 @@
         <v>20</v>
       </c>
       <c r="I1090" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1091" spans="1:9" ht="45">
@@ -36281,10 +36277,10 @@
         <v>1217</v>
       </c>
       <c r="C1091" s="31" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="D1091" s="29" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="E1091" s="29" t="s">
         <v>22</v>
@@ -36299,7 +36295,7 @@
         <v>20</v>
       </c>
       <c r="I1091" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1092" spans="1:9" ht="75">
@@ -36310,10 +36306,10 @@
         <v>1217</v>
       </c>
       <c r="C1092" s="31" t="s">
-        <v>2380</v>
+        <v>2378</v>
       </c>
       <c r="D1092" s="29" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="E1092" s="29" t="s">
         <v>22</v>
@@ -36328,21 +36324,21 @@
         <v>20</v>
       </c>
       <c r="I1092" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1093" spans="1:9" ht="45">
       <c r="A1093" s="22" t="s">
-        <v>2384</v>
+        <v>2382</v>
       </c>
       <c r="B1093" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1093" s="31" t="s">
-        <v>2381</v>
+        <v>2379</v>
       </c>
       <c r="D1093" s="29" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="E1093" s="29" t="s">
         <v>22</v>
@@ -36354,24 +36350,22 @@
         <v>15</v>
       </c>
       <c r="H1093" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1093" s="31" t="s">
-        <v>2231</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1093" s="31"/>
     </row>
     <row r="1094" spans="1:9" ht="45">
-      <c r="A1094" s="29" t="s">
-        <v>2385</v>
+      <c r="A1094" s="22" t="s">
+        <v>2383</v>
       </c>
       <c r="B1094" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1094" s="31" t="s">
-        <v>2382</v>
+        <v>2380</v>
       </c>
       <c r="D1094" s="29" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="E1094" s="29" t="s">
         <v>22</v>
@@ -36383,24 +36377,22 @@
         <v>15</v>
       </c>
       <c r="H1094" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1094" s="31" t="s">
-        <v>2231</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1094" s="31"/>
     </row>
     <row r="1095" spans="1:9" ht="45">
-      <c r="A1095" s="29" t="s">
-        <v>2386</v>
+      <c r="A1095" s="22" t="s">
+        <v>2384</v>
       </c>
       <c r="B1095" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1095" s="31" t="s">
-        <v>2383</v>
+        <v>2381</v>
       </c>
       <c r="D1095" s="29" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="E1095" s="29" t="s">
         <v>22</v>
@@ -36412,24 +36404,22 @@
         <v>15</v>
       </c>
       <c r="H1095" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1095" s="31" t="s">
-        <v>2231</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1095" s="31"/>
     </row>
     <row r="1096" spans="1:9" ht="45">
-      <c r="A1096" s="29" t="s">
-        <v>2391</v>
+      <c r="A1096" s="22" t="s">
+        <v>2388</v>
       </c>
       <c r="B1096" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1096" s="31" t="s">
-        <v>2389</v>
+        <v>2386</v>
       </c>
       <c r="D1096" s="29" t="s">
-        <v>2393</v>
+        <v>2390</v>
       </c>
       <c r="E1096" s="29" t="s">
         <v>22</v>
@@ -36441,24 +36431,22 @@
         <v>15</v>
       </c>
       <c r="H1096" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1096" s="31" t="s">
-        <v>2231</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1096" s="31"/>
     </row>
     <row r="1097" spans="1:9" ht="45">
-      <c r="A1097" s="29" t="s">
-        <v>2392</v>
+      <c r="A1097" s="22" t="s">
+        <v>2389</v>
       </c>
       <c r="B1097" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1097" s="31" t="s">
-        <v>2390</v>
+        <v>2387</v>
       </c>
       <c r="D1097" s="29" t="s">
-        <v>2394</v>
+        <v>2391</v>
       </c>
       <c r="E1097" s="29" t="s">
         <v>22</v>
@@ -36470,11 +36458,9 @@
         <v>15</v>
       </c>
       <c r="H1097" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1097" s="31" t="s">
-        <v>2231</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1097" s="31"/>
     </row>
     <row r="1098" spans="1:9" ht="45">
       <c r="A1098" s="29" t="s">
@@ -36484,10 +36470,10 @@
         <v>1217</v>
       </c>
       <c r="C1098" s="31" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="D1098" s="29" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="E1098" s="29" t="s">
         <v>22</v>
@@ -36502,7 +36488,7 @@
         <v>20</v>
       </c>
       <c r="I1098" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1099" spans="1:9" ht="60">
@@ -36513,10 +36499,10 @@
         <v>1217</v>
       </c>
       <c r="C1099" s="31" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="D1099" s="29" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="E1099" s="29" t="s">
         <v>22</v>
@@ -36531,7 +36517,7 @@
         <v>20</v>
       </c>
       <c r="I1099" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1100" spans="1:9" ht="45">
@@ -36542,7 +36528,7 @@
         <v>1217</v>
       </c>
       <c r="C1100" s="31" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="D1100" s="29"/>
       <c r="E1100" s="29" t="s">
@@ -36558,18 +36544,18 @@
         <v>21</v>
       </c>
       <c r="I1100" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1101" spans="1:9" ht="45">
       <c r="A1101" s="29" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="B1101" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1101" s="31" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
       <c r="D1101" s="29"/>
       <c r="E1101" s="29" t="s">
@@ -36585,7 +36571,7 @@
         <v>21</v>
       </c>
       <c r="I1101" s="32" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="1102" spans="1:9" ht="30">
@@ -36596,7 +36582,7 @@
         <v>1120</v>
       </c>
       <c r="C1102" s="31" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="D1102" s="29"/>
       <c r="E1102" s="29" t="s">
@@ -36621,7 +36607,7 @@
         <v>1120</v>
       </c>
       <c r="C1103" s="31" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="D1103" s="29"/>
       <c r="E1103" s="29" t="s">
@@ -36646,7 +36632,7 @@
         <v>1218</v>
       </c>
       <c r="C1104" s="31" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="D1104" s="29"/>
       <c r="E1104" s="29" t="s">
@@ -36671,7 +36657,7 @@
         <v>1218</v>
       </c>
       <c r="C1105" s="31" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="D1105" s="29"/>
       <c r="E1105" s="29" t="s">
@@ -36696,7 +36682,7 @@
         <v>1218</v>
       </c>
       <c r="C1106" s="31" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="D1106" s="29"/>
       <c r="E1106" s="29" t="s">
@@ -36721,7 +36707,7 @@
         <v>1219</v>
       </c>
       <c r="C1107" s="31" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D1107" s="29"/>
       <c r="E1107" s="29" t="s">
@@ -36748,11 +36734,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36760,6 +36741,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1102:I1107 A20:H1040 I20:I1043 A34:I1100">
@@ -36878,12 +36864,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -36932,6 +36912,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -36942,20 +36928,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36970,6 +36942,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[MS-OXCSTOR] Add new requirement
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -7187,9 +7187,6 @@
     <t>MS-OXCSTOR_R3068003:i</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCSTOR_R3068003001, MS-OXCSTOR_R3068003002.</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] When a database is restored from backup, the implementation assigns a new randomly-generated REPLGUID to the database and then adds this new REPLGUID, along with a new REPLID, to the REPLID and REPLGUID to-and-from mapping table. (&lt;17&gt; Section 3.2.3: When a database is restored from backup, Exchange 2003 and Exchange 2007 assign a new randomly-generated REPLGUID to the database and then add this new REPLGUID, along with a new REPLID, to the REPLID and REPLGUID to-and-from mapping table.)</t>
   </si>
   <si>
@@ -7497,6 +7494,10 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior]  Implementation returns the Folder ID of all of the following folders in this field [FolderIds in RopLogon ROP Success Response Buffer for Public Folders]: Public Folders Root Folder (All other folders listed here are direct or indirect children of this folder), Interpersonal messages subtree, Non-interpersonal messages subtree, EForms Registry, Free/Busy Data, Offline address book Data, EForms Registry for the user's locale, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, NNTP Article Index, Empty, Empty, Empty. (Exchange 2003, Exchange 2007 and Exchange 2010 follow this behavior)</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCSTOR_R306800301, MS-OXCSTOR_R306800302.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -7504,14 +7505,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7708,13 +7709,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -7747,7 +7748,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7772,21 +7773,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7810,6 +7796,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8776,15 +8777,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
@@ -8826,127 +8827,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8959,12 +8960,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8977,12 +8978,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8995,12 +8996,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9013,60 +9014,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9100,7 +9101,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="20" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
@@ -9125,7 +9126,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
@@ -9200,7 +9201,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A24" s="22" t="s">
         <v>47</v>
       </c>
@@ -9250,7 +9251,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="26" spans="1:12" s="23" customFormat="1">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -9425,7 +9426,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
+    <row r="33" spans="1:9" s="23" customFormat="1">
       <c r="A33" s="22" t="s">
         <v>56</v>
       </c>
@@ -9725,7 +9726,7 @@
       </c>
       <c r="I44" s="31"/>
     </row>
-    <row r="45" spans="1:9" ht="45">
+    <row r="45" spans="1:9" ht="30">
       <c r="A45" s="29" t="s">
         <v>66</v>
       </c>
@@ -9750,7 +9751,7 @@
       </c>
       <c r="I45" s="31"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9">
       <c r="A46" s="29" t="s">
         <v>67</v>
       </c>
@@ -9775,7 +9776,7 @@
       </c>
       <c r="I46" s="31"/>
     </row>
-    <row r="47" spans="1:9" ht="30">
+    <row r="47" spans="1:9">
       <c r="A47" s="29" t="s">
         <v>68</v>
       </c>
@@ -9925,7 +9926,7 @@
       </c>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="1:9" ht="45">
+    <row r="53" spans="1:9" ht="30">
       <c r="A53" s="29" t="s">
         <v>74</v>
       </c>
@@ -9952,7 +9953,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9">
       <c r="A54" s="29" t="s">
         <v>75</v>
       </c>
@@ -10002,7 +10003,7 @@
       </c>
       <c r="I55" s="31"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9">
       <c r="A56" s="29" t="s">
         <v>77</v>
       </c>
@@ -10052,7 +10053,7 @@
       </c>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="1:9" ht="30">
+    <row r="58" spans="1:9">
       <c r="A58" s="29" t="s">
         <v>79</v>
       </c>
@@ -10102,7 +10103,7 @@
       </c>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="30">
       <c r="A60" s="29" t="s">
         <v>81</v>
       </c>
@@ -10127,7 +10128,7 @@
       </c>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="1:9" ht="60">
+    <row r="61" spans="1:9" ht="45">
       <c r="A61" s="29" t="s">
         <v>82</v>
       </c>
@@ -10302,7 +10303,7 @@
       </c>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="45">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="29" t="s">
         <v>89</v>
       </c>
@@ -10329,7 +10330,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="45">
+    <row r="69" spans="1:9" ht="30">
       <c r="A69" s="29" t="s">
         <v>90</v>
       </c>
@@ -10356,7 +10357,7 @@
       </c>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9">
       <c r="A70" s="29" t="s">
         <v>91</v>
       </c>
@@ -10408,7 +10409,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9">
       <c r="A72" s="29" t="s">
         <v>93</v>
       </c>
@@ -10458,7 +10459,7 @@
       </c>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="1:9" ht="60">
+    <row r="74" spans="1:9" ht="45">
       <c r="A74" s="29" t="s">
         <v>95</v>
       </c>
@@ -10535,7 +10536,7 @@
       </c>
       <c r="I76" s="31"/>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9">
       <c r="A77" s="29" t="s">
         <v>98</v>
       </c>
@@ -10560,7 +10561,7 @@
       </c>
       <c r="I77" s="31"/>
     </row>
-    <row r="78" spans="1:9" ht="60">
+    <row r="78" spans="1:9" ht="45">
       <c r="A78" s="29" t="s">
         <v>99</v>
       </c>
@@ -10610,7 +10611,7 @@
       </c>
       <c r="I79" s="31"/>
     </row>
-    <row r="80" spans="1:9" ht="60">
+    <row r="80" spans="1:9" ht="45">
       <c r="A80" s="29" t="s">
         <v>101</v>
       </c>
@@ -10760,7 +10761,7 @@
       </c>
       <c r="I85" s="31"/>
     </row>
-    <row r="86" spans="1:9" ht="45">
+    <row r="86" spans="1:9" ht="30">
       <c r="A86" s="29" t="s">
         <v>107</v>
       </c>
@@ -10785,7 +10786,7 @@
       </c>
       <c r="I86" s="31"/>
     </row>
-    <row r="87" spans="1:9" ht="60">
+    <row r="87" spans="1:9" ht="45">
       <c r="A87" s="29" t="s">
         <v>108</v>
       </c>
@@ -10910,7 +10911,7 @@
       </c>
       <c r="I91" s="31"/>
     </row>
-    <row r="92" spans="1:9" ht="90">
+    <row r="92" spans="1:9" ht="75">
       <c r="A92" s="29" t="s">
         <v>113</v>
       </c>
@@ -10935,7 +10936,7 @@
       </c>
       <c r="I92" s="31"/>
     </row>
-    <row r="93" spans="1:9" ht="75">
+    <row r="93" spans="1:9" ht="60">
       <c r="A93" s="29" t="s">
         <v>114</v>
       </c>
@@ -11162,7 +11163,7 @@
       </c>
       <c r="I101" s="31"/>
     </row>
-    <row r="102" spans="1:9" ht="30">
+    <row r="102" spans="1:9">
       <c r="A102" s="29" t="s">
         <v>123</v>
       </c>
@@ -11237,7 +11238,7 @@
       </c>
       <c r="I104" s="31"/>
     </row>
-    <row r="105" spans="1:9" ht="45">
+    <row r="105" spans="1:9" ht="30">
       <c r="A105" s="29" t="s">
         <v>126</v>
       </c>
@@ -11262,7 +11263,7 @@
       </c>
       <c r="I105" s="31"/>
     </row>
-    <row r="106" spans="1:9" ht="45">
+    <row r="106" spans="1:9" ht="30">
       <c r="A106" s="29" t="s">
         <v>127</v>
       </c>
@@ -11312,7 +11313,7 @@
       </c>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="1:9" ht="45">
+    <row r="108" spans="1:9" ht="30">
       <c r="A108" s="29" t="s">
         <v>129</v>
       </c>
@@ -11362,7 +11363,7 @@
       </c>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="1:9" ht="45">
+    <row r="110" spans="1:9" ht="30">
       <c r="A110" s="29" t="s">
         <v>131</v>
       </c>
@@ -11412,7 +11413,7 @@
       </c>
       <c r="I111" s="31"/>
     </row>
-    <row r="112" spans="1:9" ht="45">
+    <row r="112" spans="1:9" ht="30">
       <c r="A112" s="29" t="s">
         <v>133</v>
       </c>
@@ -11512,7 +11513,7 @@
       </c>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="1:9" ht="30">
+    <row r="116" spans="1:9">
       <c r="A116" s="29" t="s">
         <v>137</v>
       </c>
@@ -11537,7 +11538,7 @@
       </c>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="1:9" ht="60">
+    <row r="117" spans="1:9" ht="45">
       <c r="A117" s="29" t="s">
         <v>138</v>
       </c>
@@ -11564,7 +11565,7 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9">
       <c r="A118" s="29" t="s">
         <v>139</v>
       </c>
@@ -11614,7 +11615,7 @@
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:9" ht="45">
+    <row r="120" spans="1:9" ht="30">
       <c r="A120" s="29" t="s">
         <v>141</v>
       </c>
@@ -11741,7 +11742,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="90">
+    <row r="125" spans="1:9" ht="75">
       <c r="A125" s="29" t="s">
         <v>146</v>
       </c>
@@ -11765,7 +11766,7 @@
         <v>17</v>
       </c>
       <c r="I125" s="20" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="30">
@@ -11793,7 +11794,7 @@
       </c>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="1:9" ht="45">
+    <row r="127" spans="1:9" ht="30">
       <c r="A127" s="29" t="s">
         <v>148</v>
       </c>
@@ -11943,7 +11944,7 @@
       </c>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="1:9" ht="60">
+    <row r="133" spans="1:9" ht="45">
       <c r="A133" s="29" t="s">
         <v>154</v>
       </c>
@@ -12095,7 +12096,7 @@
       </c>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="1:9" ht="45">
+    <row r="139" spans="1:9" ht="30">
       <c r="A139" s="29" t="s">
         <v>160</v>
       </c>
@@ -12295,7 +12296,7 @@
       </c>
       <c r="I146" s="31"/>
     </row>
-    <row r="147" spans="1:9" ht="45">
+    <row r="147" spans="1:9" ht="30">
       <c r="A147" s="29" t="s">
         <v>168</v>
       </c>
@@ -12320,7 +12321,7 @@
       </c>
       <c r="I147" s="31"/>
     </row>
-    <row r="148" spans="1:9" ht="45">
+    <row r="148" spans="1:9" ht="30">
       <c r="A148" s="29" t="s">
         <v>169</v>
       </c>
@@ -12345,7 +12346,7 @@
       </c>
       <c r="I148" s="31"/>
     </row>
-    <row r="149" spans="1:9" ht="45">
+    <row r="149" spans="1:9" ht="30">
       <c r="A149" s="29" t="s">
         <v>170</v>
       </c>
@@ -12370,7 +12371,7 @@
       </c>
       <c r="I149" s="31"/>
     </row>
-    <row r="150" spans="1:9" ht="45">
+    <row r="150" spans="1:9" ht="30">
       <c r="A150" s="29" t="s">
         <v>171</v>
       </c>
@@ -12395,7 +12396,7 @@
       </c>
       <c r="I150" s="31"/>
     </row>
-    <row r="151" spans="1:9" ht="45">
+    <row r="151" spans="1:9" ht="30">
       <c r="A151" s="29" t="s">
         <v>172</v>
       </c>
@@ -12520,7 +12521,7 @@
       </c>
       <c r="I155" s="31"/>
     </row>
-    <row r="156" spans="1:9" ht="45">
+    <row r="156" spans="1:9" ht="30">
       <c r="A156" s="29" t="s">
         <v>177</v>
       </c>
@@ -12595,7 +12596,7 @@
       </c>
       <c r="I158" s="31"/>
     </row>
-    <row r="159" spans="1:9" ht="45">
+    <row r="159" spans="1:9" ht="30">
       <c r="A159" s="29" t="s">
         <v>180</v>
       </c>
@@ -12620,7 +12621,7 @@
       </c>
       <c r="I159" s="31"/>
     </row>
-    <row r="160" spans="1:9" ht="45">
+    <row r="160" spans="1:9" ht="30">
       <c r="A160" s="29" t="s">
         <v>181</v>
       </c>
@@ -12645,7 +12646,7 @@
       </c>
       <c r="I160" s="31"/>
     </row>
-    <row r="161" spans="1:9" ht="45">
+    <row r="161" spans="1:9" ht="30">
       <c r="A161" s="29" t="s">
         <v>182</v>
       </c>
@@ -12670,7 +12671,7 @@
       </c>
       <c r="I161" s="31"/>
     </row>
-    <row r="162" spans="1:9" ht="45">
+    <row r="162" spans="1:9" ht="30">
       <c r="A162" s="29" t="s">
         <v>183</v>
       </c>
@@ -12745,7 +12746,7 @@
       </c>
       <c r="I164" s="31"/>
     </row>
-    <row r="165" spans="1:9" ht="45">
+    <row r="165" spans="1:9" ht="30">
       <c r="A165" s="29" t="s">
         <v>186</v>
       </c>
@@ -12895,7 +12896,7 @@
       </c>
       <c r="I170" s="31"/>
     </row>
-    <row r="171" spans="1:9" ht="45">
+    <row r="171" spans="1:9" ht="30">
       <c r="A171" s="29" t="s">
         <v>192</v>
       </c>
@@ -12920,7 +12921,7 @@
       </c>
       <c r="I171" s="31"/>
     </row>
-    <row r="172" spans="1:9" ht="45">
+    <row r="172" spans="1:9" ht="30">
       <c r="A172" s="29" t="s">
         <v>193</v>
       </c>
@@ -13045,7 +13046,7 @@
       </c>
       <c r="I176" s="31"/>
     </row>
-    <row r="177" spans="1:9" ht="45">
+    <row r="177" spans="1:9" ht="30">
       <c r="A177" s="29" t="s">
         <v>198</v>
       </c>
@@ -13070,7 +13071,7 @@
       </c>
       <c r="I177" s="31"/>
     </row>
-    <row r="178" spans="1:9" ht="45">
+    <row r="178" spans="1:9" ht="30">
       <c r="A178" s="29" t="s">
         <v>199</v>
       </c>
@@ -13120,7 +13121,7 @@
       </c>
       <c r="I179" s="31"/>
     </row>
-    <row r="180" spans="1:9" ht="45">
+    <row r="180" spans="1:9" ht="30">
       <c r="A180" s="29" t="s">
         <v>201</v>
       </c>
@@ -13270,7 +13271,7 @@
       </c>
       <c r="I185" s="31"/>
     </row>
-    <row r="186" spans="1:9" ht="45">
+    <row r="186" spans="1:9" ht="30">
       <c r="A186" s="29" t="s">
         <v>207</v>
       </c>
@@ -13370,7 +13371,7 @@
       </c>
       <c r="I189" s="31"/>
     </row>
-    <row r="190" spans="1:9" ht="45">
+    <row r="190" spans="1:9" ht="30">
       <c r="A190" s="29" t="s">
         <v>211</v>
       </c>
@@ -13395,7 +13396,7 @@
       </c>
       <c r="I190" s="31"/>
     </row>
-    <row r="191" spans="1:9" ht="30">
+    <row r="191" spans="1:9">
       <c r="A191" s="29" t="s">
         <v>212</v>
       </c>
@@ -13645,7 +13646,7 @@
       </c>
       <c r="I200" s="31"/>
     </row>
-    <row r="201" spans="1:9" ht="45">
+    <row r="201" spans="1:9" ht="30">
       <c r="A201" s="29" t="s">
         <v>222</v>
       </c>
@@ -13720,7 +13721,7 @@
       </c>
       <c r="I203" s="31"/>
     </row>
-    <row r="204" spans="1:9" ht="45">
+    <row r="204" spans="1:9" ht="30">
       <c r="A204" s="29" t="s">
         <v>225</v>
       </c>
@@ -13745,7 +13746,7 @@
       </c>
       <c r="I204" s="31"/>
     </row>
-    <row r="205" spans="1:9" ht="60">
+    <row r="205" spans="1:9" ht="45">
       <c r="A205" s="29" t="s">
         <v>226</v>
       </c>
@@ -13820,7 +13821,7 @@
       </c>
       <c r="I207" s="31"/>
     </row>
-    <row r="208" spans="1:9" ht="45">
+    <row r="208" spans="1:9" ht="30">
       <c r="A208" s="29" t="s">
         <v>229</v>
       </c>
@@ -13870,7 +13871,7 @@
       </c>
       <c r="I209" s="31"/>
     </row>
-    <row r="210" spans="1:9" ht="75">
+    <row r="210" spans="1:9" ht="60">
       <c r="A210" s="29" t="s">
         <v>231</v>
       </c>
@@ -13895,7 +13896,7 @@
       </c>
       <c r="I210" s="31"/>
     </row>
-    <row r="211" spans="1:9" ht="45">
+    <row r="211" spans="1:9" ht="30">
       <c r="A211" s="29" t="s">
         <v>232</v>
       </c>
@@ -13920,7 +13921,7 @@
       </c>
       <c r="I211" s="31"/>
     </row>
-    <row r="212" spans="1:9" ht="45">
+    <row r="212" spans="1:9" ht="30">
       <c r="A212" s="29" t="s">
         <v>233</v>
       </c>
@@ -13945,7 +13946,7 @@
       </c>
       <c r="I212" s="31"/>
     </row>
-    <row r="213" spans="1:9" ht="60">
+    <row r="213" spans="1:9" ht="45">
       <c r="A213" s="29" t="s">
         <v>234</v>
       </c>
@@ -14022,7 +14023,7 @@
       </c>
       <c r="I215" s="31"/>
     </row>
-    <row r="216" spans="1:9" ht="30">
+    <row r="216" spans="1:9">
       <c r="A216" s="29" t="s">
         <v>237</v>
       </c>
@@ -14047,7 +14048,7 @@
       </c>
       <c r="I216" s="31"/>
     </row>
-    <row r="217" spans="1:9" ht="45">
+    <row r="217" spans="1:9" ht="30">
       <c r="A217" s="29" t="s">
         <v>238</v>
       </c>
@@ -14097,7 +14098,7 @@
       </c>
       <c r="I218" s="31"/>
     </row>
-    <row r="219" spans="1:9" ht="45">
+    <row r="219" spans="1:9" ht="30">
       <c r="A219" s="29" t="s">
         <v>240</v>
       </c>
@@ -14122,7 +14123,7 @@
       </c>
       <c r="I219" s="31"/>
     </row>
-    <row r="220" spans="1:9" ht="45">
+    <row r="220" spans="1:9" ht="30">
       <c r="A220" s="29" t="s">
         <v>241</v>
       </c>
@@ -14147,7 +14148,7 @@
       </c>
       <c r="I220" s="31"/>
     </row>
-    <row r="221" spans="1:9" ht="45">
+    <row r="221" spans="1:9" ht="30">
       <c r="A221" s="29" t="s">
         <v>242</v>
       </c>
@@ -14272,7 +14273,7 @@
       </c>
       <c r="I225" s="31"/>
     </row>
-    <row r="226" spans="1:9" ht="90">
+    <row r="226" spans="1:9" ht="75">
       <c r="A226" s="29" t="s">
         <v>247</v>
       </c>
@@ -14372,7 +14373,7 @@
       </c>
       <c r="I229" s="31"/>
     </row>
-    <row r="230" spans="1:9" ht="45">
+    <row r="230" spans="1:9" ht="30">
       <c r="A230" s="29" t="s">
         <v>251</v>
       </c>
@@ -14399,7 +14400,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="45">
+    <row r="231" spans="1:9" ht="30">
       <c r="A231" s="29" t="s">
         <v>252</v>
       </c>
@@ -14449,7 +14450,7 @@
       </c>
       <c r="I232" s="31"/>
     </row>
-    <row r="233" spans="1:9" ht="60">
+    <row r="233" spans="1:9" ht="45">
       <c r="A233" s="29" t="s">
         <v>254</v>
       </c>
@@ -14674,7 +14675,7 @@
       </c>
       <c r="I241" s="31"/>
     </row>
-    <row r="242" spans="1:9" ht="45">
+    <row r="242" spans="1:9" ht="30">
       <c r="A242" s="29" t="s">
         <v>263</v>
       </c>
@@ -14824,7 +14825,7 @@
       </c>
       <c r="I247" s="31"/>
     </row>
-    <row r="248" spans="1:9" ht="45">
+    <row r="248" spans="1:9" ht="30">
       <c r="A248" s="29" t="s">
         <v>269</v>
       </c>
@@ -14851,7 +14852,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="45">
+    <row r="249" spans="1:9" ht="30">
       <c r="A249" s="29" t="s">
         <v>270</v>
       </c>
@@ -15001,7 +15002,7 @@
       </c>
       <c r="I254" s="31"/>
     </row>
-    <row r="255" spans="1:9" ht="60">
+    <row r="255" spans="1:9" ht="45">
       <c r="A255" s="29" t="s">
         <v>276</v>
       </c>
@@ -15028,7 +15029,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="60">
+    <row r="256" spans="1:9" ht="45">
       <c r="A256" s="29" t="s">
         <v>277</v>
       </c>
@@ -15055,7 +15056,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="60">
+    <row r="257" spans="1:9" ht="45">
       <c r="A257" s="29" t="s">
         <v>278</v>
       </c>
@@ -15082,7 +15083,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="258" spans="1:9" ht="60">
+    <row r="258" spans="1:9" ht="45">
       <c r="A258" s="29" t="s">
         <v>279</v>
       </c>
@@ -15159,7 +15160,7 @@
       </c>
       <c r="I260" s="31"/>
     </row>
-    <row r="261" spans="1:9" ht="60">
+    <row r="261" spans="1:9" ht="45">
       <c r="A261" s="29" t="s">
         <v>282</v>
       </c>
@@ -15186,7 +15187,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="60">
+    <row r="262" spans="1:9" ht="45">
       <c r="A262" s="29" t="s">
         <v>283</v>
       </c>
@@ -15213,7 +15214,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="263" spans="1:9" ht="60">
+    <row r="263" spans="1:9" ht="45">
       <c r="A263" s="29" t="s">
         <v>284</v>
       </c>
@@ -15265,7 +15266,7 @@
       </c>
       <c r="I264" s="31"/>
     </row>
-    <row r="265" spans="1:9" ht="60">
+    <row r="265" spans="1:9" ht="45">
       <c r="A265" s="29" t="s">
         <v>286</v>
       </c>
@@ -15292,7 +15293,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="60">
+    <row r="266" spans="1:9" ht="45">
       <c r="A266" s="29" t="s">
         <v>287</v>
       </c>
@@ -15319,7 +15320,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="60">
+    <row r="267" spans="1:9" ht="45">
       <c r="A267" s="29" t="s">
         <v>288</v>
       </c>
@@ -15371,7 +15372,7 @@
       </c>
       <c r="I268" s="31"/>
     </row>
-    <row r="269" spans="1:9" ht="60">
+    <row r="269" spans="1:9" ht="45">
       <c r="A269" s="29" t="s">
         <v>290</v>
       </c>
@@ -15398,7 +15399,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="45">
+    <row r="270" spans="1:9" ht="30">
       <c r="A270" s="29" t="s">
         <v>291</v>
       </c>
@@ -15448,7 +15449,7 @@
       </c>
       <c r="I271" s="31"/>
     </row>
-    <row r="272" spans="1:9" ht="60">
+    <row r="272" spans="1:9" ht="45">
       <c r="A272" s="29" t="s">
         <v>293</v>
       </c>
@@ -15523,7 +15524,7 @@
       </c>
       <c r="I274" s="31"/>
     </row>
-    <row r="275" spans="1:9" ht="45">
+    <row r="275" spans="1:9" ht="30">
       <c r="A275" s="29" t="s">
         <v>296</v>
       </c>
@@ -15598,7 +15599,7 @@
       </c>
       <c r="I277" s="31"/>
     </row>
-    <row r="278" spans="1:9" ht="45">
+    <row r="278" spans="1:9" ht="30">
       <c r="A278" s="29" t="s">
         <v>299</v>
       </c>
@@ -15623,7 +15624,7 @@
       </c>
       <c r="I278" s="31"/>
     </row>
-    <row r="279" spans="1:9" ht="45">
+    <row r="279" spans="1:9" ht="30">
       <c r="A279" s="29" t="s">
         <v>300</v>
       </c>
@@ -15723,7 +15724,7 @@
       </c>
       <c r="I282" s="31"/>
     </row>
-    <row r="283" spans="1:9" ht="45">
+    <row r="283" spans="1:9" ht="30">
       <c r="A283" s="29" t="s">
         <v>304</v>
       </c>
@@ -15848,7 +15849,7 @@
       </c>
       <c r="I287" s="31"/>
     </row>
-    <row r="288" spans="1:9" ht="45">
+    <row r="288" spans="1:9" ht="30">
       <c r="A288" s="29" t="s">
         <v>309</v>
       </c>
@@ -15873,7 +15874,7 @@
       </c>
       <c r="I288" s="31"/>
     </row>
-    <row r="289" spans="1:9" ht="45">
+    <row r="289" spans="1:9" ht="30">
       <c r="A289" s="29" t="s">
         <v>310</v>
       </c>
@@ -15898,7 +15899,7 @@
       </c>
       <c r="I289" s="31"/>
     </row>
-    <row r="290" spans="1:9" ht="45">
+    <row r="290" spans="1:9" ht="30">
       <c r="A290" s="29" t="s">
         <v>311</v>
       </c>
@@ -15923,7 +15924,7 @@
       </c>
       <c r="I290" s="31"/>
     </row>
-    <row r="291" spans="1:9" ht="45">
+    <row r="291" spans="1:9" ht="30">
       <c r="A291" s="29" t="s">
         <v>312</v>
       </c>
@@ -15998,7 +15999,7 @@
       </c>
       <c r="I293" s="31"/>
     </row>
-    <row r="294" spans="1:9" ht="45">
+    <row r="294" spans="1:9" ht="30">
       <c r="A294" s="29" t="s">
         <v>315</v>
       </c>
@@ -16048,7 +16049,7 @@
       </c>
       <c r="I295" s="31"/>
     </row>
-    <row r="296" spans="1:9" ht="60">
+    <row r="296" spans="1:9" ht="45">
       <c r="A296" s="29" t="s">
         <v>317</v>
       </c>
@@ -16148,7 +16149,7 @@
       </c>
       <c r="I299" s="31"/>
     </row>
-    <row r="300" spans="1:9" ht="45">
+    <row r="300" spans="1:9" ht="30">
       <c r="A300" s="29" t="s">
         <v>321</v>
       </c>
@@ -16198,7 +16199,7 @@
       </c>
       <c r="I301" s="31"/>
     </row>
-    <row r="302" spans="1:9" ht="45">
+    <row r="302" spans="1:9" ht="30">
       <c r="A302" s="29" t="s">
         <v>323</v>
       </c>
@@ -16323,7 +16324,7 @@
       </c>
       <c r="I306" s="31"/>
     </row>
-    <row r="307" spans="1:9" ht="45">
+    <row r="307" spans="1:9" ht="30">
       <c r="A307" s="29" t="s">
         <v>328</v>
       </c>
@@ -16348,7 +16349,7 @@
       </c>
       <c r="I307" s="31"/>
     </row>
-    <row r="308" spans="1:9" ht="45">
+    <row r="308" spans="1:9" ht="30">
       <c r="A308" s="29" t="s">
         <v>329</v>
       </c>
@@ -16573,7 +16574,7 @@
       </c>
       <c r="I316" s="31"/>
     </row>
-    <row r="317" spans="1:9" ht="45">
+    <row r="317" spans="1:9" ht="30">
       <c r="A317" s="29" t="s">
         <v>338</v>
       </c>
@@ -16673,7 +16674,7 @@
       </c>
       <c r="I320" s="31"/>
     </row>
-    <row r="321" spans="1:9" ht="45">
+    <row r="321" spans="1:9" ht="30">
       <c r="A321" s="29" t="s">
         <v>342</v>
       </c>
@@ -16823,7 +16824,7 @@
       </c>
       <c r="I326" s="31"/>
     </row>
-    <row r="327" spans="1:9" ht="45">
+    <row r="327" spans="1:9" ht="30">
       <c r="A327" s="29" t="s">
         <v>348</v>
       </c>
@@ -16873,7 +16874,7 @@
       </c>
       <c r="I328" s="31"/>
     </row>
-    <row r="329" spans="1:9" ht="30">
+    <row r="329" spans="1:9">
       <c r="A329" s="29" t="s">
         <v>350</v>
       </c>
@@ -16898,7 +16899,7 @@
       </c>
       <c r="I329" s="31"/>
     </row>
-    <row r="330" spans="1:9" ht="30">
+    <row r="330" spans="1:9">
       <c r="A330" s="29" t="s">
         <v>351</v>
       </c>
@@ -17048,7 +17049,7 @@
       </c>
       <c r="I335" s="31"/>
     </row>
-    <row r="336" spans="1:9" ht="60">
+    <row r="336" spans="1:9" ht="45">
       <c r="A336" s="29" t="s">
         <v>357</v>
       </c>
@@ -17123,7 +17124,7 @@
       </c>
       <c r="I338" s="31"/>
     </row>
-    <row r="339" spans="1:9" ht="45">
+    <row r="339" spans="1:9" ht="30">
       <c r="A339" s="29" t="s">
         <v>360</v>
       </c>
@@ -17148,7 +17149,7 @@
       </c>
       <c r="I339" s="31"/>
     </row>
-    <row r="340" spans="1:9" ht="60">
+    <row r="340" spans="1:9" ht="45">
       <c r="A340" s="29" t="s">
         <v>361</v>
       </c>
@@ -17173,7 +17174,7 @@
       </c>
       <c r="I340" s="31"/>
     </row>
-    <row r="341" spans="1:9" ht="45">
+    <row r="341" spans="1:9" ht="30">
       <c r="A341" s="29" t="s">
         <v>362</v>
       </c>
@@ -17398,7 +17399,7 @@
       </c>
       <c r="I349" s="31"/>
     </row>
-    <row r="350" spans="1:9" ht="45">
+    <row r="350" spans="1:9" ht="30">
       <c r="A350" s="29" t="s">
         <v>371</v>
       </c>
@@ -17473,7 +17474,7 @@
       </c>
       <c r="I352" s="31"/>
     </row>
-    <row r="353" spans="1:9" ht="45">
+    <row r="353" spans="1:9" ht="30">
       <c r="A353" s="29" t="s">
         <v>374</v>
       </c>
@@ -17498,7 +17499,7 @@
       </c>
       <c r="I353" s="31"/>
     </row>
-    <row r="354" spans="1:9" ht="45">
+    <row r="354" spans="1:9" ht="30">
       <c r="A354" s="29" t="s">
         <v>375</v>
       </c>
@@ -17673,7 +17674,7 @@
       </c>
       <c r="I360" s="31"/>
     </row>
-    <row r="361" spans="1:9" ht="45">
+    <row r="361" spans="1:9" ht="30">
       <c r="A361" s="29" t="s">
         <v>382</v>
       </c>
@@ -17698,7 +17699,7 @@
       </c>
       <c r="I361" s="31"/>
     </row>
-    <row r="362" spans="1:9" ht="45">
+    <row r="362" spans="1:9" ht="30">
       <c r="A362" s="29" t="s">
         <v>383</v>
       </c>
@@ -17873,7 +17874,7 @@
       </c>
       <c r="I368" s="31"/>
     </row>
-    <row r="369" spans="1:9" ht="30">
+    <row r="369" spans="1:9">
       <c r="A369" s="29" t="s">
         <v>390</v>
       </c>
@@ -18098,7 +18099,7 @@
       </c>
       <c r="I377" s="31"/>
     </row>
-    <row r="378" spans="1:9" ht="45">
+    <row r="378" spans="1:9" ht="30">
       <c r="A378" s="29" t="s">
         <v>399</v>
       </c>
@@ -18323,7 +18324,7 @@
       </c>
       <c r="I386" s="31"/>
     </row>
-    <row r="387" spans="1:9" ht="45">
+    <row r="387" spans="1:9" ht="30">
       <c r="A387" s="29" t="s">
         <v>408</v>
       </c>
@@ -18348,7 +18349,7 @@
       </c>
       <c r="I387" s="31"/>
     </row>
-    <row r="388" spans="1:9" ht="45">
+    <row r="388" spans="1:9" ht="30">
       <c r="A388" s="29" t="s">
         <v>409</v>
       </c>
@@ -18772,7 +18773,7 @@
       </c>
       <c r="I403" s="31"/>
     </row>
-    <row r="404" spans="1:9" ht="30">
+    <row r="404" spans="1:9">
       <c r="A404" s="29" t="s">
         <v>425</v>
       </c>
@@ -18847,7 +18848,7 @@
       </c>
       <c r="I406" s="31"/>
     </row>
-    <row r="407" spans="1:9" ht="30">
+    <row r="407" spans="1:9">
       <c r="A407" s="29" t="s">
         <v>428</v>
       </c>
@@ -18897,7 +18898,7 @@
       </c>
       <c r="I408" s="31"/>
     </row>
-    <row r="409" spans="1:9" ht="45">
+    <row r="409" spans="1:9" ht="30">
       <c r="A409" s="29" t="s">
         <v>430</v>
       </c>
@@ -18922,7 +18923,7 @@
       </c>
       <c r="I409" s="31"/>
     </row>
-    <row r="410" spans="1:9" ht="30">
+    <row r="410" spans="1:9">
       <c r="A410" s="29" t="s">
         <v>431</v>
       </c>
@@ -19172,7 +19173,7 @@
       </c>
       <c r="I419" s="31"/>
     </row>
-    <row r="420" spans="1:9" ht="45">
+    <row r="420" spans="1:9" ht="30">
       <c r="A420" s="29" t="s">
         <v>441</v>
       </c>
@@ -19222,7 +19223,7 @@
       </c>
       <c r="I421" s="31"/>
     </row>
-    <row r="422" spans="1:9" ht="45">
+    <row r="422" spans="1:9" ht="30">
       <c r="A422" s="29" t="s">
         <v>443</v>
       </c>
@@ -19347,7 +19348,7 @@
       </c>
       <c r="I426" s="31"/>
     </row>
-    <row r="427" spans="1:9" ht="45">
+    <row r="427" spans="1:9" ht="30">
       <c r="A427" s="29" t="s">
         <v>448</v>
       </c>
@@ -19372,7 +19373,7 @@
       </c>
       <c r="I427" s="31"/>
     </row>
-    <row r="428" spans="1:9" ht="30">
+    <row r="428" spans="1:9">
       <c r="A428" s="29" t="s">
         <v>449</v>
       </c>
@@ -19397,7 +19398,7 @@
       </c>
       <c r="I428" s="31"/>
     </row>
-    <row r="429" spans="1:9" ht="45">
+    <row r="429" spans="1:9" ht="30">
       <c r="A429" s="29" t="s">
         <v>450</v>
       </c>
@@ -19472,7 +19473,7 @@
       </c>
       <c r="I431" s="31"/>
     </row>
-    <row r="432" spans="1:9" ht="30">
+    <row r="432" spans="1:9">
       <c r="A432" s="29" t="s">
         <v>453</v>
       </c>
@@ -19522,7 +19523,7 @@
       </c>
       <c r="I433" s="31"/>
     </row>
-    <row r="434" spans="1:9" ht="30">
+    <row r="434" spans="1:9">
       <c r="A434" s="29" t="s">
         <v>455</v>
       </c>
@@ -19547,7 +19548,7 @@
       </c>
       <c r="I434" s="31"/>
     </row>
-    <row r="435" spans="1:9" ht="45">
+    <row r="435" spans="1:9" ht="30">
       <c r="A435" s="29" t="s">
         <v>456</v>
       </c>
@@ -19572,7 +19573,7 @@
       </c>
       <c r="I435" s="31"/>
     </row>
-    <row r="436" spans="1:9" ht="30">
+    <row r="436" spans="1:9">
       <c r="A436" s="29" t="s">
         <v>457</v>
       </c>
@@ -19672,7 +19673,7 @@
       </c>
       <c r="I439" s="31"/>
     </row>
-    <row r="440" spans="1:9" ht="60">
+    <row r="440" spans="1:9" ht="45">
       <c r="A440" s="29" t="s">
         <v>461</v>
       </c>
@@ -19728,7 +19729,7 @@
       </c>
       <c r="I441" s="31"/>
     </row>
-    <row r="442" spans="1:9" ht="60">
+    <row r="442" spans="1:9" ht="45">
       <c r="A442" s="29" t="s">
         <v>463</v>
       </c>
@@ -19755,7 +19756,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="443" spans="1:9" ht="60">
+    <row r="443" spans="1:9" ht="45">
       <c r="A443" s="29" t="s">
         <v>464</v>
       </c>
@@ -19780,8 +19781,8 @@
       <c r="H443" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I443" s="31" t="s">
-        <v>2314</v>
+      <c r="I443" s="20" t="s">
+        <v>2417</v>
       </c>
     </row>
     <row r="444" spans="1:9">
@@ -19967,7 +19968,7 @@
       </c>
       <c r="I450" s="31"/>
     </row>
-    <row r="451" spans="1:9" ht="45">
+    <row r="451" spans="1:9" ht="30">
       <c r="A451" s="29" t="s">
         <v>472</v>
       </c>
@@ -20017,7 +20018,7 @@
       </c>
       <c r="I452" s="31"/>
     </row>
-    <row r="453" spans="1:9" ht="30">
+    <row r="453" spans="1:9">
       <c r="A453" s="29" t="s">
         <v>474</v>
       </c>
@@ -20394,7 +20395,7 @@
       </c>
       <c r="I467" s="31"/>
     </row>
-    <row r="468" spans="1:9" ht="30">
+    <row r="468" spans="1:9">
       <c r="A468" s="29" t="s">
         <v>489</v>
       </c>
@@ -20473,7 +20474,7 @@
       </c>
       <c r="I470" s="31"/>
     </row>
-    <row r="471" spans="1:9" ht="30">
+    <row r="471" spans="1:9">
       <c r="A471" s="29" t="s">
         <v>492</v>
       </c>
@@ -20498,7 +20499,7 @@
       </c>
       <c r="I471" s="31"/>
     </row>
-    <row r="472" spans="1:9" ht="30">
+    <row r="472" spans="1:9">
       <c r="A472" s="29" t="s">
         <v>493</v>
       </c>
@@ -20548,7 +20549,7 @@
       </c>
       <c r="I473" s="31"/>
     </row>
-    <row r="474" spans="1:9" ht="60">
+    <row r="474" spans="1:9" ht="45">
       <c r="A474" s="29" t="s">
         <v>495</v>
       </c>
@@ -20623,7 +20624,7 @@
       </c>
       <c r="I476" s="31"/>
     </row>
-    <row r="477" spans="1:9" ht="45">
+    <row r="477" spans="1:9" ht="30">
       <c r="A477" s="29" t="s">
         <v>498</v>
       </c>
@@ -20648,7 +20649,7 @@
       </c>
       <c r="I477" s="31"/>
     </row>
-    <row r="478" spans="1:9" ht="60">
+    <row r="478" spans="1:9" ht="45">
       <c r="A478" s="29" t="s">
         <v>499</v>
       </c>
@@ -20698,7 +20699,7 @@
       </c>
       <c r="I479" s="31"/>
     </row>
-    <row r="480" spans="1:9" ht="45">
+    <row r="480" spans="1:9" ht="30">
       <c r="A480" s="29" t="s">
         <v>501</v>
       </c>
@@ -20723,7 +20724,7 @@
       </c>
       <c r="I480" s="31"/>
     </row>
-    <row r="481" spans="1:9" ht="45">
+    <row r="481" spans="1:9" ht="30">
       <c r="A481" s="29" t="s">
         <v>502</v>
       </c>
@@ -20748,7 +20749,7 @@
       </c>
       <c r="I481" s="31"/>
     </row>
-    <row r="482" spans="1:9" ht="45">
+    <row r="482" spans="1:9" ht="30">
       <c r="A482" s="29" t="s">
         <v>503</v>
       </c>
@@ -20848,7 +20849,7 @@
       </c>
       <c r="I485" s="31"/>
     </row>
-    <row r="486" spans="1:9" ht="30">
+    <row r="486" spans="1:9">
       <c r="A486" s="29" t="s">
         <v>507</v>
       </c>
@@ -20973,7 +20974,7 @@
       </c>
       <c r="I490" s="31"/>
     </row>
-    <row r="491" spans="1:9" ht="45">
+    <row r="491" spans="1:9" ht="30">
       <c r="A491" s="29" t="s">
         <v>512</v>
       </c>
@@ -21148,7 +21149,7 @@
       </c>
       <c r="I497" s="31"/>
     </row>
-    <row r="498" spans="1:9" ht="45">
+    <row r="498" spans="1:9" ht="30">
       <c r="A498" s="29" t="s">
         <v>519</v>
       </c>
@@ -21223,7 +21224,7 @@
       </c>
       <c r="I500" s="31"/>
     </row>
-    <row r="501" spans="1:9" ht="60">
+    <row r="501" spans="1:9" ht="45">
       <c r="A501" s="29" t="s">
         <v>522</v>
       </c>
@@ -21248,7 +21249,7 @@
       </c>
       <c r="I501" s="31"/>
     </row>
-    <row r="502" spans="1:9" ht="45">
+    <row r="502" spans="1:9" ht="30">
       <c r="A502" s="29" t="s">
         <v>523</v>
       </c>
@@ -21273,7 +21274,7 @@
       </c>
       <c r="I502" s="31"/>
     </row>
-    <row r="503" spans="1:9" ht="45">
+    <row r="503" spans="1:9" ht="30">
       <c r="A503" s="29" t="s">
         <v>524</v>
       </c>
@@ -21298,7 +21299,7 @@
       </c>
       <c r="I503" s="31"/>
     </row>
-    <row r="504" spans="1:9" ht="90">
+    <row r="504" spans="1:9" ht="75">
       <c r="A504" s="29" t="s">
         <v>525</v>
       </c>
@@ -21348,7 +21349,7 @@
       </c>
       <c r="I505" s="31"/>
     </row>
-    <row r="506" spans="1:9" ht="45">
+    <row r="506" spans="1:9" ht="30">
       <c r="A506" s="29" t="s">
         <v>527</v>
       </c>
@@ -21373,7 +21374,7 @@
       </c>
       <c r="I506" s="31"/>
     </row>
-    <row r="507" spans="1:9" ht="75">
+    <row r="507" spans="1:9" ht="60">
       <c r="A507" s="29" t="s">
         <v>528</v>
       </c>
@@ -21398,7 +21399,7 @@
       </c>
       <c r="I507" s="31"/>
     </row>
-    <row r="508" spans="1:9" ht="60">
+    <row r="508" spans="1:9" ht="45">
       <c r="A508" s="29" t="s">
         <v>529</v>
       </c>
@@ -21448,7 +21449,7 @@
       </c>
       <c r="I509" s="31"/>
     </row>
-    <row r="510" spans="1:9" ht="45">
+    <row r="510" spans="1:9" ht="30">
       <c r="A510" s="29" t="s">
         <v>531</v>
       </c>
@@ -21523,7 +21524,7 @@
       </c>
       <c r="I512" s="31"/>
     </row>
-    <row r="513" spans="1:9" ht="60">
+    <row r="513" spans="1:9" ht="45">
       <c r="A513" s="29" t="s">
         <v>534</v>
       </c>
@@ -21548,7 +21549,7 @@
       </c>
       <c r="I513" s="31"/>
     </row>
-    <row r="514" spans="1:9" ht="30">
+    <row r="514" spans="1:9">
       <c r="A514" s="29" t="s">
         <v>535</v>
       </c>
@@ -21623,7 +21624,7 @@
       </c>
       <c r="I516" s="31"/>
     </row>
-    <row r="517" spans="1:9" ht="75">
+    <row r="517" spans="1:9" ht="60">
       <c r="A517" s="29" t="s">
         <v>538</v>
       </c>
@@ -21648,7 +21649,7 @@
       </c>
       <c r="I517" s="31"/>
     </row>
-    <row r="518" spans="1:9" ht="60">
+    <row r="518" spans="1:9" ht="45">
       <c r="A518" s="29" t="s">
         <v>539</v>
       </c>
@@ -21698,7 +21699,7 @@
       </c>
       <c r="I519" s="31"/>
     </row>
-    <row r="520" spans="1:9" ht="60">
+    <row r="520" spans="1:9" ht="45">
       <c r="A520" s="29" t="s">
         <v>541</v>
       </c>
@@ -21798,7 +21799,7 @@
       </c>
       <c r="I523" s="31"/>
     </row>
-    <row r="524" spans="1:9" ht="45">
+    <row r="524" spans="1:9" ht="30">
       <c r="A524" s="29" t="s">
         <v>545</v>
       </c>
@@ -21873,7 +21874,7 @@
       </c>
       <c r="I526" s="31"/>
     </row>
-    <row r="527" spans="1:9" ht="45">
+    <row r="527" spans="1:9" ht="30">
       <c r="A527" s="29" t="s">
         <v>548</v>
       </c>
@@ -22123,7 +22124,7 @@
       </c>
       <c r="I536" s="31"/>
     </row>
-    <row r="537" spans="1:9" ht="45">
+    <row r="537" spans="1:9" ht="30">
       <c r="A537" s="29" t="s">
         <v>558</v>
       </c>
@@ -22148,7 +22149,7 @@
       </c>
       <c r="I537" s="31"/>
     </row>
-    <row r="538" spans="1:9" ht="60">
+    <row r="538" spans="1:9" ht="45">
       <c r="A538" s="29" t="s">
         <v>559</v>
       </c>
@@ -22173,7 +22174,7 @@
       </c>
       <c r="I538" s="31"/>
     </row>
-    <row r="539" spans="1:9" ht="45">
+    <row r="539" spans="1:9" ht="30">
       <c r="A539" s="29" t="s">
         <v>560</v>
       </c>
@@ -22198,7 +22199,7 @@
       </c>
       <c r="I539" s="31"/>
     </row>
-    <row r="540" spans="1:9" ht="60">
+    <row r="540" spans="1:9" ht="45">
       <c r="A540" s="29" t="s">
         <v>561</v>
       </c>
@@ -22223,7 +22224,7 @@
       </c>
       <c r="I540" s="31"/>
     </row>
-    <row r="541" spans="1:9" ht="60">
+    <row r="541" spans="1:9" ht="45">
       <c r="A541" s="29" t="s">
         <v>562</v>
       </c>
@@ -22323,7 +22324,7 @@
       </c>
       <c r="I544" s="31"/>
     </row>
-    <row r="545" spans="1:9" ht="45">
+    <row r="545" spans="1:9" ht="30">
       <c r="A545" s="29" t="s">
         <v>566</v>
       </c>
@@ -22348,7 +22349,7 @@
       </c>
       <c r="I545" s="31"/>
     </row>
-    <row r="546" spans="1:9" ht="45">
+    <row r="546" spans="1:9" ht="30">
       <c r="A546" s="29" t="s">
         <v>567</v>
       </c>
@@ -22373,7 +22374,7 @@
       </c>
       <c r="I546" s="31"/>
     </row>
-    <row r="547" spans="1:9" ht="45">
+    <row r="547" spans="1:9" ht="30">
       <c r="A547" s="29" t="s">
         <v>568</v>
       </c>
@@ -22423,7 +22424,7 @@
       </c>
       <c r="I548" s="31"/>
     </row>
-    <row r="549" spans="1:9" ht="45">
+    <row r="549" spans="1:9" ht="30">
       <c r="A549" s="29" t="s">
         <v>570</v>
       </c>
@@ -22523,7 +22524,7 @@
       </c>
       <c r="I552" s="31"/>
     </row>
-    <row r="553" spans="1:9" ht="45">
+    <row r="553" spans="1:9" ht="30">
       <c r="A553" s="29" t="s">
         <v>574</v>
       </c>
@@ -22573,7 +22574,7 @@
       </c>
       <c r="I554" s="31"/>
     </row>
-    <row r="555" spans="1:9" ht="45">
+    <row r="555" spans="1:9" ht="30">
       <c r="A555" s="29" t="s">
         <v>576</v>
       </c>
@@ -22598,7 +22599,7 @@
       </c>
       <c r="I555" s="31"/>
     </row>
-    <row r="556" spans="1:9" ht="45">
+    <row r="556" spans="1:9" ht="30">
       <c r="A556" s="29" t="s">
         <v>577</v>
       </c>
@@ -22673,7 +22674,7 @@
       </c>
       <c r="I558" s="31"/>
     </row>
-    <row r="559" spans="1:9" ht="60">
+    <row r="559" spans="1:9" ht="45">
       <c r="A559" s="29" t="s">
         <v>580</v>
       </c>
@@ -22723,7 +22724,7 @@
       </c>
       <c r="I560" s="31"/>
     </row>
-    <row r="561" spans="1:9" ht="75">
+    <row r="561" spans="1:9" ht="60">
       <c r="A561" s="29" t="s">
         <v>582</v>
       </c>
@@ -22748,7 +22749,7 @@
       </c>
       <c r="I561" s="31"/>
     </row>
-    <row r="562" spans="1:9" ht="30">
+    <row r="562" spans="1:9">
       <c r="A562" s="29" t="s">
         <v>583</v>
       </c>
@@ -22773,7 +22774,7 @@
       </c>
       <c r="I562" s="31"/>
     </row>
-    <row r="563" spans="1:9" ht="30">
+    <row r="563" spans="1:9">
       <c r="A563" s="29" t="s">
         <v>584</v>
       </c>
@@ -22848,7 +22849,7 @@
       </c>
       <c r="I565" s="31"/>
     </row>
-    <row r="566" spans="1:9" ht="30">
+    <row r="566" spans="1:9">
       <c r="A566" s="29" t="s">
         <v>587</v>
       </c>
@@ -22973,7 +22974,7 @@
       </c>
       <c r="I570" s="31"/>
     </row>
-    <row r="571" spans="1:9" ht="30">
+    <row r="571" spans="1:9">
       <c r="A571" s="29" t="s">
         <v>592</v>
       </c>
@@ -23048,7 +23049,7 @@
       </c>
       <c r="I573" s="31"/>
     </row>
-    <row r="574" spans="1:9" ht="75">
+    <row r="574" spans="1:9" ht="60">
       <c r="A574" s="29" t="s">
         <v>595</v>
       </c>
@@ -23148,7 +23149,7 @@
       </c>
       <c r="I577" s="31"/>
     </row>
-    <row r="578" spans="1:9" ht="30">
+    <row r="578" spans="1:9">
       <c r="A578" s="29" t="s">
         <v>599</v>
       </c>
@@ -23198,7 +23199,7 @@
       </c>
       <c r="I579" s="31"/>
     </row>
-    <row r="580" spans="1:9" ht="45">
+    <row r="580" spans="1:9" ht="30">
       <c r="A580" s="29" t="s">
         <v>601</v>
       </c>
@@ -23223,7 +23224,7 @@
       </c>
       <c r="I580" s="31"/>
     </row>
-    <row r="581" spans="1:9" ht="45">
+    <row r="581" spans="1:9" ht="30">
       <c r="A581" s="29" t="s">
         <v>602</v>
       </c>
@@ -23273,7 +23274,7 @@
       </c>
       <c r="I582" s="31"/>
     </row>
-    <row r="583" spans="1:9" ht="45">
+    <row r="583" spans="1:9" ht="30">
       <c r="A583" s="29" t="s">
         <v>604</v>
       </c>
@@ -23348,7 +23349,7 @@
       </c>
       <c r="I585" s="31"/>
     </row>
-    <row r="586" spans="1:9" ht="60">
+    <row r="586" spans="1:9" ht="45">
       <c r="A586" s="29" t="s">
         <v>607</v>
       </c>
@@ -23373,7 +23374,7 @@
       </c>
       <c r="I586" s="31"/>
     </row>
-    <row r="587" spans="1:9" ht="45">
+    <row r="587" spans="1:9" ht="30">
       <c r="A587" s="29" t="s">
         <v>608</v>
       </c>
@@ -23431,7 +23432,7 @@
         <v>1194</v>
       </c>
       <c r="C589" s="31" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="D589" s="29"/>
       <c r="E589" s="29" t="s">
@@ -23598,7 +23599,7 @@
       </c>
       <c r="I595" s="31"/>
     </row>
-    <row r="596" spans="1:9" ht="60">
+    <row r="596" spans="1:9" ht="45">
       <c r="A596" s="22" t="s">
         <v>617</v>
       </c>
@@ -23622,10 +23623,10 @@
         <v>17</v>
       </c>
       <c r="I596" s="20" t="s">
-        <v>2416</v>
-      </c>
-    </row>
-    <row r="597" spans="1:9" ht="45">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="597" spans="1:9" ht="30">
       <c r="A597" s="29" t="s">
         <v>618</v>
       </c>
@@ -23650,7 +23651,7 @@
       </c>
       <c r="I597" s="31"/>
     </row>
-    <row r="598" spans="1:9" ht="60">
+    <row r="598" spans="1:9" ht="45">
       <c r="A598" s="22" t="s">
         <v>619</v>
       </c>
@@ -23674,7 +23675,7 @@
         <v>17</v>
       </c>
       <c r="I598" s="20" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="599" spans="1:9" ht="45">
@@ -23729,9 +23730,9 @@
       </c>
       <c r="I600" s="31"/>
     </row>
-    <row r="601" spans="1:9" ht="60">
+    <row r="601" spans="1:9" ht="45">
       <c r="A601" s="22" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="B601" s="30" t="s">
         <v>1196</v>
@@ -23779,7 +23780,7 @@
       </c>
       <c r="I602" s="31"/>
     </row>
-    <row r="603" spans="1:9" ht="60">
+    <row r="603" spans="1:9" ht="45">
       <c r="A603" s="22" t="s">
         <v>623</v>
       </c>
@@ -23803,7 +23804,7 @@
         <v>17</v>
       </c>
       <c r="I603" s="20" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="604" spans="1:9" ht="45">
@@ -23908,7 +23909,7 @@
       </c>
       <c r="I607" s="31"/>
     </row>
-    <row r="608" spans="1:9" ht="75">
+    <row r="608" spans="1:9" ht="60">
       <c r="A608" s="22" t="s">
         <v>628</v>
       </c>
@@ -23932,10 +23933,10 @@
         <v>17</v>
       </c>
       <c r="I608" s="31" t="s">
-        <v>2350</v>
-      </c>
-    </row>
-    <row r="609" spans="1:9" ht="75">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="609" spans="1:9" ht="60">
       <c r="A609" s="29" t="s">
         <v>629</v>
       </c>
@@ -23960,7 +23961,7 @@
       </c>
       <c r="I609" s="31"/>
     </row>
-    <row r="610" spans="1:9" ht="75">
+    <row r="610" spans="1:9" ht="60">
       <c r="A610" s="29" t="s">
         <v>630</v>
       </c>
@@ -24012,7 +24013,7 @@
       </c>
       <c r="I611" s="31"/>
     </row>
-    <row r="612" spans="1:9" ht="75">
+    <row r="612" spans="1:9" ht="60">
       <c r="A612" s="29" t="s">
         <v>632</v>
       </c>
@@ -24036,7 +24037,7 @@
         <v>17</v>
       </c>
       <c r="I612" s="31" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="613" spans="1:9" ht="45">
@@ -24164,7 +24165,7 @@
       </c>
       <c r="I617" s="31"/>
     </row>
-    <row r="618" spans="1:9" ht="45">
+    <row r="618" spans="1:9" ht="30">
       <c r="A618" s="29" t="s">
         <v>638</v>
       </c>
@@ -24289,7 +24290,7 @@
       </c>
       <c r="I622" s="31"/>
     </row>
-    <row r="623" spans="1:9" ht="30">
+    <row r="623" spans="1:9">
       <c r="A623" s="29" t="s">
         <v>643</v>
       </c>
@@ -24441,7 +24442,7 @@
       </c>
       <c r="I628" s="31"/>
     </row>
-    <row r="629" spans="1:9" ht="45">
+    <row r="629" spans="1:9" ht="30">
       <c r="A629" s="29" t="s">
         <v>649</v>
       </c>
@@ -24566,7 +24567,7 @@
       </c>
       <c r="I633" s="31"/>
     </row>
-    <row r="634" spans="1:9" ht="45">
+    <row r="634" spans="1:9" ht="30">
       <c r="A634" s="29" t="s">
         <v>654</v>
       </c>
@@ -24745,7 +24746,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="641" spans="1:9" ht="45">
+    <row r="641" spans="1:9" ht="30">
       <c r="A641" s="29" t="s">
         <v>661</v>
       </c>
@@ -24772,7 +24773,7 @@
       </c>
       <c r="I641" s="31"/>
     </row>
-    <row r="642" spans="1:9" ht="60">
+    <row r="642" spans="1:9" ht="45">
       <c r="A642" s="29" t="s">
         <v>662</v>
       </c>
@@ -24797,7 +24798,7 @@
       </c>
       <c r="I642" s="31"/>
     </row>
-    <row r="643" spans="1:9" ht="60">
+    <row r="643" spans="1:9" ht="45">
       <c r="A643" s="29" t="s">
         <v>663</v>
       </c>
@@ -24822,7 +24823,7 @@
       </c>
       <c r="I643" s="31"/>
     </row>
-    <row r="644" spans="1:9" ht="60">
+    <row r="644" spans="1:9" ht="45">
       <c r="A644" s="29" t="s">
         <v>664</v>
       </c>
@@ -24847,7 +24848,7 @@
       </c>
       <c r="I644" s="31"/>
     </row>
-    <row r="645" spans="1:9" ht="60">
+    <row r="645" spans="1:9" ht="45">
       <c r="A645" s="29" t="s">
         <v>665</v>
       </c>
@@ -24897,7 +24898,7 @@
       </c>
       <c r="I646" s="31"/>
     </row>
-    <row r="647" spans="1:9" ht="45">
+    <row r="647" spans="1:9" ht="30">
       <c r="A647" s="29" t="s">
         <v>667</v>
       </c>
@@ -25072,7 +25073,7 @@
       </c>
       <c r="I653" s="31"/>
     </row>
-    <row r="654" spans="1:9" ht="30">
+    <row r="654" spans="1:9">
       <c r="A654" s="29" t="s">
         <v>674</v>
       </c>
@@ -25122,7 +25123,7 @@
       </c>
       <c r="I655" s="31"/>
     </row>
-    <row r="656" spans="1:9" ht="30">
+    <row r="656" spans="1:9">
       <c r="A656" s="29" t="s">
         <v>676</v>
       </c>
@@ -25147,7 +25148,7 @@
       </c>
       <c r="I656" s="31"/>
     </row>
-    <row r="657" spans="1:9" ht="45">
+    <row r="657" spans="1:9" ht="30">
       <c r="A657" s="29" t="s">
         <v>677</v>
       </c>
@@ -25174,7 +25175,7 @@
         <v>2221</v>
       </c>
     </row>
-    <row r="658" spans="1:9" ht="30">
+    <row r="658" spans="1:9">
       <c r="A658" s="29" t="s">
         <v>678</v>
       </c>
@@ -25224,7 +25225,7 @@
       </c>
       <c r="I659" s="31"/>
     </row>
-    <row r="660" spans="1:9" ht="30">
+    <row r="660" spans="1:9">
       <c r="A660" s="29" t="s">
         <v>680</v>
       </c>
@@ -25274,7 +25275,7 @@
       </c>
       <c r="I661" s="31"/>
     </row>
-    <row r="662" spans="1:9" ht="30">
+    <row r="662" spans="1:9">
       <c r="A662" s="29" t="s">
         <v>682</v>
       </c>
@@ -25324,7 +25325,7 @@
       </c>
       <c r="I663" s="31"/>
     </row>
-    <row r="664" spans="1:9" ht="30">
+    <row r="664" spans="1:9">
       <c r="A664" s="29" t="s">
         <v>684</v>
       </c>
@@ -25349,7 +25350,7 @@
       </c>
       <c r="I664" s="31"/>
     </row>
-    <row r="665" spans="1:9" ht="30">
+    <row r="665" spans="1:9">
       <c r="A665" s="29" t="s">
         <v>685</v>
       </c>
@@ -25424,7 +25425,7 @@
       </c>
       <c r="I667" s="31"/>
     </row>
-    <row r="668" spans="1:9" ht="30">
+    <row r="668" spans="1:9">
       <c r="A668" s="29" t="s">
         <v>688</v>
       </c>
@@ -25449,7 +25450,7 @@
       </c>
       <c r="I668" s="31"/>
     </row>
-    <row r="669" spans="1:9" ht="45">
+    <row r="669" spans="1:9" ht="30">
       <c r="A669" s="29" t="s">
         <v>689</v>
       </c>
@@ -25474,7 +25475,7 @@
       </c>
       <c r="I669" s="31"/>
     </row>
-    <row r="670" spans="1:9" ht="30">
+    <row r="670" spans="1:9">
       <c r="A670" s="29" t="s">
         <v>690</v>
       </c>
@@ -25524,7 +25525,7 @@
       </c>
       <c r="I671" s="31"/>
     </row>
-    <row r="672" spans="1:9" ht="30">
+    <row r="672" spans="1:9">
       <c r="A672" s="29" t="s">
         <v>692</v>
       </c>
@@ -25574,7 +25575,7 @@
       </c>
       <c r="I673" s="31"/>
     </row>
-    <row r="674" spans="1:9" ht="30">
+    <row r="674" spans="1:9">
       <c r="A674" s="29" t="s">
         <v>694</v>
       </c>
@@ -25599,7 +25600,7 @@
       </c>
       <c r="I674" s="31"/>
     </row>
-    <row r="675" spans="1:9" ht="45">
+    <row r="675" spans="1:9" ht="30">
       <c r="A675" s="29" t="s">
         <v>695</v>
       </c>
@@ -25649,7 +25650,7 @@
       </c>
       <c r="I676" s="31"/>
     </row>
-    <row r="677" spans="1:9" ht="45">
+    <row r="677" spans="1:9" ht="30">
       <c r="A677" s="29" t="s">
         <v>697</v>
       </c>
@@ -25774,7 +25775,7 @@
       </c>
       <c r="I681" s="31"/>
     </row>
-    <row r="682" spans="1:9" ht="45">
+    <row r="682" spans="1:9" ht="30">
       <c r="A682" s="29" t="s">
         <v>702</v>
       </c>
@@ -25874,7 +25875,7 @@
       </c>
       <c r="I685" s="31"/>
     </row>
-    <row r="686" spans="1:9" ht="45">
+    <row r="686" spans="1:9" ht="30">
       <c r="A686" s="29" t="s">
         <v>706</v>
       </c>
@@ -25924,7 +25925,7 @@
       </c>
       <c r="I687" s="31"/>
     </row>
-    <row r="688" spans="1:9" ht="90">
+    <row r="688" spans="1:9" ht="75">
       <c r="A688" s="29" t="s">
         <v>708</v>
       </c>
@@ -25974,7 +25975,7 @@
       </c>
       <c r="I689" s="31"/>
     </row>
-    <row r="690" spans="1:9" ht="45">
+    <row r="690" spans="1:9" ht="30">
       <c r="A690" s="29" t="s">
         <v>710</v>
       </c>
@@ -26049,7 +26050,7 @@
       </c>
       <c r="I692" s="31"/>
     </row>
-    <row r="693" spans="1:9" ht="45">
+    <row r="693" spans="1:9" ht="30">
       <c r="A693" s="29" t="s">
         <v>713</v>
       </c>
@@ -26074,7 +26075,7 @@
       </c>
       <c r="I693" s="31"/>
     </row>
-    <row r="694" spans="1:9" ht="45">
+    <row r="694" spans="1:9" ht="30">
       <c r="A694" s="29" t="s">
         <v>714</v>
       </c>
@@ -26174,7 +26175,7 @@
       </c>
       <c r="I697" s="31"/>
     </row>
-    <row r="698" spans="1:9" ht="30">
+    <row r="698" spans="1:9">
       <c r="A698" s="29" t="s">
         <v>718</v>
       </c>
@@ -26199,7 +26200,7 @@
       </c>
       <c r="I698" s="31"/>
     </row>
-    <row r="699" spans="1:9" ht="30">
+    <row r="699" spans="1:9">
       <c r="A699" s="29" t="s">
         <v>719</v>
       </c>
@@ -26224,7 +26225,7 @@
       </c>
       <c r="I699" s="31"/>
     </row>
-    <row r="700" spans="1:9" ht="30">
+    <row r="700" spans="1:9">
       <c r="A700" s="29" t="s">
         <v>720</v>
       </c>
@@ -26249,7 +26250,7 @@
       </c>
       <c r="I700" s="31"/>
     </row>
-    <row r="701" spans="1:9" ht="45">
+    <row r="701" spans="1:9" ht="30">
       <c r="A701" s="29" t="s">
         <v>721</v>
       </c>
@@ -26349,7 +26350,7 @@
       </c>
       <c r="I704" s="31"/>
     </row>
-    <row r="705" spans="1:9" ht="45">
+    <row r="705" spans="1:9" ht="30">
       <c r="A705" s="29" t="s">
         <v>725</v>
       </c>
@@ -26424,7 +26425,7 @@
       </c>
       <c r="I707" s="31"/>
     </row>
-    <row r="708" spans="1:9" ht="45">
+    <row r="708" spans="1:9" ht="30">
       <c r="A708" s="29" t="s">
         <v>728</v>
       </c>
@@ -26474,7 +26475,7 @@
       </c>
       <c r="I709" s="31"/>
     </row>
-    <row r="710" spans="1:9" ht="45">
+    <row r="710" spans="1:9" ht="30">
       <c r="A710" s="29" t="s">
         <v>730</v>
       </c>
@@ -26524,7 +26525,7 @@
       </c>
       <c r="I711" s="31"/>
     </row>
-    <row r="712" spans="1:9" ht="45">
+    <row r="712" spans="1:9" ht="30">
       <c r="A712" s="29" t="s">
         <v>732</v>
       </c>
@@ -26599,7 +26600,7 @@
       </c>
       <c r="I714" s="31"/>
     </row>
-    <row r="715" spans="1:9" ht="45">
+    <row r="715" spans="1:9" ht="30">
       <c r="A715" s="29" t="s">
         <v>735</v>
       </c>
@@ -26749,7 +26750,7 @@
       </c>
       <c r="I720" s="31"/>
     </row>
-    <row r="721" spans="1:9" ht="60">
+    <row r="721" spans="1:9" ht="45">
       <c r="A721" s="29" t="s">
         <v>741</v>
       </c>
@@ -26874,7 +26875,7 @@
       </c>
       <c r="I725" s="31"/>
     </row>
-    <row r="726" spans="1:9" ht="30">
+    <row r="726" spans="1:9">
       <c r="A726" s="29" t="s">
         <v>746</v>
       </c>
@@ -26899,7 +26900,7 @@
       </c>
       <c r="I726" s="31"/>
     </row>
-    <row r="727" spans="1:9" ht="30">
+    <row r="727" spans="1:9">
       <c r="A727" s="29" t="s">
         <v>747</v>
       </c>
@@ -26924,7 +26925,7 @@
       </c>
       <c r="I727" s="31"/>
     </row>
-    <row r="728" spans="1:9" ht="30">
+    <row r="728" spans="1:9">
       <c r="A728" s="29" t="s">
         <v>748</v>
       </c>
@@ -26949,7 +26950,7 @@
       </c>
       <c r="I728" s="31"/>
     </row>
-    <row r="729" spans="1:9" ht="45">
+    <row r="729" spans="1:9" ht="30">
       <c r="A729" s="29" t="s">
         <v>749</v>
       </c>
@@ -26974,7 +26975,7 @@
       </c>
       <c r="I729" s="31"/>
     </row>
-    <row r="730" spans="1:9" ht="30">
+    <row r="730" spans="1:9">
       <c r="A730" s="29" t="s">
         <v>750</v>
       </c>
@@ -26999,7 +27000,7 @@
       </c>
       <c r="I730" s="31"/>
     </row>
-    <row r="731" spans="1:9" ht="45">
+    <row r="731" spans="1:9" ht="30">
       <c r="A731" s="29" t="s">
         <v>751</v>
       </c>
@@ -27024,7 +27025,7 @@
       </c>
       <c r="I731" s="31"/>
     </row>
-    <row r="732" spans="1:9" ht="30">
+    <row r="732" spans="1:9">
       <c r="A732" s="29" t="s">
         <v>752</v>
       </c>
@@ -27074,7 +27075,7 @@
       </c>
       <c r="I733" s="31"/>
     </row>
-    <row r="734" spans="1:9" ht="30">
+    <row r="734" spans="1:9">
       <c r="A734" s="29" t="s">
         <v>754</v>
       </c>
@@ -27124,7 +27125,7 @@
       </c>
       <c r="I735" s="31"/>
     </row>
-    <row r="736" spans="1:9" ht="45">
+    <row r="736" spans="1:9" ht="30">
       <c r="A736" s="29" t="s">
         <v>756</v>
       </c>
@@ -27149,7 +27150,7 @@
       </c>
       <c r="I736" s="31"/>
     </row>
-    <row r="737" spans="1:9" ht="45">
+    <row r="737" spans="1:9" ht="30">
       <c r="A737" s="29" t="s">
         <v>757</v>
       </c>
@@ -27199,7 +27200,7 @@
       </c>
       <c r="I738" s="31"/>
     </row>
-    <row r="739" spans="1:9" ht="45">
+    <row r="739" spans="1:9" ht="30">
       <c r="A739" s="29" t="s">
         <v>759</v>
       </c>
@@ -27224,7 +27225,7 @@
       </c>
       <c r="I739" s="31"/>
     </row>
-    <row r="740" spans="1:9" ht="60">
+    <row r="740" spans="1:9" ht="45">
       <c r="A740" s="29" t="s">
         <v>760</v>
       </c>
@@ -27249,7 +27250,7 @@
       </c>
       <c r="I740" s="31"/>
     </row>
-    <row r="741" spans="1:9" ht="45">
+    <row r="741" spans="1:9" ht="30">
       <c r="A741" s="29" t="s">
         <v>761</v>
       </c>
@@ -27299,7 +27300,7 @@
       </c>
       <c r="I742" s="31"/>
     </row>
-    <row r="743" spans="1:9" ht="45">
+    <row r="743" spans="1:9" ht="30">
       <c r="A743" s="29" t="s">
         <v>763</v>
       </c>
@@ -27399,7 +27400,7 @@
       </c>
       <c r="I746" s="31"/>
     </row>
-    <row r="747" spans="1:9" ht="30">
+    <row r="747" spans="1:9">
       <c r="A747" s="29" t="s">
         <v>767</v>
       </c>
@@ -27576,7 +27577,7 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="754" spans="1:9" ht="45">
+    <row r="754" spans="1:9" ht="30">
       <c r="A754" s="29" t="s">
         <v>774</v>
       </c>
@@ -27655,7 +27656,7 @@
       </c>
       <c r="I756" s="31"/>
     </row>
-    <row r="757" spans="1:9" ht="45">
+    <row r="757" spans="1:9" ht="30">
       <c r="A757" s="29" t="s">
         <v>777</v>
       </c>
@@ -27680,7 +27681,7 @@
       </c>
       <c r="I757" s="31"/>
     </row>
-    <row r="758" spans="1:9" ht="45">
+    <row r="758" spans="1:9" ht="30">
       <c r="A758" s="22" t="s">
         <v>778</v>
       </c>
@@ -27705,7 +27706,7 @@
       </c>
       <c r="I758" s="31"/>
     </row>
-    <row r="759" spans="1:9" ht="45">
+    <row r="759" spans="1:9" ht="30">
       <c r="A759" s="29" t="s">
         <v>779</v>
       </c>
@@ -27805,7 +27806,7 @@
       </c>
       <c r="I762" s="31"/>
     </row>
-    <row r="763" spans="1:9" ht="30">
+    <row r="763" spans="1:9">
       <c r="A763" s="29" t="s">
         <v>783</v>
       </c>
@@ -27830,7 +27831,7 @@
       </c>
       <c r="I763" s="31"/>
     </row>
-    <row r="764" spans="1:9" ht="30">
+    <row r="764" spans="1:9">
       <c r="A764" s="29" t="s">
         <v>784</v>
       </c>
@@ -27855,7 +27856,7 @@
       </c>
       <c r="I764" s="31"/>
     </row>
-    <row r="765" spans="1:9" ht="30">
+    <row r="765" spans="1:9">
       <c r="A765" s="29" t="s">
         <v>785</v>
       </c>
@@ -27905,7 +27906,7 @@
       </c>
       <c r="I766" s="31"/>
     </row>
-    <row r="767" spans="1:9" ht="30">
+    <row r="767" spans="1:9">
       <c r="A767" s="29" t="s">
         <v>787</v>
       </c>
@@ -27955,7 +27956,7 @@
       </c>
       <c r="I768" s="31"/>
     </row>
-    <row r="769" spans="1:9" ht="45">
+    <row r="769" spans="1:9" ht="30">
       <c r="A769" s="29" t="s">
         <v>789</v>
       </c>
@@ -28005,7 +28006,7 @@
       </c>
       <c r="I770" s="31"/>
     </row>
-    <row r="771" spans="1:9" ht="45">
+    <row r="771" spans="1:9" ht="30">
       <c r="A771" s="29" t="s">
         <v>791</v>
       </c>
@@ -28155,7 +28156,7 @@
       </c>
       <c r="I776" s="31"/>
     </row>
-    <row r="777" spans="1:9" ht="75">
+    <row r="777" spans="1:9" ht="60">
       <c r="A777" s="29" t="s">
         <v>797</v>
       </c>
@@ -28205,7 +28206,7 @@
       </c>
       <c r="I778" s="31"/>
     </row>
-    <row r="779" spans="1:9" ht="60">
+    <row r="779" spans="1:9" ht="45">
       <c r="A779" s="29" t="s">
         <v>799</v>
       </c>
@@ -28380,7 +28381,7 @@
       </c>
       <c r="I785" s="31"/>
     </row>
-    <row r="786" spans="1:9" ht="45">
+    <row r="786" spans="1:9" ht="30">
       <c r="A786" s="29" t="s">
         <v>806</v>
       </c>
@@ -28455,7 +28456,7 @@
       </c>
       <c r="I788" s="31"/>
     </row>
-    <row r="789" spans="1:9" ht="30">
+    <row r="789" spans="1:9">
       <c r="A789" s="29" t="s">
         <v>809</v>
       </c>
@@ -28505,7 +28506,7 @@
       </c>
       <c r="I790" s="31"/>
     </row>
-    <row r="791" spans="1:9" ht="45">
+    <row r="791" spans="1:9" ht="30">
       <c r="A791" s="29" t="s">
         <v>811</v>
       </c>
@@ -28680,7 +28681,7 @@
       </c>
       <c r="I797" s="31"/>
     </row>
-    <row r="798" spans="1:9" ht="30">
+    <row r="798" spans="1:9">
       <c r="A798" s="29" t="s">
         <v>818</v>
       </c>
@@ -28755,7 +28756,7 @@
       </c>
       <c r="I800" s="31"/>
     </row>
-    <row r="801" spans="1:9" ht="60">
+    <row r="801" spans="1:9" ht="45">
       <c r="A801" s="29" t="s">
         <v>821</v>
       </c>
@@ -28780,7 +28781,7 @@
       </c>
       <c r="I801" s="31"/>
     </row>
-    <row r="802" spans="1:9" ht="30">
+    <row r="802" spans="1:9">
       <c r="A802" s="29" t="s">
         <v>822</v>
       </c>
@@ -28830,7 +28831,7 @@
       </c>
       <c r="I803" s="31"/>
     </row>
-    <row r="804" spans="1:9" ht="45">
+    <row r="804" spans="1:9" ht="30">
       <c r="A804" s="29" t="s">
         <v>824</v>
       </c>
@@ -28880,7 +28881,7 @@
       </c>
       <c r="I805" s="31"/>
     </row>
-    <row r="806" spans="1:9" ht="60">
+    <row r="806" spans="1:9" ht="45">
       <c r="A806" s="29" t="s">
         <v>826</v>
       </c>
@@ -28905,7 +28906,7 @@
       </c>
       <c r="I806" s="31"/>
     </row>
-    <row r="807" spans="1:9" ht="45">
+    <row r="807" spans="1:9" ht="30">
       <c r="A807" s="29" t="s">
         <v>827</v>
       </c>
@@ -28930,7 +28931,7 @@
       </c>
       <c r="I807" s="31"/>
     </row>
-    <row r="808" spans="1:9" ht="45">
+    <row r="808" spans="1:9" ht="30">
       <c r="A808" s="29" t="s">
         <v>828</v>
       </c>
@@ -29055,7 +29056,7 @@
       </c>
       <c r="I812" s="31"/>
     </row>
-    <row r="813" spans="1:9" ht="75">
+    <row r="813" spans="1:9" ht="60">
       <c r="A813" s="29" t="s">
         <v>833</v>
       </c>
@@ -29105,7 +29106,7 @@
       </c>
       <c r="I814" s="31"/>
     </row>
-    <row r="815" spans="1:9" ht="60">
+    <row r="815" spans="1:9" ht="45">
       <c r="A815" s="29" t="s">
         <v>835</v>
       </c>
@@ -29155,7 +29156,7 @@
       </c>
       <c r="I816" s="31"/>
     </row>
-    <row r="817" spans="1:9" ht="45">
+    <row r="817" spans="1:9" ht="30">
       <c r="A817" s="29" t="s">
         <v>837</v>
       </c>
@@ -29230,7 +29231,7 @@
       </c>
       <c r="I819" s="31"/>
     </row>
-    <row r="820" spans="1:9" ht="45">
+    <row r="820" spans="1:9" ht="30">
       <c r="A820" s="29" t="s">
         <v>840</v>
       </c>
@@ -29430,7 +29431,7 @@
       </c>
       <c r="I827" s="31"/>
     </row>
-    <row r="828" spans="1:9" ht="30">
+    <row r="828" spans="1:9">
       <c r="A828" s="29" t="s">
         <v>848</v>
       </c>
@@ -29455,7 +29456,7 @@
       </c>
       <c r="I828" s="31"/>
     </row>
-    <row r="829" spans="1:9" ht="45">
+    <row r="829" spans="1:9" ht="30">
       <c r="A829" s="29" t="s">
         <v>849</v>
       </c>
@@ -29530,7 +29531,7 @@
       </c>
       <c r="I831" s="31"/>
     </row>
-    <row r="832" spans="1:9" ht="30">
+    <row r="832" spans="1:9">
       <c r="A832" s="29" t="s">
         <v>852</v>
       </c>
@@ -29580,7 +29581,7 @@
       </c>
       <c r="I833" s="31"/>
     </row>
-    <row r="834" spans="1:9" ht="60">
+    <row r="834" spans="1:9" ht="45">
       <c r="A834" s="29" t="s">
         <v>854</v>
       </c>
@@ -29632,7 +29633,7 @@
       </c>
       <c r="I835" s="31"/>
     </row>
-    <row r="836" spans="1:9" ht="60">
+    <row r="836" spans="1:9" ht="45">
       <c r="A836" s="29" t="s">
         <v>856</v>
       </c>
@@ -29734,7 +29735,7 @@
       </c>
       <c r="I839" s="31"/>
     </row>
-    <row r="840" spans="1:9" ht="30">
+    <row r="840" spans="1:9">
       <c r="A840" s="29" t="s">
         <v>860</v>
       </c>
@@ -29809,7 +29810,7 @@
       </c>
       <c r="I842" s="31"/>
     </row>
-    <row r="843" spans="1:9" ht="60">
+    <row r="843" spans="1:9" ht="45">
       <c r="A843" s="29" t="s">
         <v>863</v>
       </c>
@@ -29834,7 +29835,7 @@
       </c>
       <c r="I843" s="31"/>
     </row>
-    <row r="844" spans="1:9" ht="30">
+    <row r="844" spans="1:9">
       <c r="A844" s="29" t="s">
         <v>864</v>
       </c>
@@ -29934,7 +29935,7 @@
       </c>
       <c r="I847" s="31"/>
     </row>
-    <row r="848" spans="1:9" ht="60">
+    <row r="848" spans="1:9" ht="45">
       <c r="A848" s="29" t="s">
         <v>868</v>
       </c>
@@ -29942,7 +29943,7 @@
         <v>1205</v>
       </c>
       <c r="C848" s="31" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="D848" s="29"/>
       <c r="E848" s="29" t="s">
@@ -29961,7 +29962,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="849" spans="1:9" ht="30">
+    <row r="849" spans="1:9">
       <c r="A849" s="29" t="s">
         <v>869</v>
       </c>
@@ -30061,7 +30062,7 @@
       </c>
       <c r="I852" s="31"/>
     </row>
-    <row r="853" spans="1:9" ht="60">
+    <row r="853" spans="1:9" ht="45">
       <c r="A853" s="29" t="s">
         <v>873</v>
       </c>
@@ -30161,7 +30162,7 @@
       </c>
       <c r="I856" s="31"/>
     </row>
-    <row r="857" spans="1:9" ht="30">
+    <row r="857" spans="1:9">
       <c r="A857" s="29" t="s">
         <v>877</v>
       </c>
@@ -30211,7 +30212,7 @@
       </c>
       <c r="I858" s="31"/>
     </row>
-    <row r="859" spans="1:9" ht="30">
+    <row r="859" spans="1:9">
       <c r="A859" s="29" t="s">
         <v>879</v>
       </c>
@@ -30261,7 +30262,7 @@
       </c>
       <c r="I860" s="31"/>
     </row>
-    <row r="861" spans="1:9" ht="45">
+    <row r="861" spans="1:9" ht="30">
       <c r="A861" s="22" t="s">
         <v>881</v>
       </c>
@@ -30269,7 +30270,7 @@
         <v>1206</v>
       </c>
       <c r="C861" s="20" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D861" s="29"/>
       <c r="E861" s="29" t="s">
@@ -30286,7 +30287,7 @@
       </c>
       <c r="I861" s="31"/>
     </row>
-    <row r="862" spans="1:9" ht="60">
+    <row r="862" spans="1:9" ht="45">
       <c r="A862" s="29" t="s">
         <v>2291</v>
       </c>
@@ -30310,7 +30311,7 @@
         <v>17</v>
       </c>
       <c r="I862" s="20" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="863" spans="1:9" ht="45">
@@ -30588,7 +30589,7 @@
       </c>
       <c r="I873" s="31"/>
     </row>
-    <row r="874" spans="1:9" ht="60">
+    <row r="874" spans="1:9" ht="45">
       <c r="A874" s="29" t="s">
         <v>893</v>
       </c>
@@ -30688,7 +30689,7 @@
       </c>
       <c r="I877" s="31"/>
     </row>
-    <row r="878" spans="1:9" ht="30">
+    <row r="878" spans="1:9">
       <c r="A878" s="29" t="s">
         <v>897</v>
       </c>
@@ -30738,7 +30739,7 @@
       </c>
       <c r="I879" s="31"/>
     </row>
-    <row r="880" spans="1:9" ht="30">
+    <row r="880" spans="1:9">
       <c r="A880" s="22" t="s">
         <v>899</v>
       </c>
@@ -30763,7 +30764,7 @@
       </c>
       <c r="I880" s="31"/>
     </row>
-    <row r="881" spans="1:9" ht="45">
+    <row r="881" spans="1:9" ht="30">
       <c r="A881" s="29" t="s">
         <v>900</v>
       </c>
@@ -30771,7 +30772,7 @@
         <v>1206</v>
       </c>
       <c r="C881" s="31" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="D881" s="29"/>
       <c r="E881" s="29" t="s">
@@ -30838,7 +30839,7 @@
       </c>
       <c r="I883" s="31"/>
     </row>
-    <row r="884" spans="1:9" ht="45">
+    <row r="884" spans="1:9" ht="30">
       <c r="A884" s="29" t="s">
         <v>903</v>
       </c>
@@ -30863,7 +30864,7 @@
       </c>
       <c r="I884" s="31"/>
     </row>
-    <row r="885" spans="1:9" ht="45">
+    <row r="885" spans="1:9" ht="30">
       <c r="A885" s="29" t="s">
         <v>904</v>
       </c>
@@ -30913,7 +30914,7 @@
       </c>
       <c r="I886" s="31"/>
     </row>
-    <row r="887" spans="1:9" ht="45">
+    <row r="887" spans="1:9" ht="30">
       <c r="A887" s="29" t="s">
         <v>906</v>
       </c>
@@ -30988,7 +30989,7 @@
       </c>
       <c r="I889" s="31"/>
     </row>
-    <row r="890" spans="1:9" ht="30">
+    <row r="890" spans="1:9">
       <c r="A890" s="29" t="s">
         <v>909</v>
       </c>
@@ -31063,7 +31064,7 @@
       </c>
       <c r="I892" s="31"/>
     </row>
-    <row r="893" spans="1:9" ht="30">
+    <row r="893" spans="1:9">
       <c r="A893" s="29" t="s">
         <v>912</v>
       </c>
@@ -31188,7 +31189,7 @@
       </c>
       <c r="I897" s="31"/>
     </row>
-    <row r="898" spans="1:9" ht="45">
+    <row r="898" spans="1:9" ht="30">
       <c r="A898" s="29" t="s">
         <v>917</v>
       </c>
@@ -31263,7 +31264,7 @@
       </c>
       <c r="I900" s="31"/>
     </row>
-    <row r="901" spans="1:9" ht="45">
+    <row r="901" spans="1:9" ht="30">
       <c r="A901" s="29" t="s">
         <v>920</v>
       </c>
@@ -31338,7 +31339,7 @@
       </c>
       <c r="I903" s="31"/>
     </row>
-    <row r="904" spans="1:9" ht="30">
+    <row r="904" spans="1:9">
       <c r="A904" s="29" t="s">
         <v>923</v>
       </c>
@@ -31388,7 +31389,7 @@
       </c>
       <c r="I905" s="31"/>
     </row>
-    <row r="906" spans="1:9" ht="30">
+    <row r="906" spans="1:9">
       <c r="A906" s="29" t="s">
         <v>925</v>
       </c>
@@ -31438,7 +31439,7 @@
       </c>
       <c r="I907" s="31"/>
     </row>
-    <row r="908" spans="1:9" ht="30">
+    <row r="908" spans="1:9">
       <c r="A908" s="29" t="s">
         <v>927</v>
       </c>
@@ -31488,7 +31489,7 @@
       </c>
       <c r="I909" s="31"/>
     </row>
-    <row r="910" spans="1:9" ht="45">
+    <row r="910" spans="1:9" ht="30">
       <c r="A910" s="29" t="s">
         <v>929</v>
       </c>
@@ -31588,7 +31589,7 @@
       </c>
       <c r="I913" s="31"/>
     </row>
-    <row r="914" spans="1:9" ht="45">
+    <row r="914" spans="1:9" ht="30">
       <c r="A914" s="29" t="s">
         <v>933</v>
       </c>
@@ -31638,7 +31639,7 @@
       </c>
       <c r="I915" s="31"/>
     </row>
-    <row r="916" spans="1:9" ht="60">
+    <row r="916" spans="1:9" ht="45">
       <c r="A916" s="29" t="s">
         <v>935</v>
       </c>
@@ -31688,7 +31689,7 @@
       </c>
       <c r="I917" s="31"/>
     </row>
-    <row r="918" spans="1:9" ht="75">
+    <row r="918" spans="1:9" ht="60">
       <c r="A918" s="29" t="s">
         <v>937</v>
       </c>
@@ -31713,7 +31714,7 @@
       </c>
       <c r="I918" s="31"/>
     </row>
-    <row r="919" spans="1:9" ht="45">
+    <row r="919" spans="1:9" ht="30">
       <c r="A919" s="29" t="s">
         <v>938</v>
       </c>
@@ -31738,7 +31739,7 @@
       </c>
       <c r="I919" s="31"/>
     </row>
-    <row r="920" spans="1:9" ht="60">
+    <row r="920" spans="1:9" ht="45">
       <c r="A920" s="29" t="s">
         <v>939</v>
       </c>
@@ -31838,7 +31839,7 @@
       </c>
       <c r="I923" s="31"/>
     </row>
-    <row r="924" spans="1:9" ht="60">
+    <row r="924" spans="1:9" ht="45">
       <c r="A924" s="29" t="s">
         <v>943</v>
       </c>
@@ -31888,7 +31889,7 @@
       </c>
       <c r="I925" s="31"/>
     </row>
-    <row r="926" spans="1:9" ht="45">
+    <row r="926" spans="1:9" ht="30">
       <c r="A926" s="29" t="s">
         <v>945</v>
       </c>
@@ -31963,7 +31964,7 @@
       </c>
       <c r="I928" s="31"/>
     </row>
-    <row r="929" spans="1:9" ht="60">
+    <row r="929" spans="1:9" ht="45">
       <c r="A929" s="29" t="s">
         <v>948</v>
       </c>
@@ -32090,7 +32091,7 @@
       </c>
       <c r="I933" s="31"/>
     </row>
-    <row r="934" spans="1:9" ht="75">
+    <row r="934" spans="1:9" ht="60">
       <c r="A934" s="29" t="s">
         <v>953</v>
       </c>
@@ -32167,7 +32168,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="937" spans="1:9" ht="45">
+    <row r="937" spans="1:9" ht="30">
       <c r="A937" s="29" t="s">
         <v>956</v>
       </c>
@@ -32194,7 +32195,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="938" spans="1:9" ht="45">
+    <row r="938" spans="1:9" ht="30">
       <c r="A938" s="29" t="s">
         <v>957</v>
       </c>
@@ -32246,7 +32247,7 @@
       </c>
       <c r="I939" s="31"/>
     </row>
-    <row r="940" spans="1:9" ht="60">
+    <row r="940" spans="1:9" ht="45">
       <c r="A940" s="29" t="s">
         <v>959</v>
       </c>
@@ -32271,7 +32272,7 @@
       </c>
       <c r="I940" s="31"/>
     </row>
-    <row r="941" spans="1:9" ht="45">
+    <row r="941" spans="1:9" ht="30">
       <c r="A941" s="29" t="s">
         <v>960</v>
       </c>
@@ -32396,7 +32397,7 @@
       </c>
       <c r="I945" s="31"/>
     </row>
-    <row r="946" spans="1:9" ht="45">
+    <row r="946" spans="1:9" ht="30">
       <c r="A946" s="29" t="s">
         <v>965</v>
       </c>
@@ -32421,7 +32422,7 @@
       </c>
       <c r="I946" s="31"/>
     </row>
-    <row r="947" spans="1:9" ht="45">
+    <row r="947" spans="1:9" ht="30">
       <c r="A947" s="29" t="s">
         <v>966</v>
       </c>
@@ -32496,7 +32497,7 @@
       </c>
       <c r="I949" s="31"/>
     </row>
-    <row r="950" spans="1:9" ht="45">
+    <row r="950" spans="1:9" ht="30">
       <c r="A950" s="29" t="s">
         <v>969</v>
       </c>
@@ -32571,7 +32572,7 @@
       </c>
       <c r="I952" s="31"/>
     </row>
-    <row r="953" spans="1:9" ht="30">
+    <row r="953" spans="1:9">
       <c r="A953" s="29" t="s">
         <v>972</v>
       </c>
@@ -32771,7 +32772,7 @@
       </c>
       <c r="I960" s="31"/>
     </row>
-    <row r="961" spans="1:9" ht="45">
+    <row r="961" spans="1:9" ht="30">
       <c r="A961" s="29" t="s">
         <v>980</v>
       </c>
@@ -32821,7 +32822,7 @@
       </c>
       <c r="I962" s="31"/>
     </row>
-    <row r="963" spans="1:9" ht="45">
+    <row r="963" spans="1:9" ht="30">
       <c r="A963" s="29" t="s">
         <v>982</v>
       </c>
@@ -32846,7 +32847,7 @@
       </c>
       <c r="I963" s="31"/>
     </row>
-    <row r="964" spans="1:9" ht="45">
+    <row r="964" spans="1:9" ht="30">
       <c r="A964" s="29" t="s">
         <v>983</v>
       </c>
@@ -32921,7 +32922,7 @@
       </c>
       <c r="I966" s="31"/>
     </row>
-    <row r="967" spans="1:9" ht="45">
+    <row r="967" spans="1:9" ht="30">
       <c r="A967" s="29" t="s">
         <v>986</v>
       </c>
@@ -32946,7 +32947,7 @@
       </c>
       <c r="I967" s="31"/>
     </row>
-    <row r="968" spans="1:9" ht="45">
+    <row r="968" spans="1:9" ht="30">
       <c r="A968" s="29" t="s">
         <v>987</v>
       </c>
@@ -33046,7 +33047,7 @@
       </c>
       <c r="I971" s="31"/>
     </row>
-    <row r="972" spans="1:9" ht="45">
+    <row r="972" spans="1:9" ht="30">
       <c r="A972" s="29" t="s">
         <v>991</v>
       </c>
@@ -33071,7 +33072,7 @@
       </c>
       <c r="I972" s="31"/>
     </row>
-    <row r="973" spans="1:9" ht="45">
+    <row r="973" spans="1:9" ht="30">
       <c r="A973" s="29" t="s">
         <v>992</v>
       </c>
@@ -33096,7 +33097,7 @@
       </c>
       <c r="I973" s="31"/>
     </row>
-    <row r="974" spans="1:9" ht="45">
+    <row r="974" spans="1:9" ht="30">
       <c r="A974" s="29" t="s">
         <v>993</v>
       </c>
@@ -33121,7 +33122,7 @@
       </c>
       <c r="I974" s="31"/>
     </row>
-    <row r="975" spans="1:9" ht="45">
+    <row r="975" spans="1:9" ht="30">
       <c r="A975" s="29" t="s">
         <v>994</v>
       </c>
@@ -33171,7 +33172,7 @@
       </c>
       <c r="I976" s="31"/>
     </row>
-    <row r="977" spans="1:9" ht="45">
+    <row r="977" spans="1:9" ht="30">
       <c r="A977" s="29" t="s">
         <v>996</v>
       </c>
@@ -33221,7 +33222,7 @@
       </c>
       <c r="I978" s="31"/>
     </row>
-    <row r="979" spans="1:9" ht="45">
+    <row r="979" spans="1:9" ht="30">
       <c r="A979" s="29" t="s">
         <v>998</v>
       </c>
@@ -33246,7 +33247,7 @@
       </c>
       <c r="I979" s="31"/>
     </row>
-    <row r="980" spans="1:9" ht="60">
+    <row r="980" spans="1:9" ht="45">
       <c r="A980" s="29" t="s">
         <v>999</v>
       </c>
@@ -33346,7 +33347,7 @@
       </c>
       <c r="I983" s="31"/>
     </row>
-    <row r="984" spans="1:9" ht="30">
+    <row r="984" spans="1:9">
       <c r="A984" s="29" t="s">
         <v>1003</v>
       </c>
@@ -33396,7 +33397,7 @@
       </c>
       <c r="I985" s="31"/>
     </row>
-    <row r="986" spans="1:9" ht="45">
+    <row r="986" spans="1:9" ht="30">
       <c r="A986" s="29" t="s">
         <v>1005</v>
       </c>
@@ -33421,7 +33422,7 @@
       </c>
       <c r="I986" s="31"/>
     </row>
-    <row r="987" spans="1:9" ht="45">
+    <row r="987" spans="1:9" ht="30">
       <c r="A987" s="29" t="s">
         <v>1006</v>
       </c>
@@ -33571,7 +33572,7 @@
       </c>
       <c r="I992" s="31"/>
     </row>
-    <row r="993" spans="1:9" ht="45">
+    <row r="993" spans="1:9" ht="30">
       <c r="A993" s="29" t="s">
         <v>1012</v>
       </c>
@@ -33696,7 +33697,7 @@
       </c>
       <c r="I997" s="31"/>
     </row>
-    <row r="998" spans="1:9" ht="30">
+    <row r="998" spans="1:9">
       <c r="A998" s="29" t="s">
         <v>1017</v>
       </c>
@@ -33748,7 +33749,7 @@
       </c>
       <c r="I999" s="31"/>
     </row>
-    <row r="1000" spans="1:9" ht="60">
+    <row r="1000" spans="1:9" ht="45">
       <c r="A1000" s="29" t="s">
         <v>1019</v>
       </c>
@@ -33775,7 +33776,7 @@
       </c>
       <c r="I1000" s="31"/>
     </row>
-    <row r="1001" spans="1:9" ht="60">
+    <row r="1001" spans="1:9" ht="45">
       <c r="A1001" s="29" t="s">
         <v>1020</v>
       </c>
@@ -33935,7 +33936,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1007" spans="1:9" ht="60">
+    <row r="1007" spans="1:9" ht="45">
       <c r="A1007" s="29" t="s">
         <v>1026</v>
       </c>
@@ -33962,7 +33963,7 @@
       </c>
       <c r="I1007" s="31"/>
     </row>
-    <row r="1008" spans="1:9" ht="75">
+    <row r="1008" spans="1:9" ht="60">
       <c r="A1008" s="29" t="s">
         <v>1027</v>
       </c>
@@ -34253,7 +34254,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1019" spans="1:9" ht="60">
+    <row r="1019" spans="1:9" ht="45">
       <c r="A1019" s="29" t="s">
         <v>1038</v>
       </c>
@@ -34311,7 +34312,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1021" spans="1:9" ht="90">
+    <row r="1021" spans="1:9" ht="75">
       <c r="A1021" s="22" t="s">
         <v>1040</v>
       </c>
@@ -34340,7 +34341,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1022" spans="1:9" ht="120">
+    <row r="1022" spans="1:9" ht="90">
       <c r="A1022" s="22" t="s">
         <v>1041</v>
       </c>
@@ -34348,7 +34349,7 @@
         <v>1217</v>
       </c>
       <c r="C1022" s="20" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="D1022" s="29" t="s">
         <v>2176</v>
@@ -34427,7 +34428,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1025" spans="1:9" ht="60">
+    <row r="1025" spans="1:9" ht="45">
       <c r="A1025" s="29" t="s">
         <v>1044</v>
       </c>
@@ -34456,7 +34457,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1026" spans="1:9" ht="60">
+    <row r="1026" spans="1:9" ht="45">
       <c r="A1026" s="29" t="s">
         <v>1045</v>
       </c>
@@ -34485,7 +34486,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1027" spans="1:9" ht="75">
+    <row r="1027" spans="1:9" ht="60">
       <c r="A1027" s="29" t="s">
         <v>1046</v>
       </c>
@@ -34541,7 +34542,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1029" spans="1:9" ht="45">
+    <row r="1029" spans="1:9" ht="30">
       <c r="A1029" s="29" t="s">
         <v>1048</v>
       </c>
@@ -34624,7 +34625,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1032" spans="1:9" ht="90">
+    <row r="1032" spans="1:9" ht="75">
       <c r="A1032" s="29" t="s">
         <v>1049</v>
       </c>
@@ -34684,7 +34685,7 @@
     </row>
     <row r="1034" spans="1:9" ht="45">
       <c r="A1034" s="22" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="B1034" s="30" t="s">
         <v>1217</v>
@@ -34713,7 +34714,7 @@
     </row>
     <row r="1035" spans="1:9" ht="45">
       <c r="A1035" s="22" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="B1035" s="30" t="s">
         <v>1217</v>
@@ -34748,10 +34749,10 @@
         <v>1217</v>
       </c>
       <c r="C1036" s="31" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1036" s="29" t="s">
         <v>2317</v>
-      </c>
-      <c r="D1036" s="29" t="s">
-        <v>2318</v>
       </c>
       <c r="E1036" s="29" t="s">
         <v>22</v>
@@ -34778,7 +34779,7 @@
         <v>2153</v>
       </c>
       <c r="D1037" s="29" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="E1037" s="29" t="s">
         <v>22</v>
@@ -34796,7 +34797,7 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="1038" spans="1:9" ht="105">
+    <row r="1038" spans="1:9" ht="90">
       <c r="A1038" s="29" t="s">
         <v>1053</v>
       </c>
@@ -34804,7 +34805,7 @@
         <v>1217</v>
       </c>
       <c r="C1038" s="31" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="D1038" s="29" t="s">
         <v>2181</v>
@@ -34825,16 +34826,16 @@
     </row>
     <row r="1039" spans="1:9" ht="45">
       <c r="A1039" s="29" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="B1039" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1039" s="31" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="D1039" s="29" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="E1039" s="29" t="s">
         <v>22</v>
@@ -34854,16 +34855,16 @@
     </row>
     <row r="1040" spans="1:9" ht="45">
       <c r="A1040" s="29" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="B1040" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1040" s="31" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="D1040" s="29" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="E1040" s="29" t="s">
         <v>22</v>
@@ -34881,7 +34882,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1041" spans="1:9" ht="45">
+    <row r="1041" spans="1:9" ht="30">
       <c r="A1041" s="29" t="s">
         <v>1054</v>
       </c>
@@ -34889,7 +34890,7 @@
         <v>1217</v>
       </c>
       <c r="C1041" s="20" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="D1041" s="29" t="s">
         <v>2182</v>
@@ -34916,7 +34917,7 @@
         <v>1217</v>
       </c>
       <c r="C1042" s="20" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="D1042" s="29" t="s">
         <v>2182</v>
@@ -34945,7 +34946,7 @@
         <v>1217</v>
       </c>
       <c r="C1043" s="20" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D1043" s="22" t="s">
         <v>2182</v>
@@ -34966,15 +34967,15 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1044" spans="1:9" ht="45">
+    <row r="1044" spans="1:9" ht="30">
       <c r="A1044" s="22" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="B1044" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1044" s="20" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D1044" s="22" t="s">
         <v>2182</v>
@@ -35001,7 +35002,7 @@
         <v>1217</v>
       </c>
       <c r="C1045" s="20" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="D1045" s="29" t="s">
         <v>2183</v>
@@ -35020,7 +35021,7 @@
       </c>
       <c r="I1045" s="31"/>
     </row>
-    <row r="1046" spans="1:9" ht="60">
+    <row r="1046" spans="1:9" ht="45">
       <c r="A1046" s="29" t="s">
         <v>1058</v>
       </c>
@@ -35028,7 +35029,7 @@
         <v>1217</v>
       </c>
       <c r="C1046" s="20" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="D1046" s="29" t="s">
         <v>2183</v>
@@ -35049,16 +35050,16 @@
     </row>
     <row r="1047" spans="1:9" ht="60">
       <c r="A1047" s="22" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="B1047" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1047" s="20" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="D1047" s="22" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="E1047" s="29" t="s">
         <v>22</v>
@@ -35076,18 +35077,18 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1048" spans="1:9" ht="60">
+    <row r="1048" spans="1:9" ht="45">
       <c r="A1048" s="22" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="B1048" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1048" s="20" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="D1048" s="22" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="E1048" s="29" t="s">
         <v>22</v>
@@ -35105,7 +35106,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1049" spans="1:9" ht="75">
+    <row r="1049" spans="1:9" ht="60">
       <c r="A1049" s="29" t="s">
         <v>1059</v>
       </c>
@@ -35113,7 +35114,7 @@
         <v>1217</v>
       </c>
       <c r="C1049" s="20" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="D1049" s="29" t="s">
         <v>2184</v>
@@ -35140,7 +35141,7 @@
         <v>1217</v>
       </c>
       <c r="C1050" s="20" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="D1050" s="29"/>
       <c r="E1050" s="29" t="s">
@@ -35167,7 +35168,7 @@
         <v>1217</v>
       </c>
       <c r="C1051" s="20" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="D1051" s="29"/>
       <c r="E1051" s="29" t="s">
@@ -35192,7 +35193,7 @@
         <v>1217</v>
       </c>
       <c r="C1052" s="20" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D1052" s="29" t="s">
         <v>2185</v>
@@ -35211,7 +35212,7 @@
       </c>
       <c r="I1052" s="31"/>
     </row>
-    <row r="1053" spans="1:9" ht="60">
+    <row r="1053" spans="1:9" ht="45">
       <c r="A1053" s="29" t="s">
         <v>1063</v>
       </c>
@@ -35219,7 +35220,7 @@
         <v>1217</v>
       </c>
       <c r="C1053" s="20" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="D1053" s="29" t="s">
         <v>2185</v>
@@ -35238,7 +35239,7 @@
       </c>
       <c r="I1053" s="31"/>
     </row>
-    <row r="1054" spans="1:9" ht="75">
+    <row r="1054" spans="1:9" ht="60">
       <c r="A1054" s="29" t="s">
         <v>1064</v>
       </c>
@@ -35246,7 +35247,7 @@
         <v>1217</v>
       </c>
       <c r="C1054" s="20" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="D1054" s="29" t="s">
         <v>2186</v>
@@ -35265,7 +35266,7 @@
       </c>
       <c r="I1054" s="31"/>
     </row>
-    <row r="1055" spans="1:9" ht="90">
+    <row r="1055" spans="1:9" ht="75">
       <c r="A1055" s="29" t="s">
         <v>1065</v>
       </c>
@@ -35273,7 +35274,7 @@
         <v>1217</v>
       </c>
       <c r="C1055" s="20" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="D1055" s="29" t="s">
         <v>2186</v>
@@ -35292,18 +35293,18 @@
       </c>
       <c r="I1055" s="31"/>
     </row>
-    <row r="1056" spans="1:9" ht="90">
+    <row r="1056" spans="1:9" ht="75">
       <c r="A1056" s="22" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="B1056" s="24" t="s">
         <v>1217</v>
       </c>
       <c r="C1056" s="20" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="D1056" s="22" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="E1056" s="29" t="s">
         <v>22</v>
@@ -35321,7 +35322,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1057" spans="1:9" ht="90">
+    <row r="1057" spans="1:9" ht="75">
       <c r="A1057" s="29" t="s">
         <v>1066</v>
       </c>
@@ -35329,10 +35330,10 @@
         <v>1217</v>
       </c>
       <c r="C1057" s="20" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="D1057" s="29" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="E1057" s="29" t="s">
         <v>22</v>
@@ -35358,7 +35359,7 @@
         <v>1217</v>
       </c>
       <c r="C1058" s="31" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="D1058" s="29" t="s">
         <v>2187</v>
@@ -35387,7 +35388,7 @@
         <v>1217</v>
       </c>
       <c r="C1059" s="20" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="D1059" s="29" t="s">
         <v>2187</v>
@@ -35416,7 +35417,7 @@
         <v>1217</v>
       </c>
       <c r="C1060" s="31" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="D1060" s="29" t="s">
         <v>2187</v>
@@ -35437,7 +35438,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1061" spans="1:9" ht="45">
+    <row r="1061" spans="1:9" ht="30">
       <c r="A1061" s="29" t="s">
         <v>1070</v>
       </c>
@@ -35445,7 +35446,7 @@
         <v>1217</v>
       </c>
       <c r="C1061" s="31" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="D1061" s="29"/>
       <c r="E1061" s="29" t="s">
@@ -35470,7 +35471,7 @@
         <v>1217</v>
       </c>
       <c r="C1062" s="31" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="D1062" s="29" t="s">
         <v>2188</v>
@@ -35497,10 +35498,10 @@
         <v>1217</v>
       </c>
       <c r="C1063" s="31" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="D1063" s="29" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="E1063" s="29" t="s">
         <v>22</v>
@@ -35526,10 +35527,10 @@
         <v>1217</v>
       </c>
       <c r="C1064" s="31" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="D1064" s="29" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="E1064" s="29" t="s">
         <v>22</v>
@@ -35549,16 +35550,16 @@
     </row>
     <row r="1065" spans="1:9" ht="45">
       <c r="A1065" s="29" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="B1065" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1065" s="31" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="D1065" s="29" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="E1065" s="29" t="s">
         <v>22</v>
@@ -35584,7 +35585,7 @@
         <v>1217</v>
       </c>
       <c r="C1066" s="31" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="D1066" s="29" t="s">
         <v>2189</v>
@@ -35603,7 +35604,7 @@
       </c>
       <c r="I1066" s="31"/>
     </row>
-    <row r="1067" spans="1:9" ht="45">
+    <row r="1067" spans="1:9" ht="30">
       <c r="A1067" s="29" t="s">
         <v>1075</v>
       </c>
@@ -35611,7 +35612,7 @@
         <v>1217</v>
       </c>
       <c r="C1067" s="31" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="D1067" s="29" t="s">
         <v>2189</v>
@@ -35630,7 +35631,7 @@
       </c>
       <c r="I1067" s="31"/>
     </row>
-    <row r="1068" spans="1:9" ht="60">
+    <row r="1068" spans="1:9" ht="45">
       <c r="A1068" s="29" t="s">
         <v>1076</v>
       </c>
@@ -35638,7 +35639,7 @@
         <v>1217</v>
       </c>
       <c r="C1068" s="31" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="D1068" s="29" t="s">
         <v>2190</v>
@@ -35665,7 +35666,7 @@
         <v>1217</v>
       </c>
       <c r="C1069" s="31" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="D1069" s="29" t="s">
         <v>2190</v>
@@ -35684,7 +35685,7 @@
       </c>
       <c r="I1069" s="31"/>
     </row>
-    <row r="1070" spans="1:9" ht="45">
+    <row r="1070" spans="1:9" ht="30">
       <c r="A1070" s="29" t="s">
         <v>1078</v>
       </c>
@@ -35692,7 +35693,7 @@
         <v>1217</v>
       </c>
       <c r="C1070" s="31" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="D1070" s="29"/>
       <c r="E1070" s="29" t="s">
@@ -35717,7 +35718,7 @@
         <v>1217</v>
       </c>
       <c r="C1071" s="31" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="D1071" s="29" t="s">
         <v>2191</v>
@@ -35744,7 +35745,7 @@
         <v>1217</v>
       </c>
       <c r="C1072" s="20" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="D1072" s="29" t="s">
         <v>2192</v>
@@ -35773,7 +35774,7 @@
         <v>1217</v>
       </c>
       <c r="C1073" s="31" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="D1073" s="29" t="s">
         <v>2192</v>
@@ -35800,7 +35801,7 @@
         <v>1217</v>
       </c>
       <c r="C1074" s="31" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="D1074" s="29" t="s">
         <v>2193</v>
@@ -35827,7 +35828,7 @@
         <v>1217</v>
       </c>
       <c r="C1075" s="31" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="D1075" s="29" t="s">
         <v>2193</v>
@@ -35854,7 +35855,7 @@
         <v>1217</v>
       </c>
       <c r="C1076" s="31" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="D1076" s="29" t="s">
         <v>2194</v>
@@ -35873,7 +35874,7 @@
       </c>
       <c r="I1076" s="31"/>
     </row>
-    <row r="1077" spans="1:9" ht="45">
+    <row r="1077" spans="1:9" ht="30">
       <c r="A1077" s="29" t="s">
         <v>1085</v>
       </c>
@@ -35881,7 +35882,7 @@
         <v>1217</v>
       </c>
       <c r="C1077" s="31" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="D1077" s="29" t="s">
         <v>2194</v>
@@ -35908,7 +35909,7 @@
         <v>1217</v>
       </c>
       <c r="C1078" s="31" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="D1078" s="29" t="s">
         <v>2195</v>
@@ -35935,7 +35936,7 @@
         <v>1217</v>
       </c>
       <c r="C1079" s="31" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="D1079" s="29" t="s">
         <v>2195</v>
@@ -35962,7 +35963,7 @@
         <v>1217</v>
       </c>
       <c r="C1080" s="31" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="D1080" s="29" t="s">
         <v>2196</v>
@@ -35981,7 +35982,7 @@
       </c>
       <c r="I1080" s="31"/>
     </row>
-    <row r="1081" spans="1:9" ht="45">
+    <row r="1081" spans="1:9" ht="30">
       <c r="A1081" s="29" t="s">
         <v>1089</v>
       </c>
@@ -35989,7 +35990,7 @@
         <v>1217</v>
       </c>
       <c r="C1081" s="31" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="D1081" s="29" t="s">
         <v>2196</v>
@@ -36016,7 +36017,7 @@
         <v>1217</v>
       </c>
       <c r="C1082" s="31" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="D1082" s="29" t="s">
         <v>2197</v>
@@ -36037,7 +36038,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1083" spans="1:9" ht="60">
+    <row r="1083" spans="1:9" ht="45">
       <c r="A1083" s="29" t="s">
         <v>1091</v>
       </c>
@@ -36045,7 +36046,7 @@
         <v>1217</v>
       </c>
       <c r="C1083" s="31" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="D1083" s="29" t="s">
         <v>2197</v>
@@ -36068,16 +36069,16 @@
     </row>
     <row r="1084" spans="1:9" ht="45">
       <c r="A1084" s="22" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="B1084" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1084" s="20" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="D1084" s="29" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="E1084" s="29" t="s">
         <v>22</v>
@@ -36095,18 +36096,18 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1085" spans="1:9" ht="60">
+    <row r="1085" spans="1:9" ht="45">
       <c r="A1085" s="22" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="B1085" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1085" s="20" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D1085" s="29" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="E1085" s="29" t="s">
         <v>22</v>
@@ -36126,16 +36127,16 @@
     </row>
     <row r="1086" spans="1:9" ht="45">
       <c r="A1086" s="29" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="B1086" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1086" s="31" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="D1086" s="29" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="E1086" s="29" t="s">
         <v>22</v>
@@ -36150,21 +36151,21 @@
         <v>17</v>
       </c>
       <c r="I1086" s="20" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="1087" spans="1:9" ht="45">
       <c r="A1087" s="29" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="B1087" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1087" s="31" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="D1087" s="29" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="E1087" s="29" t="s">
         <v>22</v>
@@ -36179,7 +36180,7 @@
         <v>17</v>
       </c>
       <c r="I1087" s="20" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="1088" spans="1:9" ht="60">
@@ -36190,7 +36191,7 @@
         <v>1217</v>
       </c>
       <c r="C1088" s="31" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="D1088" s="29" t="s">
         <v>2198</v>
@@ -36248,7 +36249,7 @@
         <v>1217</v>
       </c>
       <c r="C1090" s="31" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="D1090" s="29" t="s">
         <v>2199</v>
@@ -36298,7 +36299,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1092" spans="1:9" ht="75">
+    <row r="1092" spans="1:9" ht="60">
       <c r="A1092" s="29" t="s">
         <v>1096</v>
       </c>
@@ -36306,7 +36307,7 @@
         <v>1217</v>
       </c>
       <c r="C1092" s="31" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="D1092" s="29" t="s">
         <v>2201</v>
@@ -36327,18 +36328,18 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1093" spans="1:9" ht="45">
+    <row r="1093" spans="1:9" ht="30">
       <c r="A1093" s="22" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="B1093" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1093" s="31" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="D1093" s="29" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="E1093" s="29" t="s">
         <v>22</v>
@@ -36354,18 +36355,18 @@
       </c>
       <c r="I1093" s="31"/>
     </row>
-    <row r="1094" spans="1:9" ht="45">
+    <row r="1094" spans="1:9" ht="30">
       <c r="A1094" s="22" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="B1094" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1094" s="31" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="D1094" s="29" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="E1094" s="29" t="s">
         <v>22</v>
@@ -36381,18 +36382,18 @@
       </c>
       <c r="I1094" s="31"/>
     </row>
-    <row r="1095" spans="1:9" ht="45">
+    <row r="1095" spans="1:9" ht="30">
       <c r="A1095" s="22" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="B1095" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1095" s="31" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="D1095" s="29" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="E1095" s="29" t="s">
         <v>22</v>
@@ -36410,16 +36411,16 @@
     </row>
     <row r="1096" spans="1:9" ht="45">
       <c r="A1096" s="22" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="B1096" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1096" s="31" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="D1096" s="29" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="E1096" s="29" t="s">
         <v>22</v>
@@ -36437,16 +36438,16 @@
     </row>
     <row r="1097" spans="1:9" ht="45">
       <c r="A1097" s="22" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="B1097" s="30" t="s">
         <v>1217</v>
       </c>
       <c r="C1097" s="31" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="D1097" s="29" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E1097" s="29" t="s">
         <v>22</v>
@@ -36491,7 +36492,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1099" spans="1:9" ht="60">
+    <row r="1099" spans="1:9" ht="45">
       <c r="A1099" s="29" t="s">
         <v>1098</v>
       </c>
@@ -36674,7 +36675,7 @@
       </c>
       <c r="I1105" s="31"/>
     </row>
-    <row r="1106" spans="1:9" ht="75">
+    <row r="1106" spans="1:9" ht="60">
       <c r="A1106" s="29" t="s">
         <v>1104</v>
       </c>
@@ -36699,7 +36700,7 @@
       </c>
       <c r="I1106" s="31"/>
     </row>
-    <row r="1107" spans="1:9" ht="45">
+    <row r="1107" spans="1:9" ht="30">
       <c r="A1107" s="29" t="s">
         <v>1105</v>
       </c>
@@ -36734,6 +36735,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36741,11 +36747,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1102:I1107 A20:H1040 I20:I1043 A34:I1100">
@@ -36864,6 +36865,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -36912,32 +36928,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -36957,9 +36951,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-OXCSTOR: update according to comment.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -7787,21 +7787,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7825,6 +7810,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8753,8 +8753,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1012" sqref="A1012:XFD1012"/>
+    <sheetView tabSelected="1" topLeftCell="D878" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A886" sqref="A886:XFD886"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8809,127 +8809,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8942,12 +8942,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8960,12 +8960,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8978,12 +8978,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8996,60 +8996,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -30898,7 +30898,7 @@
         <v>15</v>
       </c>
       <c r="H886" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I886" s="31"/>
     </row>
@@ -36742,6 +36742,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36749,11 +36754,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1103:I1108 A20:I1101">
@@ -36872,18 +36872,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36936,6 +36936,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -36945,14 +36953,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Task 1933441 : [MS-OXCSTOR]: Add and update test cases for document update
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15766" uniqueCount="2422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7882" uniqueCount="2417">
   <si>
     <t>Req ID</t>
   </si>
@@ -7127,10 +7127,6 @@
     <t>[In Appendix A: Product Behavior]  Implementation returns the Folder ID of all of the following folders in this field [FolderIds in RopLogon ROP Success Response Buffer for Public Folders]: Public Folders Root Folder (All other folders listed here are direct or indirect children of this folder), Interpersonal messages subtree, Non-interpersonal messages subtree, EForms Registry, Free/Busy Data, Offline address book Data, EForms Registry for the user's locale, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, NNTP Article Index, Empty, Empty, Empty. (Exchange 2003, Exchange 2007 and Exchange 2010 follow this behavior)</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCSTOR_R306800301, MS-OXCSTOR_R306800302.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -7285,9 +7281,6 @@
   </si>
   <si>
     <t>[In Read/Write Properties] The PidTagDeleteAfterSubmit property is writable.&lt;15&gt;</t>
-  </si>
-  <si>
-    <t>[In Read/Write Properties] The PidTagDisplayName property is read/write.&lt;16&gt;</t>
   </si>
   <si>
     <t>[In PidTagComment Property] The PidTagComment property ([MS-OXPROPS] section 2.631) contains a mailbox comment.</t>
@@ -7500,23 +7493,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagComment property by using the RopSetProperties ROP ([MS-OXCROPS] section 2.2.8.6).(Microsoft Exchange Server 2013 Service Pack 1 (SP1) and Exchange 2016 follow this behavior).</t>
+    <t>[In Appendix A: Product Behavior] Implementation does return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagDisplayName property by using the RopSetProperties ROP.(Microsoft Exchange Server 2013 Service Pack 1 (SP1) and Exchange 2016 follow this behavior)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation don't return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagComment property by using the RopSetProperties ROP ([MS-OXCROPS] section 2.2.8.6).(Exchange 2007 and Exchange 2010 follow this behavior).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does support PidTagDisplayName  property as read-only. &lt;16&gt; Section 2.2.2.1.2.3:  In Exchange 2013 SP1 and Exchange 2016 this property is read-only.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does not return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagDisplayName property by using the RopSetProperties ROP.(Exchange 2007, Exchange 2010 follow this behavior)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagDisplayName property by using the RopSetProperties ROP.(Microsoft Exchange Server 2013 Service Pack 1 (SP1) and Exchange 2016 follow this behavior)</t>
+    <t>[In Read/Write Properties] The PidTagDisplayName property is read/write.&lt;16&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7807,21 +7788,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7845,6 +7811,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8440,6 +8421,7 @@
   <autoFilter ref="A19:I1108">
     <filterColumn colId="0">
       <filters>
+        <filter val="MS-OXCSTOR_R3068003"/>
         <filter val="MS-OXCSTOR_R306800301"/>
         <filter val="MS-OXCSTOR_R306800302"/>
       </filters>
@@ -8815,7 +8797,7 @@
   <dimension ref="A1:L1110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1041" sqref="C1041"/>
+      <selection activeCell="C448" sqref="C448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8859,7 +8841,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -8870,127 +8852,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -9003,12 +8985,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9021,12 +9003,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -9039,12 +9021,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -9057,60 +9039,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -10229,7 +10211,7 @@
         <v>1109</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -10245,7 +10227,7 @@
         <v>17</v>
       </c>
       <c r="I63" s="20" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -10281,7 +10263,7 @@
         <v>1109</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -10385,7 +10367,7 @@
         <v>1109</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -11541,7 +11523,7 @@
         <v>1111</v>
       </c>
       <c r="C115" s="20" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -11745,7 +11727,7 @@
         <v>1112</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -11947,7 +11929,7 @@
         <v>1112</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -13574,7 +13556,7 @@
         <v>1122</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -13624,7 +13606,7 @@
         <v>1122</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -13874,7 +13856,7 @@
         <v>1122</v>
       </c>
       <c r="C208" s="20" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -13949,7 +13931,7 @@
         <v>1124</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="D211" s="29"/>
       <c r="E211" s="29" t="s">
@@ -14376,7 +14358,7 @@
         <v>1129</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -14753,7 +14735,7 @@
         <v>1132</v>
       </c>
       <c r="C243" s="20" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="29" t="s">
@@ -14769,7 +14751,7 @@
         <v>17</v>
       </c>
       <c r="I243" s="20" t="s">
-        <v>2383</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="244" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -18429,7 +18411,7 @@
         <v>1161</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="D389" s="29"/>
       <c r="E389" s="29" t="s">
@@ -18803,7 +18785,7 @@
         <v>1162</v>
       </c>
       <c r="C403" s="20" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="D403" s="29"/>
       <c r="E403" s="29" t="s">
@@ -18878,7 +18860,7 @@
         <v>1163</v>
       </c>
       <c r="C406" s="20" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="D406" s="29"/>
       <c r="E406" s="29" t="s">
@@ -18953,7 +18935,7 @@
         <v>1164</v>
       </c>
       <c r="C409" s="20" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -19028,7 +19010,7 @@
         <v>1165</v>
       </c>
       <c r="C412" s="20" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="D412" s="29"/>
       <c r="E412" s="29" t="s">
@@ -19103,7 +19085,7 @@
         <v>1166</v>
       </c>
       <c r="C415" s="20" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="D415" s="29"/>
       <c r="E415" s="29" t="s">
@@ -19178,7 +19160,7 @@
         <v>1167</v>
       </c>
       <c r="C418" s="20" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="D418" s="29"/>
       <c r="E418" s="29" t="s">
@@ -19228,7 +19210,7 @@
         <v>1168</v>
       </c>
       <c r="C420" s="20" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="D420" s="29"/>
       <c r="E420" s="29" t="s">
@@ -19278,7 +19260,7 @@
         <v>1169</v>
       </c>
       <c r="C422" s="20" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="D422" s="29"/>
       <c r="E422" s="29" t="s">
@@ -19328,7 +19310,7 @@
         <v>1170</v>
       </c>
       <c r="C424" s="20" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="D424" s="29"/>
       <c r="E424" s="29" t="s">
@@ -19403,7 +19385,7 @@
         <v>1171</v>
       </c>
       <c r="C427" s="20" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="D427" s="29"/>
       <c r="E427" s="29" t="s">
@@ -19453,7 +19435,7 @@
         <v>1172</v>
       </c>
       <c r="C429" s="20" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="D429" s="29"/>
       <c r="E429" s="29" t="s">
@@ -19503,7 +19485,7 @@
         <v>1173</v>
       </c>
       <c r="C431" s="20" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D431" s="29"/>
       <c r="E431" s="29" t="s">
@@ -19522,13 +19504,13 @@
     </row>
     <row r="432" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="22" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="B432" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C432" s="36" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="D432" s="34"/>
       <c r="E432" s="29" t="s">
@@ -19547,13 +19529,13 @@
     </row>
     <row r="433" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="22" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="B433" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C433" s="36" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="D433" s="34"/>
       <c r="E433" s="29" t="s">
@@ -19572,13 +19554,13 @@
     </row>
     <row r="434" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="22" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="B434" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C434" s="36" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="D434" s="34"/>
       <c r="E434" s="29" t="s">
@@ -19597,13 +19579,13 @@
     </row>
     <row r="435" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="22" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="B435" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C435" s="36" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="D435" s="34"/>
       <c r="E435" s="29" t="s">
@@ -19622,13 +19604,13 @@
     </row>
     <row r="436" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="22" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="B436" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C436" s="36" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="D436" s="34"/>
       <c r="E436" s="34" t="s">
@@ -19647,13 +19629,13 @@
     </row>
     <row r="437" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="22" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="B437" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C437" s="36" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="D437" s="34"/>
       <c r="E437" s="34" t="s">
@@ -19672,13 +19654,13 @@
     </row>
     <row r="438" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="22" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="B438" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C438" s="36" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="D438" s="34"/>
       <c r="E438" s="29" t="s">
@@ -19728,7 +19710,7 @@
         <v>1175</v>
       </c>
       <c r="C440" s="20" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D440" s="29"/>
       <c r="E440" s="29" t="s">
@@ -19775,7 +19757,7 @@
         <v>456</v>
       </c>
       <c r="B442" s="24" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="C442" s="31" t="s">
         <v>1605</v>
@@ -19800,10 +19782,10 @@
         <v>457</v>
       </c>
       <c r="B443" s="24" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C443" s="20" t="s">
         <v>2342</v>
-      </c>
-      <c r="C443" s="20" t="s">
-        <v>2343</v>
       </c>
       <c r="D443" s="29"/>
       <c r="E443" s="29" t="s">
@@ -19828,7 +19810,7 @@
         <v>1176</v>
       </c>
       <c r="C444" s="20" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="D444" s="29"/>
       <c r="E444" s="29" t="s">
@@ -19853,7 +19835,7 @@
         <v>1176</v>
       </c>
       <c r="C445" s="20" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="D445" s="29" t="s">
         <v>2132</v>
@@ -19909,7 +19891,7 @@
         <v>1176</v>
       </c>
       <c r="C447" s="20" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="D447" s="29"/>
       <c r="E447" s="29" t="s">
@@ -19928,7 +19910,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="448" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A448" s="29" t="s">
         <v>462</v>
       </c>
@@ -19936,7 +19918,7 @@
         <v>1176</v>
       </c>
       <c r="C448" s="20" t="s">
-        <v>2347</v>
+        <v>2416</v>
       </c>
       <c r="D448" s="29" t="s">
         <v>2132</v>
@@ -19951,11 +19933,9 @@
         <v>15</v>
       </c>
       <c r="H448" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I448" s="20" t="s">
-        <v>2294</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I448" s="20"/>
     </row>
     <row r="449" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="29" t="s">
@@ -20098,7 +20078,7 @@
         <v>1177</v>
       </c>
       <c r="C454" s="20" t="s">
-        <v>2348</v>
+        <v>2346</v>
       </c>
       <c r="D454" s="29"/>
       <c r="E454" s="29" t="s">
@@ -20148,7 +20128,7 @@
         <v>1178</v>
       </c>
       <c r="C456" s="20" t="s">
-        <v>2349</v>
+        <v>2347</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29" t="s">
@@ -20298,7 +20278,7 @@
         <v>1180</v>
       </c>
       <c r="C462" s="20" t="s">
-        <v>2350</v>
+        <v>2348</v>
       </c>
       <c r="D462" s="29"/>
       <c r="E462" s="29" t="s">
@@ -20423,7 +20403,7 @@
         <v>1181</v>
       </c>
       <c r="C467" s="20" t="s">
-        <v>2351</v>
+        <v>2349</v>
       </c>
       <c r="D467" s="29"/>
       <c r="E467" s="29" t="s">
@@ -20629,7 +20609,7 @@
         <v>1183</v>
       </c>
       <c r="C475" s="20" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
       <c r="D475" s="29"/>
       <c r="E475" s="29" t="s">
@@ -20704,7 +20684,7 @@
         <v>1184</v>
       </c>
       <c r="C478" s="20" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29" t="s">
@@ -20929,7 +20909,7 @@
         <v>32</v>
       </c>
       <c r="C487" s="20" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="D487" s="29"/>
       <c r="E487" s="29" t="s">
@@ -23504,7 +23484,7 @@
         <v>1191</v>
       </c>
       <c r="C590" s="20" t="s">
-        <v>2354</v>
+        <v>2352</v>
       </c>
       <c r="D590" s="29"/>
       <c r="E590" s="29" t="s">
@@ -23604,7 +23584,7 @@
         <v>1192</v>
       </c>
       <c r="C594" s="20" t="s">
-        <v>2386</v>
+        <v>2384</v>
       </c>
       <c r="D594" s="29"/>
       <c r="E594" s="29" t="s">
@@ -23620,7 +23600,7 @@
         <v>17</v>
       </c>
       <c r="I594" s="20" t="s">
-        <v>2389</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="595" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -23781,7 +23761,7 @@
         <v>1194</v>
       </c>
       <c r="C601" s="20" t="s">
-        <v>2355</v>
+        <v>2353</v>
       </c>
       <c r="D601" s="29"/>
       <c r="E601" s="29" t="s">
@@ -23833,7 +23813,7 @@
         <v>1194</v>
       </c>
       <c r="C603" s="20" t="s">
-        <v>2356</v>
+        <v>2354</v>
       </c>
       <c r="D603" s="29"/>
       <c r="E603" s="29" t="s">
@@ -23849,7 +23829,7 @@
         <v>17</v>
       </c>
       <c r="I603" s="20" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="604" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -23937,7 +23917,7 @@
         <v>1194</v>
       </c>
       <c r="C607" s="20" t="s">
-        <v>2357</v>
+        <v>2355</v>
       </c>
       <c r="D607" s="29"/>
       <c r="E607" s="29" t="s">
@@ -23953,7 +23933,7 @@
         <v>17</v>
       </c>
       <c r="I607" s="20" t="s">
-        <v>2409</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="608" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -23964,7 +23944,7 @@
         <v>1194</v>
       </c>
       <c r="C608" s="20" t="s">
-        <v>2358</v>
+        <v>2356</v>
       </c>
       <c r="D608" s="29"/>
       <c r="E608" s="29" t="s">
@@ -24107,7 +24087,7 @@
         <v>17</v>
       </c>
       <c r="I613" s="20" t="s">
-        <v>2398</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="614" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -26932,7 +26912,7 @@
         <v>1198</v>
       </c>
       <c r="C726" s="20" t="s">
-        <v>2359</v>
+        <v>2357</v>
       </c>
       <c r="D726" s="29"/>
       <c r="E726" s="29" t="s">
@@ -26982,7 +26962,7 @@
         <v>1198</v>
       </c>
       <c r="C728" s="20" t="s">
-        <v>2360</v>
+        <v>2358</v>
       </c>
       <c r="D728" s="29"/>
       <c r="E728" s="29" t="s">
@@ -27007,7 +26987,7 @@
         <v>1198</v>
       </c>
       <c r="C729" s="20" t="s">
-        <v>2361</v>
+        <v>2359</v>
       </c>
       <c r="D729" s="29"/>
       <c r="E729" s="29" t="s">
@@ -30946,7 +30926,7 @@
         <v>1204</v>
       </c>
       <c r="C886" s="20" t="s">
-        <v>2362</v>
+        <v>2360</v>
       </c>
       <c r="D886" s="29"/>
       <c r="E886" s="29" t="s">
@@ -31746,7 +31726,7 @@
         <v>1208</v>
       </c>
       <c r="C918" s="20" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="D918" s="29"/>
       <c r="E918" s="29" t="s">
@@ -32146,7 +32126,7 @@
         <v>1208</v>
       </c>
       <c r="C934" s="20" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
       <c r="D934" s="29"/>
       <c r="E934" s="29" t="s">
@@ -32323,7 +32303,7 @@
         <v>1208</v>
       </c>
       <c r="C941" s="20" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
       <c r="D941" s="29"/>
       <c r="E941" s="29" t="s">
@@ -32377,7 +32357,7 @@
         <v>1208</v>
       </c>
       <c r="C943" s="20" t="s">
-        <v>2366</v>
+        <v>2364</v>
       </c>
       <c r="D943" s="29"/>
       <c r="E943" s="29" t="s">
@@ -33404,7 +33384,7 @@
         <v>1212</v>
       </c>
       <c r="C984" s="20" t="s">
-        <v>2367</v>
+        <v>2365</v>
       </c>
       <c r="D984" s="29"/>
       <c r="E984" s="29" t="s">
@@ -33420,7 +33400,7 @@
         <v>17</v>
       </c>
       <c r="I984" s="20" t="s">
-        <v>2411</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="985" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -33456,7 +33436,7 @@
         <v>1212</v>
       </c>
       <c r="C986" s="20" t="s">
-        <v>2413</v>
+        <v>2411</v>
       </c>
       <c r="D986" s="29"/>
       <c r="E986" s="29" t="s">
@@ -33631,7 +33611,7 @@
         <v>1212</v>
       </c>
       <c r="C993" s="20" t="s">
-        <v>2368</v>
+        <v>2366</v>
       </c>
       <c r="D993" s="29"/>
       <c r="E993" s="29" t="s">
@@ -33656,7 +33636,7 @@
         <v>1212</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2412</v>
+        <v>2410</v>
       </c>
       <c r="D994" s="29"/>
       <c r="E994" s="29" t="s">
@@ -34195,16 +34175,16 @@
     </row>
     <row r="1015" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1015" s="34" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="B1015" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1015" s="36" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D1015" s="34" t="s">
         <v>2302</v>
-      </c>
-      <c r="D1015" s="34" t="s">
-        <v>2303</v>
       </c>
       <c r="E1015" s="29" t="s">
         <v>22</v>
@@ -34222,16 +34202,16 @@
     </row>
     <row r="1016" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="34" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="B1016" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1016" s="36" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="D1016" s="34" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="E1016" s="29" t="s">
         <v>22</v>
@@ -34255,7 +34235,7 @@
         <v>1215</v>
       </c>
       <c r="C1017" s="20" t="s">
-        <v>2369</v>
+        <v>2367</v>
       </c>
       <c r="D1017" s="29"/>
       <c r="E1017" s="29" t="s">
@@ -34280,7 +34260,7 @@
         <v>1215</v>
       </c>
       <c r="C1018" s="20" t="s">
-        <v>2370</v>
+        <v>2368</v>
       </c>
       <c r="D1018" s="29"/>
       <c r="E1018" s="29" t="s">
@@ -34305,7 +34285,7 @@
         <v>1215</v>
       </c>
       <c r="C1019" s="20" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="D1019" s="29"/>
       <c r="E1019" s="29" t="s">
@@ -34332,7 +34312,7 @@
         <v>1215</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2372</v>
+        <v>2370</v>
       </c>
       <c r="D1020" s="29"/>
       <c r="E1020" s="29" t="s">
@@ -34357,7 +34337,7 @@
         <v>1215</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="D1021" s="29" t="s">
         <v>2138</v>
@@ -34384,7 +34364,7 @@
         <v>1215</v>
       </c>
       <c r="C1022" s="20" t="s">
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="D1022" s="29"/>
       <c r="E1022" s="29" t="s">
@@ -34409,7 +34389,7 @@
         <v>1215</v>
       </c>
       <c r="C1023" s="20" t="s">
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="D1023" s="29"/>
       <c r="E1023" s="29" t="s">
@@ -34434,7 +34414,7 @@
         <v>1215</v>
       </c>
       <c r="C1024" s="20" t="s">
-        <v>2376</v>
+        <v>2374</v>
       </c>
       <c r="D1024" s="29" t="s">
         <v>2139</v>
@@ -34492,7 +34472,7 @@
         <v>1215</v>
       </c>
       <c r="C1026" s="20" t="s">
-        <v>2377</v>
+        <v>2375</v>
       </c>
       <c r="D1026" s="29" t="s">
         <v>2140</v>
@@ -34550,7 +34530,7 @@
         <v>1215</v>
       </c>
       <c r="C1028" s="20" t="s">
-        <v>2378</v>
+        <v>2376</v>
       </c>
       <c r="D1028" s="29" t="s">
         <v>2141</v>
@@ -34608,7 +34588,7 @@
         <v>1215</v>
       </c>
       <c r="C1030" s="20" t="s">
-        <v>2379</v>
+        <v>2377</v>
       </c>
       <c r="D1030" s="29" t="s">
         <v>2142</v>
@@ -34666,7 +34646,7 @@
         <v>1215</v>
       </c>
       <c r="C1032" s="20" t="s">
-        <v>2380</v>
+        <v>2378</v>
       </c>
       <c r="D1032" s="29" t="s">
         <v>2143</v>
@@ -34695,7 +34675,7 @@
         <v>1215</v>
       </c>
       <c r="C1033" s="20" t="s">
-        <v>2381</v>
+        <v>2379</v>
       </c>
       <c r="D1033" s="29" t="s">
         <v>2143</v>
@@ -34724,7 +34704,7 @@
         <v>1215</v>
       </c>
       <c r="C1034" s="20" t="s">
-        <v>2382</v>
+        <v>2380</v>
       </c>
       <c r="D1034" s="29" t="s">
         <v>2144</v>
@@ -34805,7 +34785,7 @@
         <v>1215</v>
       </c>
       <c r="C1037" s="20" t="s">
-        <v>2415</v>
+        <v>2413</v>
       </c>
       <c r="D1037" s="29" t="s">
         <v>2233</v>
@@ -34834,7 +34814,7 @@
         <v>1215</v>
       </c>
       <c r="C1038" s="20" t="s">
-        <v>2414</v>
+        <v>2412</v>
       </c>
       <c r="D1038" s="29" t="s">
         <v>2233</v>
@@ -34863,7 +34843,7 @@
         <v>1215</v>
       </c>
       <c r="C1039" s="20" t="s">
-        <v>2384</v>
+        <v>2382</v>
       </c>
       <c r="D1039" s="29" t="s">
         <v>2145</v>
@@ -34921,7 +34901,7 @@
         <v>1215</v>
       </c>
       <c r="C1041" s="20" t="s">
-        <v>2421</v>
+        <v>2415</v>
       </c>
       <c r="D1041" s="29" t="s">
         <v>2235</v>
@@ -34950,7 +34930,7 @@
         <v>1215</v>
       </c>
       <c r="C1042" s="20" t="s">
-        <v>2416</v>
+        <v>2414</v>
       </c>
       <c r="D1042" s="29" t="s">
         <v>2235</v>
@@ -34979,7 +34959,7 @@
         <v>1215</v>
       </c>
       <c r="C1043" s="20" t="s">
-        <v>2388</v>
+        <v>2386</v>
       </c>
       <c r="D1043" s="29" t="s">
         <v>2236</v>
@@ -35035,7 +35015,7 @@
         <v>1215</v>
       </c>
       <c r="C1045" s="20" t="s">
-        <v>2385</v>
+        <v>2383</v>
       </c>
       <c r="D1045" s="29" t="s">
         <v>2146</v>
@@ -35089,7 +35069,7 @@
         <v>1215</v>
       </c>
       <c r="C1047" s="20" t="s">
-        <v>2390</v>
+        <v>2388</v>
       </c>
       <c r="D1047" s="29" t="s">
         <v>2240</v>
@@ -35116,7 +35096,7 @@
         <v>1215</v>
       </c>
       <c r="C1048" s="20" t="s">
-        <v>2391</v>
+        <v>2389</v>
       </c>
       <c r="D1048" s="29" t="s">
         <v>2147</v>
@@ -35143,7 +35123,7 @@
         <v>1215</v>
       </c>
       <c r="C1049" s="20" t="s">
-        <v>2392</v>
+        <v>2390</v>
       </c>
       <c r="D1049" s="29" t="s">
         <v>2147</v>
@@ -35172,7 +35152,7 @@
         <v>1215</v>
       </c>
       <c r="C1050" s="20" t="s">
-        <v>2393</v>
+        <v>2391</v>
       </c>
       <c r="D1050" s="22" t="s">
         <v>2147</v>
@@ -35201,7 +35181,7 @@
         <v>1215</v>
       </c>
       <c r="C1051" s="20" t="s">
-        <v>2394</v>
+        <v>2392</v>
       </c>
       <c r="D1051" s="29" t="s">
         <v>2148</v>
@@ -35230,7 +35210,7 @@
         <v>1215</v>
       </c>
       <c r="C1052" s="20" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="D1052" s="29" t="s">
         <v>2148</v>
@@ -35253,13 +35233,13 @@
     </row>
     <row r="1053" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1053" s="29" t="s">
-        <v>2407</v>
+        <v>2405</v>
       </c>
       <c r="B1053" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1053" s="20" t="s">
-        <v>2406</v>
+        <v>2404</v>
       </c>
       <c r="D1053" s="29" t="s">
         <v>2148</v>
@@ -35473,7 +35453,7 @@
         <v>1215</v>
       </c>
       <c r="C1061" s="20" t="s">
-        <v>2395</v>
+        <v>2393</v>
       </c>
       <c r="D1061" s="22" t="s">
         <v>2151</v>
@@ -35496,13 +35476,13 @@
     </row>
     <row r="1062" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1062" s="22" t="s">
-        <v>2397</v>
+        <v>2395</v>
       </c>
       <c r="B1062" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1062" s="20" t="s">
-        <v>2396</v>
+        <v>2394</v>
       </c>
       <c r="D1062" s="22" t="s">
         <v>2151</v>
@@ -36278,7 +36258,7 @@
         <v>1215</v>
       </c>
       <c r="C1090" s="20" t="s">
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="D1090" s="29" t="s">
         <v>2281</v>
@@ -36307,7 +36287,7 @@
         <v>1215</v>
       </c>
       <c r="C1091" s="20" t="s">
-        <v>2399</v>
+        <v>2397</v>
       </c>
       <c r="D1091" s="29" t="s">
         <v>2281</v>
@@ -36336,7 +36316,7 @@
         <v>1215</v>
       </c>
       <c r="C1092" s="20" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
       <c r="D1092" s="29" t="s">
         <v>2163</v>
@@ -36394,7 +36374,7 @@
         <v>1215</v>
       </c>
       <c r="C1094" s="20" t="s">
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="D1094" s="29" t="s">
         <v>2164</v>
@@ -36452,7 +36432,7 @@
         <v>1215</v>
       </c>
       <c r="C1096" s="20" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="D1096" s="29" t="s">
         <v>2166</v>
@@ -36481,7 +36461,7 @@
         <v>1215</v>
       </c>
       <c r="C1097" s="20" t="s">
-        <v>2410</v>
+        <v>2408</v>
       </c>
       <c r="D1097" s="29" t="s">
         <v>2278</v>
@@ -36510,7 +36490,7 @@
         <v>1215</v>
       </c>
       <c r="C1098" s="20" t="s">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="D1098" s="22" t="s">
         <v>2278</v>
@@ -36803,6 +36783,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36810,11 +36795,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1103:I1108 A20:I1101">
@@ -36933,6 +36913,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -36981,32 +36976,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37026,9 +36999,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MAPI: MS-OXCSTOR update rs
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1112</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpBE30" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="tmpBE30" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-rexu\AppData\Local\Temp\tmpBE30.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7882" uniqueCount="2417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7918" uniqueCount="2425">
   <si>
     <t>Req ID</t>
   </si>
@@ -7127,9 +7127,6 @@
     <t>[In Appendix A: Product Behavior]  Implementation returns the Folder ID of all of the following folders in this field [FolderIds in RopLogon ROP Success Response Buffer for Public Folders]: Public Folders Root Folder (All other folders listed here are direct or indirect children of this folder), Interpersonal messages subtree, Non-interpersonal messages subtree, EForms Registry, Free/Busy Data, Offline address book Data, EForms Registry for the user's locale, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, NNTP Article Index, Empty, Empty, Empty. (Exchange 2003, Exchange 2007 and Exchange 2010 follow this behavior)</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>[In RopLogon ROP Request Buffer] [OpenFlags] The description of flag NO_MAIL: This flag is ignored.&lt;4&gt;</t>
   </si>
   <si>
@@ -7451,9 +7448,6 @@
     <t>[In Appendix A: Product Behavior] Implementation's maximum value of MaxDataSize is 4096. (If MaxDataSize &gt; [server's suitable maximum (4096)], then Implementation does adjust the value of MaxDataSize to the suitable maximum value (4096) in Microsoft Exchanges. &lt;47&gt; Section 3.2.5.12.1: Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013 and Exchange 2016 use 4096 for the maximum value.)</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] If the data is not properly formed, the implementation does fail with a ReturnValue of 0x8004011B.(Exchange 2013 and above follow this behavior.)</t>
-  </si>
-  <si>
     <t>Verified by derived requirements: MS-OXCSTOR_R193, MS-OXCSTOR_R1268001.</t>
   </si>
   <si>
@@ -7467,12 +7461,6 @@
   </si>
   <si>
     <t xml:space="preserve">Verified by derived requirement: MS-OXCSTOR_R1329, MS-OXCSTOR_R3102001. </t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] If the data is not properly formed, the implementation does fail with a ReturnValue of 0x000004ED. &lt;48&gt; Section 3.2.5.13.1:  Exchange 2007 and Exchange 2010 fail the operation with 0x000004ED (ecFmtError) if the data is not properly formed. ((Exchange 2007 and Exchange 2010 follow this behavior.))</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXCSTOR_R1021001, MS-OXCSTOR_R1021002.</t>
   </si>
   <si>
     <t>[In Behavior Common to Both Private Mailbox and Public Folder Logon] The error code ecCorruptData: The data cumulatively written could not be parsed as a proper serialized IDSET with REPLGUIDs, as specified in [MS-OXCFXICS] section 2.2.2.4.2.</t>
@@ -7499,12 +7487,48 @@
   <si>
     <t>[In Read/Write Properties] The PidTagDisplayName property is read/write.&lt;16&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If the data is not properly formed, the implementation does fail with a ReturnValue of 0x000004ED. &lt;48&gt; Section 3.2.5.13.1: If the data is not properly formed, Exchange 2007 fails the operation with 0x000004ED (ecFmtError)  ((Exchange 2007 follows this behavior.))</t>
+  </si>
+  <si>
+    <t>MS-OXCSTOR_R1021003</t>
+  </si>
+  <si>
+    <t>MS-OXCSTOR_R1021004</t>
+  </si>
+  <si>
+    <t>MS-OXCSTOR_R1021005</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If the data is not properly formed, the implementation does fail with a ReturnValue of 0x8004011B. (Exchange 2016 follows this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-OXCSTOR_R1021006</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior]  For public folder logon, if the data is not properly formed,  the implementation does fail with a ReturnValue of 0x000004ED. &lt;48&gt; Section 3.2.5.13.1: For public folder logon, Exchange 2010 fails the operation with 0x000004ED. (Exchange 2010 follows this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] For public folder logon, if the data is not properly formed,  the implementation does fail with a ReturnValue of 0x8004011B. &lt;48&gt; Section 3.2.5.13.1: For public folder logon, Exchange 2013 fails the operation with 0x8004011B. (Exchange 2013 follows this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] For private mailbox logon, if the data is not properly formed, the implementation does returns 0x00000000. &lt;48&gt; Section 3.2.5.13.1: For private mailbox logon, Exchange 2013 returns 0x00000000. (Exchange 2013 follows this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] For private mailbox logon, if the data is not properly formed, the implementation does fail with a ReturnValue of 0x80070057. &lt;48&gt; Section 3.2.5.13.1: For private mailbox logon, Exchange 2010 fails the operation with 0x80070057. (Exchange 2010 follows this behavior.)</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCSTOR_R1021001, MS-OXCSTOR_R1021002,MS-OXCSTOR_R1021003,MS-OXCSTOR_R1021004,MS-OXCSTOR_R1021005,MS-OXCSTOR_R1021006.</t>
+  </si>
+  <si>
+    <t>21.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7559,6 +7583,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -7788,21 +7813,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7827,11 +7837,144 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8170,124 +8313,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8417,34 +8442,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1108" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I1108" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1112" tableType="xml" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" connectionId="1">
+  <autoFilter ref="A19:I1112"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="38">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="37">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="36">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="35">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="34">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="33">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="32">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="31">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="30">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8453,12 +8478,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="24"/>
+    <tableColumn id="2" name="Test" dataDxfId="23"/>
+    <tableColumn id="3" name="Description" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8540,23 +8565,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8592,23 +8600,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8784,9 +8775,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L1110"/>
+  <dimension ref="A1:L1114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -8831,138 +8822,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>2294</v>
+        <v>2424</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>43021</v>
+        <v>43081</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8975,12 +8966,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8993,12 +8984,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9011,12 +9002,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9029,60 +9020,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -10201,7 +10192,7 @@
         <v>1109</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -10217,7 +10208,7 @@
         <v>17</v>
       </c>
       <c r="I63" s="20" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="30">
@@ -10253,7 +10244,7 @@
         <v>1109</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -10357,7 +10348,7 @@
         <v>1109</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -11513,7 +11504,7 @@
         <v>1111</v>
       </c>
       <c r="C115" s="20" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -11717,7 +11708,7 @@
         <v>1112</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -11919,7 +11910,7 @@
         <v>1112</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -13546,7 +13537,7 @@
         <v>1122</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -13596,7 +13587,7 @@
         <v>1122</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -13846,7 +13837,7 @@
         <v>1122</v>
       </c>
       <c r="C208" s="20" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -13921,7 +13912,7 @@
         <v>1124</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="D211" s="29"/>
       <c r="E211" s="29" t="s">
@@ -14348,7 +14339,7 @@
         <v>1129</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -14725,7 +14716,7 @@
         <v>1132</v>
       </c>
       <c r="C243" s="20" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="29" t="s">
@@ -14741,7 +14732,7 @@
         <v>17</v>
       </c>
       <c r="I243" s="20" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="244" spans="1:9" ht="30">
@@ -18401,7 +18392,7 @@
         <v>1161</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="D389" s="29"/>
       <c r="E389" s="29" t="s">
@@ -18775,7 +18766,7 @@
         <v>1162</v>
       </c>
       <c r="C403" s="20" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="D403" s="29"/>
       <c r="E403" s="29" t="s">
@@ -18850,7 +18841,7 @@
         <v>1163</v>
       </c>
       <c r="C406" s="20" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="D406" s="29"/>
       <c r="E406" s="29" t="s">
@@ -18925,7 +18916,7 @@
         <v>1164</v>
       </c>
       <c r="C409" s="20" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -19000,7 +18991,7 @@
         <v>1165</v>
       </c>
       <c r="C412" s="20" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="D412" s="29"/>
       <c r="E412" s="29" t="s">
@@ -19075,7 +19066,7 @@
         <v>1166</v>
       </c>
       <c r="C415" s="20" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="D415" s="29"/>
       <c r="E415" s="29" t="s">
@@ -19150,7 +19141,7 @@
         <v>1167</v>
       </c>
       <c r="C418" s="20" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="D418" s="29"/>
       <c r="E418" s="29" t="s">
@@ -19200,7 +19191,7 @@
         <v>1168</v>
       </c>
       <c r="C420" s="20" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="D420" s="29"/>
       <c r="E420" s="29" t="s">
@@ -19250,7 +19241,7 @@
         <v>1169</v>
       </c>
       <c r="C422" s="20" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="D422" s="29"/>
       <c r="E422" s="29" t="s">
@@ -19300,7 +19291,7 @@
         <v>1170</v>
       </c>
       <c r="C424" s="20" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="D424" s="29"/>
       <c r="E424" s="29" t="s">
@@ -19375,7 +19366,7 @@
         <v>1171</v>
       </c>
       <c r="C427" s="20" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="D427" s="29"/>
       <c r="E427" s="29" t="s">
@@ -19425,7 +19416,7 @@
         <v>1172</v>
       </c>
       <c r="C429" s="20" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="D429" s="29"/>
       <c r="E429" s="29" t="s">
@@ -19475,7 +19466,7 @@
         <v>1173</v>
       </c>
       <c r="C431" s="20" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="D431" s="29"/>
       <c r="E431" s="29" t="s">
@@ -19494,13 +19485,13 @@
     </row>
     <row r="432" spans="1:9" ht="30">
       <c r="A432" s="22" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="B432" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C432" s="36" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D432" s="34"/>
       <c r="E432" s="29" t="s">
@@ -19519,13 +19510,13 @@
     </row>
     <row r="433" spans="1:9" ht="45">
       <c r="A433" s="22" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="B433" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C433" s="36" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="D433" s="34"/>
       <c r="E433" s="29" t="s">
@@ -19544,13 +19535,13 @@
     </row>
     <row r="434" spans="1:9" ht="75">
       <c r="A434" s="22" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="B434" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C434" s="36" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="D434" s="34"/>
       <c r="E434" s="29" t="s">
@@ -19569,13 +19560,13 @@
     </row>
     <row r="435" spans="1:9" ht="45">
       <c r="A435" s="22" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="B435" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C435" s="36" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="D435" s="34"/>
       <c r="E435" s="29" t="s">
@@ -19594,13 +19585,13 @@
     </row>
     <row r="436" spans="1:9" ht="45">
       <c r="A436" s="22" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="B436" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C436" s="36" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="D436" s="34"/>
       <c r="E436" s="34" t="s">
@@ -19619,13 +19610,13 @@
     </row>
     <row r="437" spans="1:9" ht="30">
       <c r="A437" s="22" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="B437" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C437" s="36" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="D437" s="34"/>
       <c r="E437" s="34" t="s">
@@ -19644,13 +19635,13 @@
     </row>
     <row r="438" spans="1:9" ht="30">
       <c r="A438" s="22" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="B438" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C438" s="36" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="D438" s="34"/>
       <c r="E438" s="29" t="s">
@@ -19700,7 +19691,7 @@
         <v>1175</v>
       </c>
       <c r="C440" s="20" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D440" s="29"/>
       <c r="E440" s="29" t="s">
@@ -19747,7 +19738,7 @@
         <v>456</v>
       </c>
       <c r="B442" s="24" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="C442" s="31" t="s">
         <v>1605</v>
@@ -19772,10 +19763,10 @@
         <v>457</v>
       </c>
       <c r="B443" s="24" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C443" s="20" t="s">
         <v>2341</v>
-      </c>
-      <c r="C443" s="20" t="s">
-        <v>2342</v>
       </c>
       <c r="D443" s="29"/>
       <c r="E443" s="29" t="s">
@@ -19800,7 +19791,7 @@
         <v>1176</v>
       </c>
       <c r="C444" s="20" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="D444" s="29"/>
       <c r="E444" s="29" t="s">
@@ -19825,7 +19816,7 @@
         <v>1176</v>
       </c>
       <c r="C445" s="20" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="D445" s="29" t="s">
         <v>2132</v>
@@ -19881,7 +19872,7 @@
         <v>1176</v>
       </c>
       <c r="C447" s="20" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="D447" s="29"/>
       <c r="E447" s="29" t="s">
@@ -19908,7 +19899,7 @@
         <v>1176</v>
       </c>
       <c r="C448" s="20" t="s">
-        <v>2416</v>
+        <v>2412</v>
       </c>
       <c r="D448" s="29" t="s">
         <v>2132</v>
@@ -20068,7 +20059,7 @@
         <v>1177</v>
       </c>
       <c r="C454" s="20" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="D454" s="29"/>
       <c r="E454" s="29" t="s">
@@ -20118,7 +20109,7 @@
         <v>1178</v>
       </c>
       <c r="C456" s="20" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29" t="s">
@@ -20268,7 +20259,7 @@
         <v>1180</v>
       </c>
       <c r="C462" s="20" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="D462" s="29"/>
       <c r="E462" s="29" t="s">
@@ -20393,7 +20384,7 @@
         <v>1181</v>
       </c>
       <c r="C467" s="20" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="D467" s="29"/>
       <c r="E467" s="29" t="s">
@@ -20599,7 +20590,7 @@
         <v>1183</v>
       </c>
       <c r="C475" s="20" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="D475" s="29"/>
       <c r="E475" s="29" t="s">
@@ -20674,7 +20665,7 @@
         <v>1184</v>
       </c>
       <c r="C478" s="20" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29" t="s">
@@ -20899,7 +20890,7 @@
         <v>32</v>
       </c>
       <c r="C487" s="20" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="D487" s="29"/>
       <c r="E487" s="29" t="s">
@@ -23474,7 +23465,7 @@
         <v>1191</v>
       </c>
       <c r="C590" s="20" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="D590" s="29"/>
       <c r="E590" s="29" t="s">
@@ -23574,7 +23565,7 @@
         <v>1192</v>
       </c>
       <c r="C594" s="20" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="D594" s="29"/>
       <c r="E594" s="29" t="s">
@@ -23590,7 +23581,7 @@
         <v>17</v>
       </c>
       <c r="I594" s="20" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="595" spans="1:9" ht="30">
@@ -23751,7 +23742,7 @@
         <v>1194</v>
       </c>
       <c r="C601" s="20" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="D601" s="29"/>
       <c r="E601" s="29" t="s">
@@ -23803,7 +23794,7 @@
         <v>1194</v>
       </c>
       <c r="C603" s="20" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="D603" s="29"/>
       <c r="E603" s="29" t="s">
@@ -23819,7 +23810,7 @@
         <v>17</v>
       </c>
       <c r="I603" s="20" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="604" spans="1:9" ht="45">
@@ -23907,7 +23898,7 @@
         <v>1194</v>
       </c>
       <c r="C607" s="20" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="D607" s="29"/>
       <c r="E607" s="29" t="s">
@@ -23923,7 +23914,7 @@
         <v>17</v>
       </c>
       <c r="I607" s="20" t="s">
-        <v>2407</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="608" spans="1:9" ht="45">
@@ -23934,7 +23925,7 @@
         <v>1194</v>
       </c>
       <c r="C608" s="20" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="D608" s="29"/>
       <c r="E608" s="29" t="s">
@@ -24077,7 +24068,7 @@
         <v>17</v>
       </c>
       <c r="I613" s="20" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="614" spans="1:9" ht="75">
@@ -26902,7 +26893,7 @@
         <v>1198</v>
       </c>
       <c r="C726" s="20" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="D726" s="29"/>
       <c r="E726" s="29" t="s">
@@ -26952,7 +26943,7 @@
         <v>1198</v>
       </c>
       <c r="C728" s="20" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="D728" s="29"/>
       <c r="E728" s="29" t="s">
@@ -26977,7 +26968,7 @@
         <v>1198</v>
       </c>
       <c r="C729" s="20" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="D729" s="29"/>
       <c r="E729" s="29" t="s">
@@ -30916,7 +30907,7 @@
         <v>1204</v>
       </c>
       <c r="C886" s="20" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="D886" s="29"/>
       <c r="E886" s="29" t="s">
@@ -31716,7 +31707,7 @@
         <v>1208</v>
       </c>
       <c r="C918" s="20" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="D918" s="29"/>
       <c r="E918" s="29" t="s">
@@ -32116,7 +32107,7 @@
         <v>1208</v>
       </c>
       <c r="C934" s="20" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="D934" s="29"/>
       <c r="E934" s="29" t="s">
@@ -32293,7 +32284,7 @@
         <v>1208</v>
       </c>
       <c r="C941" s="20" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="D941" s="29"/>
       <c r="E941" s="29" t="s">
@@ -32347,7 +32338,7 @@
         <v>1208</v>
       </c>
       <c r="C943" s="20" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="D943" s="29"/>
       <c r="E943" s="29" t="s">
@@ -33366,7 +33357,7 @@
       </c>
       <c r="I983" s="31"/>
     </row>
-    <row r="984" spans="1:9" ht="60">
+    <row r="984" spans="1:9" ht="120">
       <c r="A984" s="29" t="s">
         <v>996</v>
       </c>
@@ -33374,7 +33365,7 @@
         <v>1212</v>
       </c>
       <c r="C984" s="20" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="D984" s="29"/>
       <c r="E984" s="29" t="s">
@@ -33390,7 +33381,7 @@
         <v>17</v>
       </c>
       <c r="I984" s="20" t="s">
-        <v>2409</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="985" spans="1:9" ht="60">
@@ -33426,7 +33417,7 @@
         <v>1212</v>
       </c>
       <c r="C986" s="20" t="s">
-        <v>2411</v>
+        <v>2407</v>
       </c>
       <c r="D986" s="29"/>
       <c r="E986" s="29" t="s">
@@ -33601,7 +33592,7 @@
         <v>1212</v>
       </c>
       <c r="C993" s="20" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="D993" s="29"/>
       <c r="E993" s="29" t="s">
@@ -33626,7 +33617,7 @@
         <v>1212</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2410</v>
+        <v>2406</v>
       </c>
       <c r="D994" s="29"/>
       <c r="E994" s="29" t="s">
@@ -34165,16 +34156,16 @@
     </row>
     <row r="1015" spans="1:9" ht="60">
       <c r="A1015" s="34" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="B1015" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1015" s="36" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D1015" s="34" t="s">
         <v>2301</v>
-      </c>
-      <c r="D1015" s="34" t="s">
-        <v>2302</v>
       </c>
       <c r="E1015" s="29" t="s">
         <v>22</v>
@@ -34192,16 +34183,16 @@
     </row>
     <row r="1016" spans="1:9" ht="45">
       <c r="A1016" s="34" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="B1016" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1016" s="36" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="D1016" s="34" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="E1016" s="29" t="s">
         <v>22</v>
@@ -34225,7 +34216,7 @@
         <v>1215</v>
       </c>
       <c r="C1017" s="20" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="D1017" s="29"/>
       <c r="E1017" s="29" t="s">
@@ -34250,7 +34241,7 @@
         <v>1215</v>
       </c>
       <c r="C1018" s="20" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="D1018" s="29"/>
       <c r="E1018" s="29" t="s">
@@ -34275,7 +34266,7 @@
         <v>1215</v>
       </c>
       <c r="C1019" s="20" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="D1019" s="29"/>
       <c r="E1019" s="29" t="s">
@@ -34302,7 +34293,7 @@
         <v>1215</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="D1020" s="29"/>
       <c r="E1020" s="29" t="s">
@@ -34327,7 +34318,7 @@
         <v>1215</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="D1021" s="29" t="s">
         <v>2138</v>
@@ -34354,7 +34345,7 @@
         <v>1215</v>
       </c>
       <c r="C1022" s="20" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="D1022" s="29"/>
       <c r="E1022" s="29" t="s">
@@ -34379,7 +34370,7 @@
         <v>1215</v>
       </c>
       <c r="C1023" s="20" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="D1023" s="29"/>
       <c r="E1023" s="29" t="s">
@@ -34404,7 +34395,7 @@
         <v>1215</v>
       </c>
       <c r="C1024" s="20" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="D1024" s="29" t="s">
         <v>2139</v>
@@ -34462,7 +34453,7 @@
         <v>1215</v>
       </c>
       <c r="C1026" s="20" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="D1026" s="29" t="s">
         <v>2140</v>
@@ -34520,7 +34511,7 @@
         <v>1215</v>
       </c>
       <c r="C1028" s="20" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="D1028" s="29" t="s">
         <v>2141</v>
@@ -34578,7 +34569,7 @@
         <v>1215</v>
       </c>
       <c r="C1030" s="20" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="D1030" s="29" t="s">
         <v>2142</v>
@@ -34636,7 +34627,7 @@
         <v>1215</v>
       </c>
       <c r="C1032" s="20" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="D1032" s="29" t="s">
         <v>2143</v>
@@ -34665,7 +34656,7 @@
         <v>1215</v>
       </c>
       <c r="C1033" s="20" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="D1033" s="29" t="s">
         <v>2143</v>
@@ -34694,7 +34685,7 @@
         <v>1215</v>
       </c>
       <c r="C1034" s="20" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="D1034" s="29" t="s">
         <v>2144</v>
@@ -34775,7 +34766,7 @@
         <v>1215</v>
       </c>
       <c r="C1037" s="20" t="s">
-        <v>2413</v>
+        <v>2409</v>
       </c>
       <c r="D1037" s="29" t="s">
         <v>2233</v>
@@ -34804,7 +34795,7 @@
         <v>1215</v>
       </c>
       <c r="C1038" s="20" t="s">
-        <v>2412</v>
+        <v>2408</v>
       </c>
       <c r="D1038" s="29" t="s">
         <v>2233</v>
@@ -34833,7 +34824,7 @@
         <v>1215</v>
       </c>
       <c r="C1039" s="20" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="D1039" s="29" t="s">
         <v>2145</v>
@@ -34891,7 +34882,7 @@
         <v>1215</v>
       </c>
       <c r="C1041" s="20" t="s">
-        <v>2415</v>
+        <v>2411</v>
       </c>
       <c r="D1041" s="29" t="s">
         <v>2235</v>
@@ -34920,7 +34911,7 @@
         <v>1215</v>
       </c>
       <c r="C1042" s="20" t="s">
-        <v>2414</v>
+        <v>2410</v>
       </c>
       <c r="D1042" s="29" t="s">
         <v>2235</v>
@@ -34949,7 +34940,7 @@
         <v>1215</v>
       </c>
       <c r="C1043" s="20" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="D1043" s="29" t="s">
         <v>2236</v>
@@ -35005,7 +34996,7 @@
         <v>1215</v>
       </c>
       <c r="C1045" s="20" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="D1045" s="29" t="s">
         <v>2146</v>
@@ -35059,7 +35050,7 @@
         <v>1215</v>
       </c>
       <c r="C1047" s="20" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="D1047" s="29" t="s">
         <v>2240</v>
@@ -35086,7 +35077,7 @@
         <v>1215</v>
       </c>
       <c r="C1048" s="20" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="D1048" s="29" t="s">
         <v>2147</v>
@@ -35113,7 +35104,7 @@
         <v>1215</v>
       </c>
       <c r="C1049" s="20" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="D1049" s="29" t="s">
         <v>2147</v>
@@ -35142,7 +35133,7 @@
         <v>1215</v>
       </c>
       <c r="C1050" s="20" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="D1050" s="22" t="s">
         <v>2147</v>
@@ -35171,7 +35162,7 @@
         <v>1215</v>
       </c>
       <c r="C1051" s="20" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="D1051" s="29" t="s">
         <v>2148</v>
@@ -35200,7 +35191,7 @@
         <v>1215</v>
       </c>
       <c r="C1052" s="20" t="s">
-        <v>2406</v>
+        <v>2404</v>
       </c>
       <c r="D1052" s="29" t="s">
         <v>2148</v>
@@ -35223,13 +35214,13 @@
     </row>
     <row r="1053" spans="1:9" ht="45">
       <c r="A1053" s="29" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
       <c r="B1053" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1053" s="20" t="s">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="D1053" s="29" t="s">
         <v>2148</v>
@@ -35443,7 +35434,7 @@
         <v>1215</v>
       </c>
       <c r="C1061" s="20" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="D1061" s="22" t="s">
         <v>2151</v>
@@ -35466,13 +35457,13 @@
     </row>
     <row r="1062" spans="1:9" ht="90">
       <c r="A1062" s="22" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="B1062" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1062" s="20" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="D1062" s="22" t="s">
         <v>2151</v>
@@ -36248,7 +36239,7 @@
         <v>1215</v>
       </c>
       <c r="C1090" s="20" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D1090" s="29" t="s">
         <v>2281</v>
@@ -36277,7 +36268,7 @@
         <v>1215</v>
       </c>
       <c r="C1091" s="20" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="D1091" s="29" t="s">
         <v>2281</v>
@@ -36306,7 +36297,7 @@
         <v>1215</v>
       </c>
       <c r="C1092" s="20" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="D1092" s="29" t="s">
         <v>2163</v>
@@ -36364,7 +36355,7 @@
         <v>1215</v>
       </c>
       <c r="C1094" s="20" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="D1094" s="29" t="s">
         <v>2164</v>
@@ -36422,7 +36413,7 @@
         <v>1215</v>
       </c>
       <c r="C1096" s="20" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="D1096" s="29" t="s">
         <v>2166</v>
@@ -36451,7 +36442,7 @@
         <v>1215</v>
       </c>
       <c r="C1097" s="20" t="s">
-        <v>2408</v>
+        <v>2413</v>
       </c>
       <c r="D1097" s="29" t="s">
         <v>2278</v>
@@ -36472,7 +36463,7 @@
         <v>2195</v>
       </c>
     </row>
-    <row r="1098" spans="1:9" ht="45">
+    <row r="1098" spans="1:9" ht="60">
       <c r="A1098" s="22" t="s">
         <v>2277</v>
       </c>
@@ -36480,7 +36471,7 @@
         <v>1215</v>
       </c>
       <c r="C1098" s="20" t="s">
-        <v>2402</v>
+        <v>2420</v>
       </c>
       <c r="D1098" s="22" t="s">
         <v>2278</v>
@@ -36501,184 +36492,196 @@
         <v>2195</v>
       </c>
     </row>
-    <row r="1099" spans="1:9" ht="45">
-      <c r="A1099" s="29" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B1099" s="30" t="s">
+    <row r="1099" spans="1:9" ht="60">
+      <c r="A1099" s="22" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B1099" s="24" t="s">
         <v>1215</v>
       </c>
-      <c r="C1099" s="31" t="s">
-        <v>2121</v>
+      <c r="C1099" s="20" t="s">
+        <v>2419</v>
       </c>
       <c r="D1099" s="29" t="s">
-        <v>2167</v>
+        <v>2278</v>
       </c>
       <c r="E1099" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F1099" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1099" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H1099" s="29" t="s">
+      <c r="H1099" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I1099" s="31" t="s">
         <v>2195</v>
       </c>
     </row>
-    <row r="1100" spans="1:9" ht="60">
-      <c r="A1100" s="29" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B1100" s="30" t="s">
+    <row r="1100" spans="1:9" ht="45">
+      <c r="A1100" s="22" t="s">
+        <v>2415</v>
+      </c>
+      <c r="B1100" s="24" t="s">
         <v>1215</v>
       </c>
-      <c r="C1100" s="31" t="s">
-        <v>2122</v>
+      <c r="C1100" s="20" t="s">
+        <v>2421</v>
       </c>
       <c r="D1100" s="29" t="s">
-        <v>2168</v>
+        <v>2278</v>
       </c>
       <c r="E1100" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F1100" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1100" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H1100" s="29" t="s">
+      <c r="H1100" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I1100" s="31" t="s">
         <v>2195</v>
       </c>
     </row>
-    <row r="1101" spans="1:9" ht="45">
-      <c r="A1101" s="29" t="s">
-        <v>1097</v>
-      </c>
-      <c r="B1101" s="30" t="s">
+    <row r="1101" spans="1:9" ht="60">
+      <c r="A1101" s="22" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B1101" s="24" t="s">
         <v>1215</v>
       </c>
-      <c r="C1101" s="31" t="s">
-        <v>2123</v>
-      </c>
-      <c r="D1101" s="29"/>
+      <c r="C1101" s="20" t="s">
+        <v>2422</v>
+      </c>
+      <c r="D1101" s="29" t="s">
+        <v>2278</v>
+      </c>
       <c r="E1101" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F1101" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1101" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H1101" s="29" t="s">
-        <v>21</v>
+      <c r="H1101" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="I1101" s="31" t="s">
         <v>2195</v>
       </c>
     </row>
     <row r="1102" spans="1:9" ht="45">
-      <c r="A1102" s="29" t="s">
-        <v>2199</v>
-      </c>
-      <c r="B1102" s="30" t="s">
+      <c r="A1102" s="22" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B1102" s="24" t="s">
         <v>1215</v>
       </c>
-      <c r="C1102" s="31" t="s">
-        <v>2200</v>
-      </c>
-      <c r="D1102" s="29"/>
+      <c r="C1102" s="20" t="s">
+        <v>2417</v>
+      </c>
+      <c r="D1102" s="29" t="s">
+        <v>2278</v>
+      </c>
       <c r="E1102" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F1102" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1102" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H1102" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1102" s="32" t="s">
+      <c r="H1102" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1102" s="31" t="s">
         <v>2195</v>
       </c>
     </row>
-    <row r="1103" spans="1:9" ht="30">
+    <row r="1103" spans="1:9" ht="45">
       <c r="A1103" s="29" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B1103" s="30" t="s">
-        <v>1118</v>
+        <v>1215</v>
       </c>
       <c r="C1103" s="31" t="s">
-        <v>2124</v>
-      </c>
-      <c r="D1103" s="29"/>
+        <v>2121</v>
+      </c>
+      <c r="D1103" s="29" t="s">
+        <v>2167</v>
+      </c>
       <c r="E1103" s="29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1103" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1103" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H1103" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1103" s="31"/>
-    </row>
-    <row r="1104" spans="1:9">
+        <v>20</v>
+      </c>
+      <c r="I1103" s="31" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:9" ht="60">
       <c r="A1104" s="29" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B1104" s="30" t="s">
-        <v>1118</v>
+        <v>1215</v>
       </c>
       <c r="C1104" s="31" t="s">
-        <v>2125</v>
-      </c>
-      <c r="D1104" s="29"/>
+        <v>2122</v>
+      </c>
+      <c r="D1104" s="29" t="s">
+        <v>2168</v>
+      </c>
       <c r="E1104" s="29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1104" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1104" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H1104" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1104" s="31"/>
-    </row>
-    <row r="1105" spans="1:9">
+        <v>20</v>
+      </c>
+      <c r="I1104" s="31" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:9" ht="45">
       <c r="A1105" s="29" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="B1105" s="30" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C1105" s="31" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
       <c r="D1105" s="29"/>
       <c r="E1105" s="29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1105" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1105" s="29" t="s">
         <v>15</v>
@@ -36686,24 +36689,26 @@
       <c r="H1105" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I1105" s="31"/>
-    </row>
-    <row r="1106" spans="1:9" ht="30">
+      <c r="I1105" s="31" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:9" ht="45">
       <c r="A1106" s="29" t="s">
-        <v>1101</v>
+        <v>2199</v>
       </c>
       <c r="B1106" s="30" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C1106" s="31" t="s">
-        <v>2127</v>
+        <v>2200</v>
       </c>
       <c r="D1106" s="29"/>
       <c r="E1106" s="29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1106" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1106" s="29" t="s">
         <v>15</v>
@@ -36711,17 +36716,19 @@
       <c r="H1106" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I1106" s="31"/>
-    </row>
-    <row r="1107" spans="1:9" ht="75">
+      <c r="I1106" s="32" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:9" ht="30">
       <c r="A1107" s="29" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="B1107" s="30" t="s">
-        <v>1216</v>
+        <v>1118</v>
       </c>
       <c r="C1107" s="31" t="s">
-        <v>2128</v>
+        <v>2124</v>
       </c>
       <c r="D1107" s="29"/>
       <c r="E1107" s="29" t="s">
@@ -36738,15 +36745,15 @@
       </c>
       <c r="I1107" s="31"/>
     </row>
-    <row r="1108" spans="1:9" ht="45">
+    <row r="1108" spans="1:9">
       <c r="A1108" s="29" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="B1108" s="30" t="s">
-        <v>1217</v>
+        <v>1118</v>
       </c>
       <c r="C1108" s="31" t="s">
-        <v>2129</v>
+        <v>2125</v>
       </c>
       <c r="D1108" s="29"/>
       <c r="E1108" s="29" t="s">
@@ -36764,15 +36771,120 @@
       <c r="I1108" s="31"/>
     </row>
     <row r="1109" spans="1:9">
-      <c r="A1109" s="3"/>
-      <c r="B1109" s="10"/>
-    </row>
-    <row r="1110" spans="1:9">
-      <c r="A1110" s="3"/>
-      <c r="B1110" s="10"/>
+      <c r="A1109" s="29" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B1109" s="30" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C1109" s="31" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D1109" s="29"/>
+      <c r="E1109" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1109" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1109" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1109" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1109" s="31"/>
+    </row>
+    <row r="1110" spans="1:9" ht="30">
+      <c r="A1110" s="29" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B1110" s="30" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C1110" s="31" t="s">
+        <v>2127</v>
+      </c>
+      <c r="D1110" s="29"/>
+      <c r="E1110" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1110" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1110" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1110" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1110" s="31"/>
+    </row>
+    <row r="1111" spans="1:9" ht="75">
+      <c r="A1111" s="29" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B1111" s="30" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C1111" s="31" t="s">
+        <v>2128</v>
+      </c>
+      <c r="D1111" s="29"/>
+      <c r="E1111" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1111" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1111" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1111" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1111" s="31"/>
+    </row>
+    <row r="1112" spans="1:9" ht="45">
+      <c r="A1112" s="29" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1112" s="30" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C1112" s="31" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D1112" s="29"/>
+      <c r="E1112" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1112" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1112" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1112" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1112" s="31"/>
+    </row>
+    <row r="1113" spans="1:9">
+      <c r="A1113" s="3"/>
+      <c r="B1113" s="10"/>
+    </row>
+    <row r="1114" spans="1:9">
+      <c r="A1114" s="3"/>
+      <c r="B1114" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36780,110 +36892,105 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1103:I1108 A20:I1101">
-    <cfRule type="expression" dxfId="40" priority="67">
+  <conditionalFormatting sqref="A1107:I1112 A20:I1105">
+    <cfRule type="expression" dxfId="21" priority="67">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="68">
+    <cfRule type="expression" dxfId="20" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="75">
+    <cfRule type="expression" dxfId="19" priority="75">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1103:I1108 A20:I1101">
-    <cfRule type="expression" dxfId="37" priority="21">
+  <conditionalFormatting sqref="A1107:I1112 A20:I1105">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="22">
+    <cfRule type="expression" dxfId="17" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="23">
+    <cfRule type="expression" dxfId="16" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1103:F1108 F20:F1101">
-    <cfRule type="expression" dxfId="34" priority="27">
+  <conditionalFormatting sqref="F1107:F1112 F20:F1105">
+    <cfRule type="expression" dxfId="15" priority="27">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="28">
+    <cfRule type="expression" dxfId="14" priority="28">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1103:I1108">
-    <cfRule type="expression" dxfId="32" priority="18">
+  <conditionalFormatting sqref="I1107:I1112">
+    <cfRule type="expression" dxfId="13" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="19">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="20">
+    <cfRule type="expression" dxfId="11" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1103:I1108">
-    <cfRule type="expression" dxfId="29" priority="15">
+  <conditionalFormatting sqref="I1107:I1112">
+    <cfRule type="expression" dxfId="10" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="16">
+    <cfRule type="expression" dxfId="9" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="17">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1102:H1102">
-    <cfRule type="expression" dxfId="26" priority="12">
+  <conditionalFormatting sqref="A1106:H1106">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="13">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="14">
+    <cfRule type="expression" dxfId="5" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1102:H1102">
-    <cfRule type="expression" dxfId="23" priority="7">
+  <conditionalFormatting sqref="A1106:H1106">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1102">
-    <cfRule type="expression" dxfId="20" priority="10">
-      <formula>NOT(VLOOKUP(F1102,$A$12:$C$15,2,FALSE)="In")</formula>
+  <conditionalFormatting sqref="F1106">
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>NOT(VLOOKUP(F1106,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="11">
-      <formula>(VLOOKUP(F1102,$A$12:$C$15,2,FALSE)="In")</formula>
+    <cfRule type="expression" dxfId="0" priority="11">
+      <formula>(VLOOKUP(F1106,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1108" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1112">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1108" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1112">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1108" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1112">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1108" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1112">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -36893,7 +37000,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B431 B444:B1014 B1054:B1061 B1063:B1098 B1099:B1110 B1017:B1052" numberStoredAsText="1"/>
+    <ignoredError sqref="B19:B431 B444:B1014 B1054:B1061 B1063:B1098 B1103:B1114 B1017:B1052" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -36903,18 +37010,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36967,6 +37074,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -36976,14 +37091,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[MS-OXCSTOR] Update capture code and fix case failure on Exchange 2019
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7520A6B4-6162-4AB6-9DB9-DA39DC1926A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmpBE30" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpBE30" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-rexu\AppData\Local\Temp\tmpBE30.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -7531,7 +7532,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7821,6 +7822,27 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7845,150 +7867,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8327,6 +8210,124 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8456,34 +8457,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1113" tableType="xml" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" connectionId="1">
-  <autoFilter ref="A19:I1113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1113" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I1113" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="37">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="36">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="35">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="33">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="32">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="31">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="30">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8492,12 +8493,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="24"/>
-    <tableColumn id="2" name="Test" dataDxfId="23"/>
-    <tableColumn id="3" name="Description" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8579,6 +8580,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8614,6 +8632,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8789,13 +8824,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8849,127 +8882,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8982,12 +9015,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9000,12 +9033,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9018,12 +9051,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9036,60 +9069,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -19131,23 +19164,23 @@
       <c r="B417" s="30" t="s">
         <v>1166</v>
       </c>
-      <c r="C417" s="51" t="s">
+      <c r="C417" s="38" t="s">
         <v>2401</v>
       </c>
-      <c r="D417" s="50"/>
+      <c r="D417" s="37"/>
       <c r="E417" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F417" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G417" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="H417" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="I417" s="51"/>
+      <c r="G417" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H417" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I417" s="38"/>
     </row>
     <row r="418" spans="1:9">
       <c r="A418" s="29" t="s">
@@ -36921,11 +36954,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36933,105 +36961,110 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1108:I1113 A20:I1106">
-    <cfRule type="expression" dxfId="21" priority="67">
+    <cfRule type="expression" dxfId="40" priority="67">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="68">
+    <cfRule type="expression" dxfId="39" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="75">
+    <cfRule type="expression" dxfId="38" priority="75">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1108:I1113 A20:I1106">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1108:F1113 F20:F1106">
-    <cfRule type="expression" dxfId="15" priority="27">
+    <cfRule type="expression" dxfId="34" priority="27">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="28">
+    <cfRule type="expression" dxfId="33" priority="28">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1108:I1113">
-    <cfRule type="expression" dxfId="13" priority="18">
+    <cfRule type="expression" dxfId="32" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="19">
+    <cfRule type="expression" dxfId="31" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20">
+    <cfRule type="expression" dxfId="30" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1108:I1113">
-    <cfRule type="expression" dxfId="10" priority="15">
+    <cfRule type="expression" dxfId="29" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="16">
+    <cfRule type="expression" dxfId="28" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="17">
+    <cfRule type="expression" dxfId="27" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1107:H1107">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="26" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="25" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="14">
+    <cfRule type="expression" dxfId="24" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1107:H1107">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1107">
-    <cfRule type="expression" dxfId="1" priority="10">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>NOT(VLOOKUP(F1107,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="11">
+    <cfRule type="expression" dxfId="19" priority="11">
       <formula>(VLOOKUP(F1107,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1113" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1113" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1113" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1113">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1113" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -37051,18 +37084,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37115,14 +37148,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -37132,6 +37157,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
MS-OXCFOLD, MS-OXCMSG,MS-OXCSTOR: update RS
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCSTOR/MS-OXCSTOR_RequirementSpecification.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7520A6B4-6162-4AB6-9DB9-DA39DC1926A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -21,8 +20,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpBE30" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="tmpBE30" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-rexu\AppData\Local\Temp\tmpBE30.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -7116,24 +7115,12 @@
     <t>[In RopLogon ROP Request Buffer] [OpenFlags] The description of flag SUPPORT_PROGRESS: Indicates that the client supports asynchronous processing of RopSetReadFlags, as specified in [MS-OXCMSG] section 2.2.3.10.1.&lt;6&gt;</t>
   </si>
   <si>
-    <t>[In RopLogon ROP Success Response Buffer for Private Mailbox] StoreState: This field MUST be set to 0x00000000 by the server. &lt;8&gt;</t>
-  </si>
-  <si>
     <t>[In RopLogon ROP Success Response Buffer for Public Folders] FolderIds: This field contains the Folder ID of the following folders: &lt;9&gt; Public Folders Root Folder (All other folders listed here are direct or indirect children of this folder), Interpersonal messages subtree, Non-interpersonal messages subtree, EForms Registry, Free/Busy Data, Offline address book Data, EForms Registry for the user's locale, Local Site's Free/Busy Data, Local Site's Offline Address, Book Data, NNTP Article Index, Empty, Empty, Empty.</t>
   </si>
   <si>
     <t>[In RopLogon ROP Success Response Buffer for Public Folders] PerUserGuid: The server SHOULD set this field to an empty GUID (all zeroes).&lt;10&gt;</t>
   </si>
   <si>
-    <t>[In RopGetReceiveFolderTable ROP Success Response Buffer] 	[Rows] PidTagFolderId property ([MS-OXPROPS] section 2.694): A PtypInteger64 value that specifies the folder ID (FID) ([MS-OXCDATA] section 2.2.1.1) of the Receive folder, which is the folder to which messages of the specified message class will be delivered.</t>
-  </si>
-  <si>
-    <t>[In RopGetReceiveFolderTable ROP Success Response Buffer] [Rows] PidTagMessageClass property ([MS-OXPROPS] section 2.781): A PtypString8 value.</t>
-  </si>
-  <si>
-    <t>[In RopGetReceiveFolderTable ROP Success Response Buffer]  [Rows] PidTagLastModificationTime property: PidTagLastModificationTime property ([MS-OXPROPS] section 2.758) -- A PtypTime value that specifies the time, in Coordinated Universal Time (UTC), when the server created or last modified the row in the Receive folder table.</t>
-  </si>
-  <si>
     <t>[In RopGetStoreState ROP] The RopGetStoreState ROP ([MS-OXCROPS] section 2.2.3.5) is used to obtain state information about the current mailbox.&lt;11&gt;</t>
   </si>
   <si>
@@ -7146,51 +7133,12 @@
     <t>[In Read-Only Properties] The read-only properties that are available on a private mailbox logon are specified in section 2.2.2.1.1.1 through section 2.2.2.1.1.15.</t>
   </si>
   <si>
-    <t>[In PidTagExtendedRuleSizeLimit Property] The PidTagExtendedRuleSizeLimit property ([MS-OXPROPS] section 2.688) contains the Maximum size, in bytes, the user is allowed to accumulate for a single "extended" rule.</t>
-  </si>
-  <si>
-    <t>[In PidTagMaximumSubmitMessageSize Property] The PidTagMaximumSubmitMessageSize property ([MS-OXPROPS] section 2.775) contains the maximum size, in kilobytes, of a message a user is allowed to submit for transmission to another user.</t>
-  </si>
-  <si>
-    <t>[In PidTagProhibitReceiveQuota Property] The PidTagProhibitReceiveQuota property ([MS-OXPROPS] section 2.868) contains the maximum size, in kilobytes, a user is allowed to accumulate in their mailbox, before no further mail will be delivered.</t>
-  </si>
-  <si>
-    <t>[In PidTagProhibitSendQuota Property] The PidTagProhibitSendQuota property ([MS-OXPROPS] section 2.869) contains the maximum size, in kilobytes, a user is allowed to accumulate in their mailbox, before the user can no longer submit any more mail.</t>
-  </si>
-  <si>
-    <t>[In PidTagStoreState Property] The PidTagStoreState property ([MS-OXPROPS] section 2.1023) indicates whether the mailbox has any active search folders.</t>
-  </si>
-  <si>
-    <t>[In PidTagContentCount Property] The PidTagContentCount property ([MS-OXPROPS] section 2.640) contains the cumulative count of non-folder associated information (FAI) messages in the mailbox.</t>
-  </si>
-  <si>
-    <t>[In PidTagMailboxOwnerEntryId Property] The PidTagMailboxOwnerEntryId property ([MS-OXPROPS] section 2.771) contains the EntryID in the Global Address List (GAL) of the owner of the mailbox.</t>
-  </si>
-  <si>
-    <t>[In PidTagMailboxOwnerName Property] The PidTagMailboxOwnerName property ([MS-OXPROPS] section 2.772) contains the display name of the owner of the mailbox.</t>
-  </si>
-  <si>
-    <t>[In PidTagMessageSize Property] The PidTagMessageSize property ([MS-OXPROPS] section 2.790) contains the cumulative size, in bytes, of all content in the mailbox.</t>
-  </si>
-  <si>
-    <t>[In PidTagMessageSizeExtended Property] The PidTagMessageSizeExtended property ([MS-OXPROPS] section 2.791) contains the cumulative size, in bytes, of all content in the mailbox.</t>
-  </si>
-  <si>
-    <t>[In PidTagUserEntryId Property] The PidTagUserEntryId property ([MS-OXPROPS] section 2.1047) contains the Address book EntryID of the user logged on to the mailbox.</t>
-  </si>
-  <si>
-    <t>[In PidTagLocaleId Property] The PidTagLocaleId property ([MS-OXPROPS] section 2.768) establishes the language locale for translating system-generated messages, such as delivery reports. For more details, see [MS-LCID].</t>
-  </si>
-  <si>
     <t>[In PidTagSerializedReplidGuidMap Property] Type of PidTagSerializedReplidGuidMap: PtypBinary ([MS-OXCDATA] section 2.11.1)</t>
   </si>
   <si>
     <t>MS-OXCSTOR_R4003001</t>
   </si>
   <si>
-    <t xml:space="preserve">[In PidTagSerializedReplidGuidMap Property] The PidTagSerializedReplidGuidMap property ([MS-OXPROPS] section 2.1013) contains a serialized list of REPLID and REPLGUID pairs which represents all or part of the REPLID /REPLGUID mapping of the associated Logon object. </t>
-  </si>
-  <si>
     <t>[In PidTagSerializedReplidGuidMap Property] For additional information on REPLID and REPLGUID mapping, please see section 3.2.5.8 and section 3.2.5.9.</t>
   </si>
   <si>
@@ -7224,39 +7172,15 @@
     <t>MS-OXCSTOR_R4003007</t>
   </si>
   <si>
-    <t>[In PidTagSortLocaleId Property] The PidTagSortLocaleId property ([MS-OXPROPS] section 2.1015) establishes the language locale for sorting the contents of tables. For more details, see [MS-LCID].</t>
-  </si>
-  <si>
     <t>2.2.2.1.1.15</t>
   </si>
   <si>
-    <t>[In PidTagCodePageId Property] The PidTagCodePageId property ([MS-OXPROPS] section 2.630) establishes the client code page for Unicode to double-byte character set (DBCS) string conversion. For details, see [MS-UCODEREF].</t>
-  </si>
-  <si>
     <t>[In Read/Write Properties] The PidTagComment property is read/write. &lt;14&gt;</t>
   </si>
   <si>
     <t>[In Read/Write Properties] The PidTagDeleteAfterSubmit property is writable.&lt;15&gt;</t>
   </si>
   <si>
-    <t>[In PidTagComment Property] The PidTagComment property ([MS-OXPROPS] section 2.631) contains a mailbox comment.</t>
-  </si>
-  <si>
-    <t>[In PidTagDeleteAfterSubmit Property] The PidTagDeleteAfterSubmit property ([MS-OXPROPS] section 2.662) indicates whether a transport deletes all submitted mail after transmission.</t>
-  </si>
-  <si>
-    <t>[In PidTagOutOfOfficeState Property] The PidTagOutOfOfficeState property ([MS-OXPROPS] section 2.849) indicates whether the user is Out of Office (OOF).</t>
-  </si>
-  <si>
-    <t>[In PidTagSentMailSvrEID Property] The PidTagSentMailSvrEID property ([MS-OXPROPS] section 2.1005) contains the structure identifying the Sent Items folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagUserEntryId Property] The PidTagUserEntryId property ([MS-OXPROPS] section 2.1047) contains the Address book EntryID of the user logged on to the public folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagAddressBookMessageId Property] The PidTagAddressBookMessageId property ([MS-OXPROPS] section 2.545) contains the short-term MID of the first message in the local site's offline address book public folder, if it exists and has a local replica.</t>
-  </si>
-  <si>
     <t>[In Initialization] These steps [to ensure that the server does not re-issue a REPLGUID that was issued prior to the restoration] are implementation-specific. &lt;18&gt;</t>
   </si>
   <si>
@@ -7272,19 +7196,7 @@
     <t>[In Private Mailbox Logon] If the client has made more than five attempts within a 10-second period to log on to a mailbox that is not hosted on the server, the server MUST fail the operation with ecServerPaused, as specified in section 3.2.5.1.3, in the ReturnValue field.</t>
   </si>
   <si>
-    <t>[In Receiving a RopSetReceiveFolder ROP Request] "Folder ID" column (PidTagFolderId property ([MS-OXPROPS] section 2.694)) - Contains the Folder ID, as specified in [MS-OXCDATA] section 2.2.1.1, of the Receive folder, which is the folder to which messages of the specified message class will be delivered.</t>
-  </si>
-  <si>
-    <t>[In Receiving a RopSetReceiveFolder ROP Request] "Message Class" column (PidTagMessageClass property ([MS-OXPROPS] section 2.781)) - Contains a string that specifies the message class that is configured for the Receive folder.</t>
-  </si>
-  <si>
-    <t>[In Receiving a RopSetReceiveFolder ROP Request] "Last-modification Time" column (PidTagLastModificationTime property ([MS-OXPROPS] section 2.758)) - Contains the current system-time, in UTC, when the entry was created or last modified.</t>
-  </si>
-  <si>
     <t xml:space="preserve">[In Receiving a RopIdFromLongTermId ROP Request] The error code ecInvalidParam: The LongTermId field of the request contained zeros for either the replica GUID component. </t>
-  </si>
-  <si>
-    <t>[In Behavior Common to Both Private Mailbox and Public Folder Logon] If the user marks a message as read, the current value of that message's PidTagChangeNumber property ([MS-OXPROPS] section 2.626) is added to the change number set (CNSET).</t>
   </si>
   <si>
     <t>[In Behavior Common to Both Private Mailbox and Public Folder Logon] If the value of the DataOffset field is less than zero, the server SHOULD&lt;45&gt; fail the operation with 0x80004005 (ecError) in the ReturnValue field.</t>
@@ -7460,79 +7372,166 @@
     <t>[In Read/Write Properties] The read/write properties that are available on a private mailbox logon are specified in section 2.2.2.1.2.1 through section 2.2.2.1.2.5.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation does not support the Ghosted flag.  (&lt;1&gt; Section 2.2.1.1.1: Exchange 2013, Exchange 2016 and Exchange 2019 Preview follows this behavior.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does implement SUPPORT_PROGRESS flag. ( &lt;6&gt; Section 2.2.1.1.1: Microsoft Exchange Server 2010 Service Pack 1 (SP1), Exchange 2013, Exchange 2016 and Exchange 2019 Preview implement this flag [SUPPORT_PROGRESS].)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] &lt;6&gt; Section 2.2.1.1.1: Microsoft Outlook 2010 Service Pack 1 (SP1), Outlook 2013, and Outlook 2016 and outlook 2019 Preview implement this flag [SUPPORT_PROGRESS].</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] The implementation returns the empty Folder ID structures for the following folders: Free/Busy Data, Offline Address Book Data, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, and NNTP Article Index. (&lt;9&gt; Section 2.2.1.1.4: Exchange 2013 Exchange 2016 and Exchange 2019 Preview returns the empty Folder ID structures for the following folders: Free/Busy Data, Offline Address Book Data, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, and NNTP Article Index.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] The implementation does not implement the RopGetStoreState remote operation (ROP). (&lt;11&gt; Section 2.2.1.5: Exchange 2010, Exchange 2013,  Exchange 2016 and Exchange 2019 Preview does not implement the RopGetStoreState remote operation (ROP) ([MS-OXCROPS] section 2.2.3.5))</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does support each public folder has exactly one replica, the folder's content mailbox. (Exchange 2013, Exchange 16 and Exchange 2019 Preview follow this behavior.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagComment property by using the RopSetProperties ROP ([MS-OXCROPS] section 2.2.8.6).(Microsoft Exchange Server 2013 Service Pack 1 (SP1), Exchange 2016 and Exchange 2019 Preview follow this behavior).</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] The implementation returns 0x80070005 (ecAccessDenied) when the client attempts to set PidTagDeleteAfterSubmit property by using the RopSetProperties ROP. (&lt;15&gt; Section 2.2.2.1.2.2: In Exchange 2013, Exchange 2016 and Exchange 2019 Preview the server returns 0x80070005 (ecAccessDenied) when the client attempts to set this property [PidTagDeleteAfterSubmit] by using the RopSetProperties ROP ([MS-OXCROPS] section 2.2.8.6).)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagDisplayName property by using the RopSetProperties ROP.(Microsoft Exchange Server 2013 Service Pack 1 (SP1), Exchange 2016 and Exchange 2019 Preview follow this behavior)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] The behavior of the implementation is undefined if the client sets an undefined flag in either the LogonFlags field or the OpenFlags field. (&lt;23&gt; Section 3.2.5.1.1: The behavior of Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013,  Exchange 2016 and Exchange 2019 Preview is undefined if the client sets an undefined flag in either the LogonFlags field or the OpenFlags field.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] The implementation does implement the SUPPORT_PROGRESS flag. (&lt;24&gt; Section 3.2.5.1.1: Exchange 2010 SP1, Exchange 2013, Exchange 2016 and Exchange 2019 Preview implement the SUPPORT_PROGRESS flag.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] The implementation does support the GET/read operation for the PidTagSortLocaleId property.(&lt;25&gt; Section 3.2.5.1.1: Exchange 2010, Exchange 2013,  Exchange 2016 and Exchange 2019 Preview support the GET/read operation for the PidTagSortLocaleId property.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] If the logon is the first on the RPC session, then the implementation does fail with an RPC fault. (&lt;27&gt; Section 3.2.5.1.1: In Exchange 2013, Exchange 2016 and Exchange 2019 Preview, if the logon is the first on the RPC session, then the server fails with an RPC fault; if the logon is additional on the RPC session and it is to the same mailbox that is associated with the first logon, then the server returns ecInvalidParameter.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior]  Implementation does not fail the operation [RopLogon] with ecAccessDenied [if the user does not match the owner of the mailbox]. (&lt;31&gt; Section 3.2.5.1.1: Exchange 2016, Exchange 2013 and Exchange 2019 Preview return ecNone.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does support the USE_AUTODISCOVER_FOR_PUBLIC_FOLDER_CONFIGURATION flag. (&lt;34&gt; Section 3.2.5.1.2: Exchange 2013, Exchange 2016 and Exchange 2019 Preview always set the USE_AUTODISCOVER_FOR_PUBLIC_FOLDER_CONFIGURATION flag.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] &lt;35&gt; Section 3.2.5.1.2: The behavior of Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview is undefined if the client sets an undefined flag in either the LogonFlags field or the OpenFlags field.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior]&lt;39&gt; Section 3.2.5.6: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview remove servers that have a connection cost greater than 500.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior]&lt;41&gt; Section 3.2.5.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview query Active Directory for cost information.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior]&lt;42&gt; Section 3.2.5.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview remove servers that have a connection cost greater than 500.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does not fail the operation [RopLongTermIdFromId] with 0x8004010F, but ecNone. &lt;43&gt; Section 3.2.5.8: If the ObjectId field is set to zero, Exchange 2013, Exchange 2016 and Exchange 2019 Preview returns ecNone.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation's default value of MaxDataSize is 4096. (If MaxDataSize equals 0, then the server MUST adjust the value of MaxDataSize to a suitable default value (4096). &lt;46&gt; Section 3.2.5.12.1: Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview use 4096 for the default value.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation's maximum value of MaxDataSize is 4096. (If MaxDataSize &gt; [server's suitable maximum (4096)], then Implementation does adjust the value of MaxDataSize to the suitable maximum value (4096) in Microsoft Exchanges. &lt;47&gt; Section 3.2.5.12.1: Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview use 4096 for the maximum value.)</t>
-  </si>
-  <si>
-    <t>22.0</t>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>[In RopLogon ROP Success Response Buffer for Private Mailbox] StoreState: This field SHOULD be set to 0x00000000 by the server. &lt;8&gt;</t>
+  </si>
+  <si>
+    <t>[In RopGetReceiveFolderTable ROP Success Response Buffer] 	[Rows] PidTagFolderId property ([MS-OXPROPS] section 2.696): A PtypInteger64 value that specifies the folder ID (FID) ([MS-OXCDATA] section 2.2.1.1) of the Receive folder, which is the folder to which messages of the specified message class will be delivered.</t>
+  </si>
+  <si>
+    <t>[In RopGetReceiveFolderTable ROP Success Response Buffer] [Rows] PidTagMessageClass property ([MS-OXPROPS] section 2.783): A PtypString8 value.</t>
+  </si>
+  <si>
+    <t>[In RopGetReceiveFolderTable ROP Success Response Buffer]  [Rows] PidTagLastModificationTime property: PidTagLastModificationTime property ([MS-OXPROPS] section 2.760) -- A PtypTime value that specifies the time, in Coordinated Universal Time (UTC), when the server created or last modified the row in the Receive folder table.</t>
+  </si>
+  <si>
+    <t>[In PidTagExtendedRuleSizeLimit Property] The PidTagExtendedRuleSizeLimit property ([MS-OXPROPS] section 2.690) contains the Maximum size, in bytes, the user is allowed to accumulate for a single "extended" rule.</t>
+  </si>
+  <si>
+    <t>[In PidTagMaximumSubmitMessageSize Property] The PidTagMaximumSubmitMessageSize property ([MS-OXPROPS] section 2.777) contains the maximum size, in kilobytes, of a message a user is allowed to submit for transmission to another user.</t>
+  </si>
+  <si>
+    <t>[In PidTagProhibitReceiveQuota Property] The PidTagProhibitReceiveQuota property ([MS-OXPROPS] section 2.870) contains the maximum size, in kilobytes, a user is allowed to accumulate in their mailbox, before no further mail will be delivered.</t>
+  </si>
+  <si>
+    <t>[In PidTagProhibitSendQuota Property] The PidTagProhibitSendQuota property ([MS-OXPROPS] section 2.871) contains the maximum size, in kilobytes, a user is allowed to accumulate in their mailbox, before the user can no longer submit any more mail.</t>
+  </si>
+  <si>
+    <t>[In PidTagStoreState Property] The PidTagStoreState property ([MS-OXPROPS] section 2.1025) indicates whether the mailbox has any active search folders.</t>
+  </si>
+  <si>
+    <t>[In PidTagContentCount Property] The PidTagContentCount property ([MS-OXPROPS] section 2.642) contains the cumulative count of non-folder associated information (FAI) messages in the mailbox.</t>
+  </si>
+  <si>
+    <t>[In PidTagMailboxOwnerEntryId Property] The PidTagMailboxOwnerEntryId property ([MS-OXPROPS] section 2.773) contains the EntryID in the Global Address List (GAL) of the owner of the mailbox.</t>
+  </si>
+  <si>
+    <t>[In PidTagMailboxOwnerName Property] The PidTagMailboxOwnerName property ([MS-OXPROPS] section 2.774) contains the display name of the owner of the mailbox.</t>
+  </si>
+  <si>
+    <t>[In PidTagMessageSize Property] The PidTagMessageSize property ([MS-OXPROPS] section 2.792) contains the cumulative size, in bytes, of all content in the mailbox.</t>
+  </si>
+  <si>
+    <t>[In PidTagMessageSizeExtended Property] The PidTagMessageSizeExtended property ([MS-OXPROPS] section 2.793) contains the cumulative size, in bytes, of all content in the mailbox.</t>
+  </si>
+  <si>
+    <t>[In PidTagUserEntryId Property] The PidTagUserEntryId property ([MS-OXPROPS] section 2.1049) contains the Address book EntryID of the user logged on to the mailbox.</t>
+  </si>
+  <si>
+    <t>[In PidTagLocaleId Property] The PidTagLocaleId property ([MS-OXPROPS] section 2.770) establishes the language locale for translating system-generated messages, such as delivery reports. For more details, see [MS-LCID].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In PidTagSerializedReplidGuidMap Property] The PidTagSerializedReplidGuidMap property ([MS-OXPROPS] section 2.1015) contains a serialized list of REPLID and REPLGUID pairs which represents all or part of the REPLID /REPLGUID mapping of the associated Logon object. </t>
+  </si>
+  <si>
+    <t>[In PidTagSortLocaleId Property] The PidTagSortLocaleId property ([MS-OXPROPS] section 2.1017) establishes the language locale for sorting the contents of tables. For more details, see [MS-LCID].</t>
+  </si>
+  <si>
+    <t>[In PidTagCodePageId Property] The PidTagCodePageId property ([MS-OXPROPS] section 2.632) establishes the client code page for Unicode to double-byte character set (DBCS) string conversion. For details, see [MS-UCODEREF].</t>
+  </si>
+  <si>
+    <t>[In PidTagComment Property] The PidTagComment property ([MS-OXPROPS] section 2.633) contains a mailbox comment.</t>
+  </si>
+  <si>
+    <t>[In PidTagDeleteAfterSubmit Property] The PidTagDeleteAfterSubmit property ([MS-OXPROPS] section 2.664) indicates whether a transport deletes all submitted mail after transmission.</t>
+  </si>
+  <si>
+    <t>[In PidTagOutOfOfficeState Property] The PidTagOutOfOfficeState property ([MS-OXPROPS] section 2.851) indicates whether the user is Out of Office (OOF).</t>
+  </si>
+  <si>
+    <t>[In PidTagSentMailSvrEID Property] The PidTagSentMailSvrEID property ([MS-OXPROPS] section 2.1007) contains the structure identifying the Sent Items folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagUserEntryId Property] The PidTagUserEntryId property ([MS-OXPROPS] section 2.1049) contains the Address book EntryID of the user logged on to the public folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagAddressBookMessageId Property] The PidTagAddressBookMessageId property ([MS-OXPROPS] section 2.547) contains the short-term MID of the first message in the local site's offline address book public folder, if it exists and has a local replica.</t>
+  </si>
+  <si>
+    <t>[In Receiving a RopSetReceiveFolder ROP Request] "Folder ID" column (PidTagFolderId property ([MS-OXPROPS] section 2.696)) - Contains the Folder ID, as specified in [MS-OXCDATA] section 2.2.1.1, of the Receive folder, which is the folder to which messages of the specified message class will be delivered.</t>
+  </si>
+  <si>
+    <t>[In Receiving a RopSetReceiveFolder ROP Request] "Message Class" column (PidTagMessageClass property ([MS-OXPROPS] section 2.783)) - Contains a string that specifies the message class that is configured for the Receive folder.</t>
+  </si>
+  <si>
+    <t>[In Receiving a RopSetReceiveFolder ROP Request] "Last-modification Time" column (PidTagLastModificationTime property ([MS-OXPROPS] section 2.760)) - Contains the current system-time, in UTC, when the entry was created or last modified.</t>
+  </si>
+  <si>
+    <t>[In Behavior Common to Both Private Mailbox and Public Folder Logon] If the user marks a message as read, the current value of that message's PidTagChangeNumber property ([MS-OXPROPS] section 2.628) is added to the change number set (CNSET).</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does not support the Ghosted flag.  (&lt;1&gt; Section 2.2.1.1.1: Exchange 2013, Exchange 2016 and Exchange 2019 follows this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does support each public folder has exactly one replica, the folder's content mailbox. (Exchange 2013, Exchange 16 and Exchange 2019 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagDisplayName property by using the RopSetProperties ROP.(Microsoft Exchange Server 2013 Service Pack 1 (SP1), Exchange 2016 and Exchange 2019 follow this behavior)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The behavior of the implementation is undefined if the client sets an undefined flag in either the LogonFlags field or the OpenFlags field. (&lt;23&gt; Section 3.2.5.1.1: The behavior of Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013,  Exchange 2016 and Exchange 2019 is undefined if the client sets an undefined flag in either the LogonFlags field or the OpenFlags field.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation does support the GET/read operation for the PidTagSortLocaleId property.(&lt;25&gt; Section 3.2.5.1.1: Exchange 2010, Exchange 2013,  Exchange 2016 and Exchange 2019 support the GET/read operation for the PidTagSortLocaleId property.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does return 0x80070005 (ecAccessDenied) when the client attempts to set the PidTagComment property by using the RopSetProperties ROP ([MS-OXCROPS] section 2.2.8.6).(Microsoft Exchange Server 2013 Service Pack 1 (SP1), Exchange 2016 and Exchange 2019 follow this behavior).</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does implement SUPPORT_PROGRESS flag. ( &lt;6&gt; Section 2.2.1.1.1: Microsoft Exchange Server 2010 Service Pack 1 (SP1), Exchange 2013, Exchange 2016 and Exchange 2019 implement this flag [SUPPORT_PROGRESS].)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;6&gt; Section 2.2.1.1.1: Microsoft Outlook 2010 Service Pack 1 (SP1), Outlook 2013, and Outlook 2016 and outlook 2019 implement this flag [SUPPORT_PROGRESS].</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation returns the empty Folder ID structures for the following folders: Free/Busy Data, Offline Address Book Data, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, and NNTP Article Index. (&lt;9&gt; Section 2.2.1.1.4: Exchange 2013 Exchange 2016 and Exchange 2019 returns the empty Folder ID structures for the following folders: Free/Busy Data, Offline Address Book Data, Local Site's Free/Busy Data, Local Site's Offline Address Book Data, and NNTP Article Index.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation does not implement the RopGetStoreState remote operation (ROP). (&lt;11&gt; Section 2.2.1.5: Exchange 2010, Exchange 2013,  Exchange 2016 and Exchange 2019 does not implement the RopGetStoreState remote operation (ROP) ([MS-OXCROPS] section 2.2.3.5))</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation does implement the SUPPORT_PROGRESS flag. (&lt;24&gt; Section 3.2.5.1.1: Exchange 2010 SP1, Exchange 2013, Exchange 2016 and Exchange 2019 implement the SUPPORT_PROGRESS flag.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;35&gt; Section 3.2.5.1.2: The behavior of Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 is undefined if the client sets an undefined flag in either the LogonFlags field or the OpenFlags field.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If the logon is the first on the RPC session, then the implementation does fail with an RPC fault. (&lt;27&gt; Section 3.2.5.1.1: In Exchange 2013, Exchange 2016 and Exchange 2019 if the logon is the first on the RPC session, then the server fails with an RPC fault; if the logon is additional on the RPC session and it is to the same mailbox that is associated with the first logon, then the server returns ecInvalidParameter.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation returns 0x80070005 (ecAccessDenied) when the client attempts to set PidTagDeleteAfterSubmit property by using the RopSetProperties ROP. (&lt;15&gt; Section 2.2.2.1.2.2: In Exchange 2013, Exchange 2016 and Exchange 2019 the server returns 0x80070005 (ecAccessDenied) when the client attempts to set this property [PidTagDeleteAfterSubmit] by using the RopSetProperties ROP ([MS-OXCROPS] section 2.2.8.6).)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior]  Implementation does not fail the operation [RopLogon] with ecAccessDenied [if the user does not match the owner of the mailbox]. (&lt;31&gt; Section 3.2.5.1.1: Exchange 2016, Exchange 2013 and Exchange 2019 return ecNone.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior]&lt;39&gt; Section 3.2.5.6: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 remove servers that have a connection cost greater than 500.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation's default value of MaxDataSize is 4096. (If MaxDataSize equals 0, then the server MUST adjust the value of MaxDataSize to a suitable default value (4096). &lt;46&gt; Section 3.2.5.12.1: Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 use 4096 for the default value.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does not fail the operation [RopLongTermIdFromId] with 0x8004010F, but ecNone. &lt;43&gt; Section 3.2.5.8: If the ObjectId field is set to zero, Exchange 2013, Exchange 2016 and Exchange 2019 returns ecNone.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior]&lt;42&gt; Section 3.2.5.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 remove servers that have a connection cost greater than 500.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior]&lt;41&gt; Section 3.2.5.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 query Active Directory for cost information.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does support the USE_AUTODISCOVER_FOR_PUBLIC_FOLDER_CONFIGURATION flag. (&lt;34&gt; Section 3.2.5.1.2: Exchange 2013, Exchange 2016 and Exchange 2019 always set the USE_AUTODISCOVER_FOR_PUBLIC_FOLDER_CONFIGURATION flag.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation's maximum value of MaxDataSize is 4096. (If MaxDataSize &gt; [server's suitable maximum (4096)], then Implementation does adjust the value of MaxDataSize to the suitable maximum value (4096) in Microsoft Exchanges. &lt;47&gt; Section 3.2.5.12.1: Exchange 2003, Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 use 4096 for the maximum value.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7828,21 +7827,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7866,6 +7850,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8457,34 +8456,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1113" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I1113" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1113" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I1113"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8493,12 +8492,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8580,23 +8579,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8632,23 +8614,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8824,11 +8789,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1089" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1097" sqref="C1097"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8871,138 +8838,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>2426</v>
+        <v>2375</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>43305</v>
+        <v>43374</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9015,12 +8982,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9033,12 +9000,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9051,12 +9018,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9069,60 +9036,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -11553,7 +11520,7 @@
         <v>1111</v>
       </c>
       <c r="C115" s="20" t="s">
-        <v>2290</v>
+        <v>2376</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -11579,7 +11546,7 @@
       <c r="B116" s="30" t="s">
         <v>1111</v>
       </c>
-      <c r="C116" s="31" t="s">
+      <c r="C116" s="20" t="s">
         <v>1308</v>
       </c>
       <c r="D116" s="29"/>
@@ -11757,7 +11724,7 @@
         <v>1112</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -11959,7 +11926,7 @@
         <v>1112</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -13586,7 +13553,7 @@
         <v>1122</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>2293</v>
+        <v>2377</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -13636,7 +13603,7 @@
         <v>1122</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>2294</v>
+        <v>2378</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -13886,7 +13853,7 @@
         <v>1122</v>
       </c>
       <c r="C208" s="20" t="s">
-        <v>2295</v>
+        <v>2379</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -13961,7 +13928,7 @@
         <v>1124</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>2296</v>
+        <v>2292</v>
       </c>
       <c r="D211" s="29"/>
       <c r="E211" s="29" t="s">
@@ -14388,7 +14355,7 @@
         <v>1129</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>2297</v>
+        <v>2293</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -14765,7 +14732,7 @@
         <v>1132</v>
       </c>
       <c r="C243" s="20" t="s">
-        <v>2298</v>
+        <v>2294</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="29" t="s">
@@ -14781,7 +14748,7 @@
         <v>17</v>
       </c>
       <c r="I243" s="20" t="s">
-        <v>2362</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="244" spans="1:9" ht="30">
@@ -18441,7 +18408,7 @@
         <v>1161</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>2299</v>
+        <v>2295</v>
       </c>
       <c r="D389" s="29"/>
       <c r="E389" s="29" t="s">
@@ -18815,7 +18782,7 @@
         <v>1162</v>
       </c>
       <c r="C403" s="20" t="s">
-        <v>2300</v>
+        <v>2380</v>
       </c>
       <c r="D403" s="29"/>
       <c r="E403" s="29" t="s">
@@ -18890,7 +18857,7 @@
         <v>1163</v>
       </c>
       <c r="C406" s="20" t="s">
-        <v>2301</v>
+        <v>2381</v>
       </c>
       <c r="D406" s="29"/>
       <c r="E406" s="29" t="s">
@@ -18965,7 +18932,7 @@
         <v>1164</v>
       </c>
       <c r="C409" s="20" t="s">
-        <v>2302</v>
+        <v>2382</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -18989,7 +18956,7 @@
       <c r="B410" s="30" t="s">
         <v>1164</v>
       </c>
-      <c r="C410" s="31" t="s">
+      <c r="C410" s="20" t="s">
         <v>1590</v>
       </c>
       <c r="D410" s="29"/>
@@ -19040,7 +19007,7 @@
         <v>1165</v>
       </c>
       <c r="C412" s="20" t="s">
-        <v>2303</v>
+        <v>2383</v>
       </c>
       <c r="D412" s="29"/>
       <c r="E412" s="29" t="s">
@@ -19115,7 +19082,7 @@
         <v>1166</v>
       </c>
       <c r="C415" s="20" t="s">
-        <v>2304</v>
+        <v>2384</v>
       </c>
       <c r="D415" s="29"/>
       <c r="E415" s="29" t="s">
@@ -19140,7 +19107,7 @@
         <v>1166</v>
       </c>
       <c r="C416" s="20" t="s">
-        <v>2400</v>
+        <v>2371</v>
       </c>
       <c r="D416" s="29"/>
       <c r="E416" s="29" t="s">
@@ -19159,13 +19126,13 @@
     </row>
     <row r="417" spans="1:9">
       <c r="A417" s="22" t="s">
-        <v>2402</v>
+        <v>2373</v>
       </c>
       <c r="B417" s="30" t="s">
         <v>1166</v>
       </c>
       <c r="C417" s="38" t="s">
-        <v>2401</v>
+        <v>2372</v>
       </c>
       <c r="D417" s="37"/>
       <c r="E417" s="29" t="s">
@@ -19215,7 +19182,7 @@
         <v>1167</v>
       </c>
       <c r="C419" s="20" t="s">
-        <v>2305</v>
+        <v>2385</v>
       </c>
       <c r="D419" s="29"/>
       <c r="E419" s="29" t="s">
@@ -19265,7 +19232,7 @@
         <v>1168</v>
       </c>
       <c r="C421" s="20" t="s">
-        <v>2306</v>
+        <v>2386</v>
       </c>
       <c r="D421" s="29"/>
       <c r="E421" s="29" t="s">
@@ -19315,7 +19282,7 @@
         <v>1169</v>
       </c>
       <c r="C423" s="20" t="s">
-        <v>2307</v>
+        <v>2387</v>
       </c>
       <c r="D423" s="29"/>
       <c r="E423" s="29" t="s">
@@ -19365,7 +19332,7 @@
         <v>1170</v>
       </c>
       <c r="C425" s="20" t="s">
-        <v>2308</v>
+        <v>2388</v>
       </c>
       <c r="D425" s="29"/>
       <c r="E425" s="29" t="s">
@@ -19440,7 +19407,7 @@
         <v>1171</v>
       </c>
       <c r="C428" s="20" t="s">
-        <v>2309</v>
+        <v>2389</v>
       </c>
       <c r="D428" s="29"/>
       <c r="E428" s="29" t="s">
@@ -19490,7 +19457,7 @@
         <v>1172</v>
       </c>
       <c r="C430" s="20" t="s">
-        <v>2310</v>
+        <v>2390</v>
       </c>
       <c r="D430" s="29"/>
       <c r="E430" s="29" t="s">
@@ -19540,7 +19507,7 @@
         <v>1173</v>
       </c>
       <c r="C432" s="20" t="s">
-        <v>2311</v>
+        <v>2391</v>
       </c>
       <c r="D432" s="29"/>
       <c r="E432" s="29" t="s">
@@ -19559,13 +19526,13 @@
     </row>
     <row r="433" spans="1:9" ht="30">
       <c r="A433" s="22" t="s">
-        <v>2313</v>
+        <v>2297</v>
       </c>
       <c r="B433" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C433" s="36" t="s">
-        <v>2312</v>
+        <v>2296</v>
       </c>
       <c r="D433" s="34"/>
       <c r="E433" s="29" t="s">
@@ -19584,13 +19551,13 @@
     </row>
     <row r="434" spans="1:9" ht="45">
       <c r="A434" s="22" t="s">
-        <v>2320</v>
+        <v>2303</v>
       </c>
       <c r="B434" s="30" t="s">
         <v>1174</v>
       </c>
-      <c r="C434" s="36" t="s">
-        <v>2314</v>
+      <c r="C434" s="20" t="s">
+        <v>2392</v>
       </c>
       <c r="D434" s="34"/>
       <c r="E434" s="29" t="s">
@@ -19609,13 +19576,13 @@
     </row>
     <row r="435" spans="1:9" ht="75">
       <c r="A435" s="22" t="s">
-        <v>2321</v>
+        <v>2304</v>
       </c>
       <c r="B435" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C435" s="36" t="s">
-        <v>2316</v>
+        <v>2299</v>
       </c>
       <c r="D435" s="34"/>
       <c r="E435" s="29" t="s">
@@ -19634,13 +19601,13 @@
     </row>
     <row r="436" spans="1:9" ht="45">
       <c r="A436" s="22" t="s">
-        <v>2322</v>
+        <v>2305</v>
       </c>
       <c r="B436" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C436" s="36" t="s">
-        <v>2317</v>
+        <v>2300</v>
       </c>
       <c r="D436" s="34"/>
       <c r="E436" s="29" t="s">
@@ -19659,13 +19626,13 @@
     </row>
     <row r="437" spans="1:9" ht="45">
       <c r="A437" s="22" t="s">
-        <v>2323</v>
+        <v>2306</v>
       </c>
       <c r="B437" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C437" s="36" t="s">
-        <v>2319</v>
+        <v>2302</v>
       </c>
       <c r="D437" s="34"/>
       <c r="E437" s="34" t="s">
@@ -19684,13 +19651,13 @@
     </row>
     <row r="438" spans="1:9" ht="30">
       <c r="A438" s="22" t="s">
-        <v>2324</v>
+        <v>2307</v>
       </c>
       <c r="B438" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C438" s="36" t="s">
-        <v>2318</v>
+        <v>2301</v>
       </c>
       <c r="D438" s="34"/>
       <c r="E438" s="34" t="s">
@@ -19709,13 +19676,13 @@
     </row>
     <row r="439" spans="1:9" ht="30">
       <c r="A439" s="22" t="s">
-        <v>2325</v>
+        <v>2308</v>
       </c>
       <c r="B439" s="30" t="s">
         <v>1174</v>
       </c>
       <c r="C439" s="36" t="s">
-        <v>2315</v>
+        <v>2298</v>
       </c>
       <c r="D439" s="34"/>
       <c r="E439" s="29" t="s">
@@ -19765,7 +19732,7 @@
         <v>1175</v>
       </c>
       <c r="C441" s="20" t="s">
-        <v>2326</v>
+        <v>2393</v>
       </c>
       <c r="D441" s="29"/>
       <c r="E441" s="29" t="s">
@@ -19812,7 +19779,7 @@
         <v>456</v>
       </c>
       <c r="B443" s="24" t="s">
-        <v>2327</v>
+        <v>2309</v>
       </c>
       <c r="C443" s="31" t="s">
         <v>1604</v>
@@ -19837,10 +19804,10 @@
         <v>457</v>
       </c>
       <c r="B444" s="24" t="s">
-        <v>2327</v>
+        <v>2309</v>
       </c>
       <c r="C444" s="20" t="s">
-        <v>2328</v>
+        <v>2394</v>
       </c>
       <c r="D444" s="29"/>
       <c r="E444" s="29" t="s">
@@ -19865,7 +19832,7 @@
         <v>1176</v>
       </c>
       <c r="C445" s="20" t="s">
-        <v>2403</v>
+        <v>2374</v>
       </c>
       <c r="D445" s="29"/>
       <c r="E445" s="29" t="s">
@@ -19890,7 +19857,7 @@
         <v>1176</v>
       </c>
       <c r="C446" s="20" t="s">
-        <v>2329</v>
+        <v>2310</v>
       </c>
       <c r="D446" s="29" t="s">
         <v>2131</v>
@@ -19946,7 +19913,7 @@
         <v>1176</v>
       </c>
       <c r="C448" s="20" t="s">
-        <v>2330</v>
+        <v>2311</v>
       </c>
       <c r="D448" s="29"/>
       <c r="E448" s="29" t="s">
@@ -19973,7 +19940,7 @@
         <v>1176</v>
       </c>
       <c r="C449" s="20" t="s">
-        <v>2387</v>
+        <v>2358</v>
       </c>
       <c r="D449" s="29" t="s">
         <v>2131</v>
@@ -20133,7 +20100,7 @@
         <v>1177</v>
       </c>
       <c r="C455" s="20" t="s">
-        <v>2331</v>
+        <v>2395</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -20183,7 +20150,7 @@
         <v>1178</v>
       </c>
       <c r="C457" s="20" t="s">
-        <v>2332</v>
+        <v>2396</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29" t="s">
@@ -20282,7 +20249,7 @@
       <c r="B461" s="30" t="s">
         <v>1179</v>
       </c>
-      <c r="C461" s="31" t="s">
+      <c r="C461" s="20" t="s">
         <v>1615</v>
       </c>
       <c r="D461" s="29"/>
@@ -20333,7 +20300,7 @@
         <v>1180</v>
       </c>
       <c r="C463" s="20" t="s">
-        <v>2333</v>
+        <v>2397</v>
       </c>
       <c r="D463" s="29"/>
       <c r="E463" s="29" t="s">
@@ -20458,7 +20425,7 @@
         <v>1181</v>
       </c>
       <c r="C468" s="20" t="s">
-        <v>2334</v>
+        <v>2398</v>
       </c>
       <c r="D468" s="29"/>
       <c r="E468" s="29" t="s">
@@ -20664,7 +20631,7 @@
         <v>1183</v>
       </c>
       <c r="C476" s="20" t="s">
-        <v>2335</v>
+        <v>2399</v>
       </c>
       <c r="D476" s="29"/>
       <c r="E476" s="29" t="s">
@@ -20739,7 +20706,7 @@
         <v>1184</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>2336</v>
+        <v>2400</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -20964,7 +20931,7 @@
         <v>32</v>
       </c>
       <c r="C488" s="20" t="s">
-        <v>2365</v>
+        <v>2336</v>
       </c>
       <c r="D488" s="29"/>
       <c r="E488" s="29" t="s">
@@ -23539,7 +23506,7 @@
         <v>1191</v>
       </c>
       <c r="C591" s="20" t="s">
-        <v>2337</v>
+        <v>2312</v>
       </c>
       <c r="D591" s="29"/>
       <c r="E591" s="29" t="s">
@@ -23639,7 +23606,7 @@
         <v>1192</v>
       </c>
       <c r="C595" s="20" t="s">
-        <v>2364</v>
+        <v>2335</v>
       </c>
       <c r="D595" s="29"/>
       <c r="E595" s="29" t="s">
@@ -23655,7 +23622,7 @@
         <v>17</v>
       </c>
       <c r="I595" s="20" t="s">
-        <v>2367</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="596" spans="1:9" ht="30">
@@ -23816,7 +23783,7 @@
         <v>1194</v>
       </c>
       <c r="C602" s="20" t="s">
-        <v>2338</v>
+        <v>2313</v>
       </c>
       <c r="D602" s="29"/>
       <c r="E602" s="29" t="s">
@@ -23868,7 +23835,7 @@
         <v>1194</v>
       </c>
       <c r="C604" s="20" t="s">
-        <v>2339</v>
+        <v>2314</v>
       </c>
       <c r="D604" s="29"/>
       <c r="E604" s="29" t="s">
@@ -23884,7 +23851,7 @@
         <v>17</v>
       </c>
       <c r="I604" s="20" t="s">
-        <v>2379</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="605" spans="1:9" ht="45">
@@ -23972,7 +23939,7 @@
         <v>1194</v>
       </c>
       <c r="C608" s="20" t="s">
-        <v>2340</v>
+        <v>2315</v>
       </c>
       <c r="D608" s="29"/>
       <c r="E608" s="29" t="s">
@@ -23988,7 +23955,7 @@
         <v>17</v>
       </c>
       <c r="I608" s="20" t="s">
-        <v>2383</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="609" spans="1:9" ht="45">
@@ -23999,7 +23966,7 @@
         <v>1194</v>
       </c>
       <c r="C609" s="20" t="s">
-        <v>2341</v>
+        <v>2316</v>
       </c>
       <c r="D609" s="29"/>
       <c r="E609" s="29" t="s">
@@ -24142,7 +24109,7 @@
         <v>17</v>
       </c>
       <c r="I614" s="20" t="s">
-        <v>2375</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="615" spans="1:9" ht="75">
@@ -26967,7 +26934,7 @@
         <v>1198</v>
       </c>
       <c r="C727" s="20" t="s">
-        <v>2342</v>
+        <v>2401</v>
       </c>
       <c r="D727" s="29"/>
       <c r="E727" s="29" t="s">
@@ -27017,7 +26984,7 @@
         <v>1198</v>
       </c>
       <c r="C729" s="20" t="s">
-        <v>2343</v>
+        <v>2402</v>
       </c>
       <c r="D729" s="29"/>
       <c r="E729" s="29" t="s">
@@ -27042,7 +27009,7 @@
         <v>1198</v>
       </c>
       <c r="C730" s="20" t="s">
-        <v>2344</v>
+        <v>2403</v>
       </c>
       <c r="D730" s="29"/>
       <c r="E730" s="29" t="s">
@@ -30981,7 +30948,7 @@
         <v>1204</v>
       </c>
       <c r="C887" s="20" t="s">
-        <v>2345</v>
+        <v>2317</v>
       </c>
       <c r="D887" s="29"/>
       <c r="E887" s="29" t="s">
@@ -31781,7 +31748,7 @@
         <v>1208</v>
       </c>
       <c r="C919" s="20" t="s">
-        <v>2346</v>
+        <v>2404</v>
       </c>
       <c r="D919" s="29"/>
       <c r="E919" s="29" t="s">
@@ -32181,7 +32148,7 @@
         <v>1208</v>
       </c>
       <c r="C935" s="20" t="s">
-        <v>2347</v>
+        <v>2318</v>
       </c>
       <c r="D935" s="29"/>
       <c r="E935" s="29" t="s">
@@ -32358,7 +32325,7 @@
         <v>1208</v>
       </c>
       <c r="C942" s="20" t="s">
-        <v>2348</v>
+        <v>2319</v>
       </c>
       <c r="D942" s="29"/>
       <c r="E942" s="29" t="s">
@@ -32412,7 +32379,7 @@
         <v>1208</v>
       </c>
       <c r="C944" s="20" t="s">
-        <v>2349</v>
+        <v>2320</v>
       </c>
       <c r="D944" s="29"/>
       <c r="E944" s="29" t="s">
@@ -33439,7 +33406,7 @@
         <v>1212</v>
       </c>
       <c r="C985" s="20" t="s">
-        <v>2350</v>
+        <v>2321</v>
       </c>
       <c r="D985" s="29"/>
       <c r="E985" s="29" t="s">
@@ -33455,7 +33422,7 @@
         <v>17</v>
       </c>
       <c r="I985" s="20" t="s">
-        <v>2398</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="986" spans="1:9" ht="60">
@@ -33491,7 +33458,7 @@
         <v>1212</v>
       </c>
       <c r="C987" s="20" t="s">
-        <v>2385</v>
+        <v>2356</v>
       </c>
       <c r="D987" s="29"/>
       <c r="E987" s="29" t="s">
@@ -33666,7 +33633,7 @@
         <v>1212</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2351</v>
+        <v>2322</v>
       </c>
       <c r="D994" s="29"/>
       <c r="E994" s="29" t="s">
@@ -33691,7 +33658,7 @@
         <v>1212</v>
       </c>
       <c r="C995" s="20" t="s">
-        <v>2384</v>
+        <v>2355</v>
       </c>
       <c r="D995" s="29"/>
       <c r="E995" s="29" t="s">
@@ -34064,7 +34031,7 @@
       </c>
       <c r="I1009" s="31"/>
     </row>
-    <row r="1010" spans="1:9" ht="45">
+    <row r="1010" spans="1:9" ht="30">
       <c r="A1010" s="29" t="s">
         <v>1021</v>
       </c>
@@ -34072,7 +34039,7 @@
         <v>1215</v>
       </c>
       <c r="C1010" s="20" t="s">
-        <v>2404</v>
+        <v>2405</v>
       </c>
       <c r="D1010" s="29" t="s">
         <v>2134</v>
@@ -34290,7 +34257,7 @@
         <v>1215</v>
       </c>
       <c r="C1018" s="20" t="s">
-        <v>2352</v>
+        <v>2323</v>
       </c>
       <c r="D1018" s="29"/>
       <c r="E1018" s="29" t="s">
@@ -34315,7 +34282,7 @@
         <v>1215</v>
       </c>
       <c r="C1019" s="20" t="s">
-        <v>2353</v>
+        <v>2324</v>
       </c>
       <c r="D1019" s="29"/>
       <c r="E1019" s="29" t="s">
@@ -34340,7 +34307,7 @@
         <v>1215</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2405</v>
+        <v>2411</v>
       </c>
       <c r="D1020" s="29"/>
       <c r="E1020" s="29" t="s">
@@ -34367,7 +34334,7 @@
         <v>1215</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2406</v>
+        <v>2412</v>
       </c>
       <c r="D1021" s="29"/>
       <c r="E1021" s="29" t="s">
@@ -34392,7 +34359,7 @@
         <v>1215</v>
       </c>
       <c r="C1022" s="20" t="s">
-        <v>2354</v>
+        <v>2325</v>
       </c>
       <c r="D1022" s="29" t="s">
         <v>2137</v>
@@ -34419,7 +34386,7 @@
         <v>1215</v>
       </c>
       <c r="C1023" s="20" t="s">
-        <v>2355</v>
+        <v>2326</v>
       </c>
       <c r="D1023" s="29"/>
       <c r="E1023" s="29" t="s">
@@ -34444,7 +34411,7 @@
         <v>1215</v>
       </c>
       <c r="C1024" s="20" t="s">
-        <v>2356</v>
+        <v>2327</v>
       </c>
       <c r="D1024" s="29"/>
       <c r="E1024" s="29" t="s">
@@ -34469,7 +34436,7 @@
         <v>1215</v>
       </c>
       <c r="C1025" s="20" t="s">
-        <v>2357</v>
+        <v>2328</v>
       </c>
       <c r="D1025" s="29" t="s">
         <v>2138</v>
@@ -34527,7 +34494,7 @@
         <v>1215</v>
       </c>
       <c r="C1027" s="20" t="s">
-        <v>2358</v>
+        <v>2329</v>
       </c>
       <c r="D1027" s="29" t="s">
         <v>2139</v>
@@ -34585,7 +34552,7 @@
         <v>1215</v>
       </c>
       <c r="C1029" s="20" t="s">
-        <v>2407</v>
+        <v>2413</v>
       </c>
       <c r="D1029" s="29" t="s">
         <v>2140</v>
@@ -34643,7 +34610,7 @@
         <v>1215</v>
       </c>
       <c r="C1031" s="20" t="s">
-        <v>2359</v>
+        <v>2330</v>
       </c>
       <c r="D1031" s="29" t="s">
         <v>2141</v>
@@ -34701,7 +34668,7 @@
         <v>1215</v>
       </c>
       <c r="C1033" s="20" t="s">
-        <v>2408</v>
+        <v>2414</v>
       </c>
       <c r="D1033" s="29" t="s">
         <v>2142</v>
@@ -34730,7 +34697,7 @@
         <v>1215</v>
       </c>
       <c r="C1034" s="20" t="s">
-        <v>2360</v>
+        <v>2331</v>
       </c>
       <c r="D1034" s="29" t="s">
         <v>2142</v>
@@ -34759,7 +34726,7 @@
         <v>1215</v>
       </c>
       <c r="C1035" s="20" t="s">
-        <v>2361</v>
+        <v>2332</v>
       </c>
       <c r="D1035" s="29" t="s">
         <v>2143</v>
@@ -34815,7 +34782,7 @@
         <v>1215</v>
       </c>
       <c r="C1037" s="20" t="s">
-        <v>2409</v>
+        <v>2406</v>
       </c>
       <c r="D1037" s="29"/>
       <c r="E1037" s="29" t="s">
@@ -34869,7 +34836,7 @@
         <v>1215</v>
       </c>
       <c r="C1039" s="20" t="s">
-        <v>2399</v>
+        <v>2370</v>
       </c>
       <c r="D1039" s="29" t="s">
         <v>2230</v>
@@ -34898,7 +34865,7 @@
         <v>1215</v>
       </c>
       <c r="C1040" s="20" t="s">
-        <v>2411</v>
+        <v>2418</v>
       </c>
       <c r="D1040" s="29" t="s">
         <v>2144</v>
@@ -34956,7 +34923,7 @@
         <v>1215</v>
       </c>
       <c r="C1042" s="20" t="s">
-        <v>2412</v>
+        <v>2407</v>
       </c>
       <c r="D1042" s="29" t="s">
         <v>2232</v>
@@ -34985,7 +34952,7 @@
         <v>1215</v>
       </c>
       <c r="C1043" s="20" t="s">
-        <v>2386</v>
+        <v>2357</v>
       </c>
       <c r="D1043" s="29" t="s">
         <v>2232</v>
@@ -35014,7 +34981,7 @@
         <v>1215</v>
       </c>
       <c r="C1044" s="20" t="s">
-        <v>2366</v>
+        <v>2337</v>
       </c>
       <c r="D1044" s="29" t="s">
         <v>2233</v>
@@ -35070,7 +35037,7 @@
         <v>1215</v>
       </c>
       <c r="C1046" s="20" t="s">
-        <v>2363</v>
+        <v>2334</v>
       </c>
       <c r="D1046" s="29" t="s">
         <v>2145</v>
@@ -35124,7 +35091,7 @@
         <v>1215</v>
       </c>
       <c r="C1048" s="20" t="s">
-        <v>2368</v>
+        <v>2339</v>
       </c>
       <c r="D1048" s="29" t="s">
         <v>2237</v>
@@ -35151,7 +35118,7 @@
         <v>1215</v>
       </c>
       <c r="C1049" s="20" t="s">
-        <v>2369</v>
+        <v>2340</v>
       </c>
       <c r="D1049" s="29" t="s">
         <v>2146</v>
@@ -35178,7 +35145,7 @@
         <v>1215</v>
       </c>
       <c r="C1050" s="20" t="s">
-        <v>2370</v>
+        <v>2341</v>
       </c>
       <c r="D1050" s="29" t="s">
         <v>2146</v>
@@ -35207,7 +35174,7 @@
         <v>1215</v>
       </c>
       <c r="C1051" s="20" t="s">
-        <v>2371</v>
+        <v>2342</v>
       </c>
       <c r="D1051" s="22" t="s">
         <v>2146</v>
@@ -35236,7 +35203,7 @@
         <v>1215</v>
       </c>
       <c r="C1052" s="20" t="s">
-        <v>2372</v>
+        <v>2343</v>
       </c>
       <c r="D1052" s="29" t="s">
         <v>2147</v>
@@ -35265,7 +35232,7 @@
         <v>1215</v>
       </c>
       <c r="C1053" s="20" t="s">
-        <v>2382</v>
+        <v>2353</v>
       </c>
       <c r="D1053" s="29" t="s">
         <v>2147</v>
@@ -35288,13 +35255,13 @@
     </row>
     <row r="1054" spans="1:9" ht="45">
       <c r="A1054" s="29" t="s">
-        <v>2381</v>
+        <v>2352</v>
       </c>
       <c r="B1054" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1054" s="20" t="s">
-        <v>2380</v>
+        <v>2351</v>
       </c>
       <c r="D1054" s="29" t="s">
         <v>2147</v>
@@ -35321,7 +35288,7 @@
         <v>1215</v>
       </c>
       <c r="C1055" s="20" t="s">
-        <v>2413</v>
+        <v>2408</v>
       </c>
       <c r="D1055" s="29" t="s">
         <v>2148</v>
@@ -35348,7 +35315,7 @@
         <v>1215</v>
       </c>
       <c r="C1056" s="20" t="s">
-        <v>2414</v>
+        <v>2415</v>
       </c>
       <c r="D1056" s="29"/>
       <c r="E1056" s="29" t="s">
@@ -35427,7 +35394,7 @@
         <v>1215</v>
       </c>
       <c r="C1059" s="20" t="s">
-        <v>2415</v>
+        <v>2409</v>
       </c>
       <c r="D1059" s="29" t="s">
         <v>2149</v>
@@ -35500,7 +35467,7 @@
       </c>
       <c r="I1061" s="31"/>
     </row>
-    <row r="1062" spans="1:9" ht="90">
+    <row r="1062" spans="1:9" ht="75">
       <c r="A1062" s="22" t="s">
         <v>2242</v>
       </c>
@@ -35508,7 +35475,7 @@
         <v>1215</v>
       </c>
       <c r="C1062" s="20" t="s">
-        <v>2416</v>
+        <v>2417</v>
       </c>
       <c r="D1062" s="22" t="s">
         <v>2150</v>
@@ -35531,13 +35498,13 @@
     </row>
     <row r="1063" spans="1:9" ht="90">
       <c r="A1063" s="22" t="s">
-        <v>2374</v>
+        <v>2345</v>
       </c>
       <c r="B1063" s="35" t="s">
         <v>1215</v>
       </c>
       <c r="C1063" s="20" t="s">
-        <v>2373</v>
+        <v>2344</v>
       </c>
       <c r="D1063" s="22" t="s">
         <v>2150</v>
@@ -35792,7 +35759,7 @@
         <v>1215</v>
       </c>
       <c r="C1072" s="20" t="s">
-        <v>2417</v>
+        <v>2419</v>
       </c>
       <c r="D1072" s="29" t="s">
         <v>2253</v>
@@ -35875,7 +35842,7 @@
         <v>1215</v>
       </c>
       <c r="C1075" s="20" t="s">
-        <v>2418</v>
+        <v>2425</v>
       </c>
       <c r="D1075" s="29" t="s">
         <v>2154</v>
@@ -35956,7 +35923,7 @@
         <v>1215</v>
       </c>
       <c r="C1078" s="20" t="s">
-        <v>2419</v>
+        <v>2416</v>
       </c>
       <c r="D1078" s="29" t="s">
         <v>2155</v>
@@ -36174,7 +36141,7 @@
         <v>1215</v>
       </c>
       <c r="C1086" s="20" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
       <c r="D1086" s="29" t="s">
         <v>2159</v>
@@ -36228,7 +36195,7 @@
         <v>1215</v>
       </c>
       <c r="C1088" s="20" t="s">
-        <v>2422</v>
+        <v>2423</v>
       </c>
       <c r="D1088" s="29" t="s">
         <v>2160</v>
@@ -36247,7 +36214,7 @@
       </c>
       <c r="I1088" s="31"/>
     </row>
-    <row r="1089" spans="1:9" ht="60">
+    <row r="1089" spans="1:9" ht="45">
       <c r="A1089" s="29" t="s">
         <v>1088</v>
       </c>
@@ -36255,7 +36222,7 @@
         <v>1215</v>
       </c>
       <c r="C1089" s="20" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="D1089" s="29" t="s">
         <v>2161</v>
@@ -36313,7 +36280,7 @@
         <v>1215</v>
       </c>
       <c r="C1091" s="20" t="s">
-        <v>2377</v>
+        <v>2348</v>
       </c>
       <c r="D1091" s="29" t="s">
         <v>2268</v>
@@ -36342,7 +36309,7 @@
         <v>1215</v>
       </c>
       <c r="C1092" s="20" t="s">
-        <v>2376</v>
+        <v>2347</v>
       </c>
       <c r="D1092" s="29" t="s">
         <v>2268</v>
@@ -36371,7 +36338,7 @@
         <v>1215</v>
       </c>
       <c r="C1093" s="20" t="s">
-        <v>2378</v>
+        <v>2349</v>
       </c>
       <c r="D1093" s="29" t="s">
         <v>2162</v>
@@ -36429,7 +36396,7 @@
         <v>1215</v>
       </c>
       <c r="C1095" s="20" t="s">
-        <v>2424</v>
+        <v>2421</v>
       </c>
       <c r="D1095" s="29" t="s">
         <v>2163</v>
@@ -36487,7 +36454,7 @@
         <v>1215</v>
       </c>
       <c r="C1097" s="20" t="s">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="D1097" s="29" t="s">
         <v>2165</v>
@@ -36516,7 +36483,7 @@
         <v>1215</v>
       </c>
       <c r="C1098" s="20" t="s">
-        <v>2388</v>
+        <v>2359</v>
       </c>
       <c r="D1098" s="29" t="s">
         <v>2265</v>
@@ -36545,7 +36512,7 @@
         <v>1215</v>
       </c>
       <c r="C1099" s="20" t="s">
-        <v>2395</v>
+        <v>2366</v>
       </c>
       <c r="D1099" s="22" t="s">
         <v>2265</v>
@@ -36568,13 +36535,13 @@
     </row>
     <row r="1100" spans="1:9" ht="60">
       <c r="A1100" s="22" t="s">
-        <v>2389</v>
+        <v>2360</v>
       </c>
       <c r="B1100" s="24" t="s">
         <v>1215</v>
       </c>
       <c r="C1100" s="20" t="s">
-        <v>2394</v>
+        <v>2365</v>
       </c>
       <c r="D1100" s="29" t="s">
         <v>2265</v>
@@ -36597,13 +36564,13 @@
     </row>
     <row r="1101" spans="1:9" ht="45">
       <c r="A1101" s="22" t="s">
-        <v>2390</v>
+        <v>2361</v>
       </c>
       <c r="B1101" s="24" t="s">
         <v>1215</v>
       </c>
       <c r="C1101" s="20" t="s">
-        <v>2396</v>
+        <v>2367</v>
       </c>
       <c r="D1101" s="29" t="s">
         <v>2265</v>
@@ -36626,13 +36593,13 @@
     </row>
     <row r="1102" spans="1:9" ht="60">
       <c r="A1102" s="22" t="s">
-        <v>2391</v>
+        <v>2362</v>
       </c>
       <c r="B1102" s="24" t="s">
         <v>1215</v>
       </c>
       <c r="C1102" s="20" t="s">
-        <v>2397</v>
+        <v>2368</v>
       </c>
       <c r="D1102" s="29" t="s">
         <v>2265</v>
@@ -36655,13 +36622,13 @@
     </row>
     <row r="1103" spans="1:9" ht="45">
       <c r="A1103" s="22" t="s">
-        <v>2393</v>
+        <v>2364</v>
       </c>
       <c r="B1103" s="24" t="s">
         <v>1215</v>
       </c>
       <c r="C1103" s="20" t="s">
-        <v>2392</v>
+        <v>2363</v>
       </c>
       <c r="D1103" s="29" t="s">
         <v>2265</v>
@@ -36954,6 +36921,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36961,11 +36933,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1108:I1113 A20:I1106">
@@ -37051,20 +37018,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1113" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1113">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1113" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1113">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1113" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1113">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1113" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H1113">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -37084,18 +37051,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37148,6 +37115,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -37157,14 +37132,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>